<commit_message>
minor changes, mapping SI data to standardized data
</commit_message>
<xml_diff>
--- a/data/column_descriptors_standardized.xlsx
+++ b/data/column_descriptors_standardized.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="349">
   <si>
     <t xml:space="preserve">column_ID</t>
   </si>
@@ -331,6 +331,9 @@
     <t xml:space="preserve">kieser_dPonA1</t>
   </si>
   <si>
+    <t xml:space="preserve">2015_Kieser_GI_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mutants exhibiting altered fitness in the absence of gene ponA1, a major peptidoglycan biosynthetic enzyme. </t>
   </si>
   <si>
@@ -361,6 +364,9 @@
     <t xml:space="preserve">nambi_2015_ctpC</t>
   </si>
   <si>
+    <t xml:space="preserve">2016_Nambi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mutants exhibiting altered fitness in mouse infection model (spleen) in the absence of gene ctpC</t>
   </si>
   <si>
@@ -520,6 +526,9 @@
     <t xml:space="preserve">xu_van_16</t>
   </si>
   <si>
+    <t xml:space="preserve">2017_Xu_1A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mutants exhibiting altered fitness in presence of vancomycin</t>
   </si>
   <si>
@@ -553,6 +562,9 @@
     <t xml:space="preserve">xu_rif_4</t>
   </si>
   <si>
+    <t xml:space="preserve">2017_Xu_1B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mutants exhibiting altered fitness in presence of rifampin</t>
   </si>
   <si>
@@ -568,6 +580,9 @@
     <t xml:space="preserve">xu_inh_02</t>
   </si>
   <si>
+    <t xml:space="preserve">2017_Xu_1C</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mutants exhibiting altered fitness in presence of isoniazid</t>
   </si>
   <si>
@@ -589,6 +604,9 @@
     <t xml:space="preserve">xu_emb_2.5</t>
   </si>
   <si>
+    <t xml:space="preserve">2017_Xu_1D</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mutants exhibiting altered fitness in presence of ethambutol</t>
   </si>
   <si>
@@ -751,6 +769,9 @@
     <t xml:space="preserve">ritterhaus_hypoxia_H3</t>
   </si>
   <si>
+    <t xml:space="preserve">2018_Rittershaus_1B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mutants exhibiting altered fitness in hypoxic culture (as measured after 3 weeks of culture) (compared to input pool)</t>
   </si>
   <si>
@@ -773,6 +794,9 @@
   </si>
   <si>
     <t xml:space="preserve">ritterhaus_hypoxia_H6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018_Rittershaus_1A</t>
   </si>
   <si>
     <t xml:space="preserve">Mutants exhibiting altered fitness in hypoxic culture (as measured after 6 weeks of culture) (compared to input pool)</t>
@@ -1330,11 +1354,11 @@
   <dimension ref="A1:CA65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F34" activeCellId="0" sqref="F34"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F47" activeCellId="0" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2978,7 +3002,9 @@
         <f aca="false">CONCATENATE(D14,"_vs_",C14)</f>
         <v>kieser_dPonA1_vs_mbio_H37Rv</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="G14" s="5" t="n">
         <v>14</v>
       </c>
@@ -2986,22 +3012,22 @@
         <v>1</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J14" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O14" s="5" t="s">
         <v>57</v>
@@ -3017,10 +3043,10 @@
       </c>
       <c r="S14" s="5"/>
       <c r="T14" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="V14" s="5" t="s">
         <v>39</v>
@@ -3085,23 +3111,25 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B15" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E15" s="4" t="str">
         <f aca="false">CONCATENATE(D15,"_vs_",C15)</f>
         <v>nambi_2015_ctpC_vs_nambi_2015_wt</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="G15" s="5" t="n">
         <v>2</v>
       </c>
@@ -3109,22 +3137,22 @@
         <v>2</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J15" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>34</v>
@@ -3136,10 +3164,10 @@
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="V15" s="5" t="s">
         <v>39</v>
@@ -3204,24 +3232,24 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B16" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E16" s="4" t="str">
         <f aca="false">CONCATENATE(D16,"_vs_",C16)</f>
         <v>korte_2016_otsa_trehalose_vs_korte_2016_otsa_7h9</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G16" s="5" t="n">
         <v>1</v>
@@ -3230,41 +3258,41 @@
         <v>1</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J16" s="5" t="n">
         <v>2016</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q16" s="11" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="R16" s="11" t="s">
         <v>48</v>
       </c>
       <c r="S16" s="5"/>
       <c r="T16" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="V16" s="5" t="s">
         <v>39</v>
@@ -3329,17 +3357,17 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B17" s="12" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E17" s="4" t="str">
         <f aca="false">CONCATENATE(D17,"_vs_",C17)</f>
@@ -3357,13 +3385,13 @@
         <v>2017</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L17" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N17" s="12" t="s">
         <v>46</v>
@@ -3383,7 +3411,7 @@
         <v>39</v>
       </c>
       <c r="W17" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
@@ -3444,17 +3472,17 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B18" s="12" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E18" s="4" t="str">
         <f aca="false">CONCATENATE(D18,"_vs_",C18)</f>
@@ -3468,19 +3496,19 @@
         <v>3</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J18" s="12" t="n">
         <v>2017</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N18" s="12" t="s">
         <v>46</v>
@@ -3495,14 +3523,14 @@
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
       <c r="T18" s="12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="U18" s="12"/>
       <c r="V18" s="12" t="s">
         <v>39</v>
       </c>
       <c r="W18" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
@@ -3563,17 +3591,17 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B19" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E19" s="4" t="str">
         <f aca="false">CONCATENATE(D19,"_vs_",C19)</f>
@@ -3587,19 +3615,19 @@
         <v>3</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J19" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N19" s="5" t="s">
         <v>46</v>
@@ -3614,14 +3642,14 @@
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="U19" s="5"/>
       <c r="V19" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W19" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
@@ -3682,17 +3710,17 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B20" s="12" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E20" s="4" t="str">
         <f aca="false">CONCATENATE(D20,"_vs_",C20)</f>
@@ -3706,19 +3734,19 @@
         <v>3</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J20" s="12" t="n">
         <v>2017</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N20" s="12" t="s">
         <v>46</v>
@@ -3733,14 +3761,14 @@
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
       <c r="T20" s="12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="U20" s="12"/>
       <c r="V20" s="12" t="s">
         <v>39</v>
       </c>
       <c r="W20" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
@@ -3801,17 +3829,17 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B21" s="12" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E21" s="4" t="str">
         <f aca="false">CONCATENATE(D21,"_vs_",C21)</f>
@@ -3825,19 +3853,19 @@
         <v>2</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J21" s="12" t="n">
         <v>2017</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N21" s="12" t="s">
         <v>46</v>
@@ -3852,14 +3880,14 @@
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
       <c r="T21" s="12" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="U21" s="12"/>
       <c r="V21" s="12" t="s">
         <v>39</v>
       </c>
       <c r="W21" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
@@ -3920,17 +3948,17 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B22" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E22" s="4" t="str">
         <f aca="false">CONCATENATE(D22,"_vs_",C22)</f>
@@ -3944,19 +3972,19 @@
         <v>3</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J22" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N22" s="5" t="s">
         <v>46</v>
@@ -3971,14 +3999,14 @@
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="U22" s="5"/>
       <c r="V22" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W22" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
@@ -4039,17 +4067,17 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B23" s="12" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E23" s="4" t="str">
         <f aca="false">CONCATENATE(D23,"_vs_",C23)</f>
@@ -4063,19 +4091,19 @@
         <v>3</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J23" s="12" t="n">
         <v>2017</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L23" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N23" s="12" t="s">
         <v>46</v>
@@ -4090,14 +4118,14 @@
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
       <c r="T23" s="12" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="U23" s="12"/>
       <c r="V23" s="12" t="s">
         <v>39</v>
       </c>
       <c r="W23" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X23" s="12"/>
       <c r="Y23" s="12"/>
@@ -4158,17 +4186,17 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B24" s="12" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E24" s="4" t="str">
         <f aca="false">CONCATENATE(D24,"_vs_",C24)</f>
@@ -4182,19 +4210,19 @@
         <v>2</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J24" s="12" t="n">
         <v>2017</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L24" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N24" s="12" t="s">
         <v>46</v>
@@ -4209,14 +4237,14 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="U24" s="12"/>
       <c r="V24" s="12" t="s">
         <v>39</v>
       </c>
       <c r="W24" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X24" s="12"/>
       <c r="Y24" s="12"/>
@@ -4277,17 +4305,17 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B25" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E25" s="4" t="str">
         <f aca="false">CONCATENATE(D25,"_vs_",C25)</f>
@@ -4301,19 +4329,19 @@
         <v>3</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J25" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N25" s="5" t="s">
         <v>46</v>
@@ -4328,14 +4356,14 @@
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
       <c r="T25" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="U25" s="5"/>
       <c r="V25" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W25" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
@@ -4396,17 +4424,17 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B26" s="12" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E26" s="4" t="str">
         <f aca="false">CONCATENATE(D26,"_vs_",C26)</f>
@@ -4420,19 +4448,19 @@
         <v>3</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J26" s="12" t="n">
         <v>2017</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L26" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N26" s="12" t="s">
         <v>46</v>
@@ -4447,14 +4475,14 @@
       <c r="R26" s="12"/>
       <c r="S26" s="12"/>
       <c r="T26" s="12" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="U26" s="12"/>
       <c r="V26" s="12" t="s">
         <v>39</v>
       </c>
       <c r="W26" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
@@ -4515,23 +4543,25 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B27" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E27" s="4" t="str">
         <f aca="false">CONCATENATE(D27,"_vs_",C27)</f>
         <v>xu_van_16_vs_xu_van_0</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="10" t="s">
+        <v>168</v>
+      </c>
       <c r="G27" s="5" t="n">
         <v>3</v>
       </c>
@@ -4539,37 +4569,37 @@
         <v>3</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="J27" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="P27" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="R27" s="5" t="s">
         <v>48</v>
       </c>
       <c r="S27" s="5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="T27" s="3"/>
       <c r="U27" s="5"/>
@@ -4636,23 +4666,25 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B28" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E28" s="4" t="str">
         <f aca="false">CONCATENATE(D28,"_vs_",C28)</f>
         <v>xu_rif_4_vs_xu_rif_0</v>
       </c>
-      <c r="F28" s="4"/>
+      <c r="F28" s="10" t="s">
+        <v>180</v>
+      </c>
       <c r="G28" s="5" t="n">
         <v>3</v>
       </c>
@@ -4660,37 +4692,37 @@
         <v>3</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="J28" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="P28" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="R28" s="5" t="s">
         <v>48</v>
       </c>
       <c r="S28" s="5" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
@@ -4757,23 +4789,25 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B29" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E29" s="4" t="str">
         <f aca="false">CONCATENATE(D29,"_vs_",C29)</f>
         <v>xu_inh_02_vs_xu_inh_0</v>
       </c>
-      <c r="F29" s="4"/>
+      <c r="F29" s="10" t="s">
+        <v>186</v>
+      </c>
       <c r="G29" s="5" t="n">
         <v>4</v>
       </c>
@@ -4781,37 +4815,37 @@
         <v>3</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="J29" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="P29" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="R29" s="5" t="s">
         <v>48</v>
       </c>
       <c r="S29" s="5" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
@@ -4878,23 +4912,23 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B30" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E30" s="4" t="str">
         <f aca="false">CONCATENATE(D30,"_vs_",C30)</f>
         <v>xu_inh_025_vs_xu_inh_0</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="10"/>
       <c r="G30" s="5" t="n">
         <v>4</v>
       </c>
@@ -4902,37 +4936,37 @@
         <v>3</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="J30" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="P30" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q30" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="R30" s="5" t="s">
         <v>48</v>
       </c>
       <c r="S30" s="5" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
@@ -4999,23 +5033,25 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B31" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E31" s="4" t="str">
         <f aca="false">CONCATENATE(D31,"_vs_",C31)</f>
         <v>xu_emb_2.5_vs_xu_emb_0</v>
       </c>
-      <c r="F31" s="4"/>
+      <c r="F31" s="10" t="s">
+        <v>194</v>
+      </c>
       <c r="G31" s="5" t="n">
         <v>3</v>
       </c>
@@ -5023,37 +5059,37 @@
         <v>3</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="J31" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="P31" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q31" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="R31" s="5" t="s">
         <v>48</v>
       </c>
       <c r="S31" s="5" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
@@ -5120,23 +5156,23 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B32" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E32" s="4" t="str">
         <f aca="false">CONCATENATE(D32,"_vs_",C32)</f>
         <v>xu_emb_3_vs_xu_emb_0</v>
       </c>
-      <c r="F32" s="4"/>
+      <c r="F32" s="10"/>
       <c r="G32" s="5" t="n">
         <v>3</v>
       </c>
@@ -5144,37 +5180,37 @@
         <v>3</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="J32" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="P32" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="R32" s="5" t="s">
         <v>48</v>
       </c>
       <c r="S32" s="5" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
@@ -5241,23 +5277,25 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B33" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="E33" s="4" t="str">
         <f aca="false">CONCATENATE(D33,"_vs_",C33)</f>
         <v>xu_mero_2.5_vs_xu_mero_0</v>
       </c>
-      <c r="F33" s="4"/>
+      <c r="F33" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="G33" s="5" t="n">
         <v>2</v>
       </c>
@@ -5265,37 +5303,37 @@
         <v>2</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="J33" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="P33" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q33" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="R33" s="5" t="s">
         <v>48</v>
       </c>
       <c r="S33" s="5" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
@@ -5362,24 +5400,24 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B34" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="E34" s="4" t="str">
         <f aca="false">CONCATENATE(D34,"_vs_",C34)</f>
         <v>mishra_C3H_vs_mishra_B6</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="G34" s="5" t="n">
         <v>3</v>
@@ -5392,16 +5430,16 @@
         <v>2017</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="O34" s="5" t="s">
         <v>34</v>
@@ -5419,7 +5457,7 @@
       </c>
       <c r="W34" s="5"/>
       <c r="X34" s="5" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="Y34" s="5"/>
       <c r="Z34" s="5" t="s">
@@ -5481,24 +5519,24 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B35" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="E35" s="4" t="str">
         <f aca="false">CONCATENATE(D35,"_vs_",C35)</f>
         <v>mishra_NOS2_vs_mishra_B6</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="G35" s="5" t="n">
         <v>3</v>
@@ -5511,16 +5549,16 @@
         <v>2017</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="O35" s="5" t="s">
         <v>34</v>
@@ -5538,7 +5576,7 @@
       </c>
       <c r="W35" s="5"/>
       <c r="X35" s="5" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="Y35" s="5"/>
       <c r="Z35" s="5" t="s">
@@ -5600,17 +5638,17 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B36" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="E36" s="4" t="str">
         <f aca="false">CONCATENATE(D36,"_vs_",C36)</f>
@@ -5628,16 +5666,16 @@
         <v>2017</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="O36" s="5" t="s">
         <v>34</v>
@@ -5655,7 +5693,7 @@
       </c>
       <c r="W36" s="5"/>
       <c r="X36" s="5" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="Y36" s="5"/>
       <c r="Z36" s="5" t="s">
@@ -5717,7 +5755,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B37" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -5727,13 +5765,15 @@
         <v>42</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E37" s="4" t="str">
         <f aca="false">CONCATENATE(D37,"_vs_",C37)</f>
         <v>carey_621_vs_mbio_H37Rv</v>
       </c>
-      <c r="F37" s="4"/>
+      <c r="F37" s="4" t="s">
+        <v>217</v>
+      </c>
       <c r="G37" s="5" t="n">
         <v>14</v>
       </c>
@@ -5741,25 +5781,25 @@
         <v>2</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="J37" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="P37" s="5" t="s">
         <v>35</v>
@@ -5838,7 +5878,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B38" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -5848,13 +5888,15 @@
         <v>42</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="E38" s="4" t="str">
         <f aca="false">CONCATENATE(D38,"_vs_",C38)</f>
         <v>carey_630_vs_mbio_H37Rv</v>
       </c>
-      <c r="F38" s="4"/>
+      <c r="F38" s="4" t="s">
+        <v>225</v>
+      </c>
       <c r="G38" s="5" t="n">
         <v>14</v>
       </c>
@@ -5862,25 +5904,25 @@
         <v>2</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="J38" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="P38" s="5" t="s">
         <v>35</v>
@@ -5959,7 +6001,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B39" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -5969,13 +6011,15 @@
         <v>42</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="E39" s="4" t="str">
         <f aca="false">CONCATENATE(D39,"_vs_",C39)</f>
         <v>carey_631_vs_mbio_H37Rv</v>
       </c>
-      <c r="F39" s="4"/>
+      <c r="F39" s="4" t="s">
+        <v>228</v>
+      </c>
       <c r="G39" s="5" t="n">
         <v>14</v>
       </c>
@@ -5983,25 +6027,25 @@
         <v>2</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="J39" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="P39" s="5" t="s">
         <v>35</v>
@@ -6080,7 +6124,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B40" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -6090,13 +6134,15 @@
         <v>42</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="E40" s="4" t="str">
         <f aca="false">CONCATENATE(D40,"_vs_",C40)</f>
         <v>carey_632_vs_mbio_H37Rv</v>
       </c>
-      <c r="F40" s="4"/>
+      <c r="F40" s="4" t="s">
+        <v>231</v>
+      </c>
       <c r="G40" s="5" t="n">
         <v>14</v>
       </c>
@@ -6104,25 +6150,25 @@
         <v>2</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="J40" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="P40" s="5" t="s">
         <v>35</v>
@@ -6201,7 +6247,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B41" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -6211,13 +6257,15 @@
         <v>42</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E41" s="4" t="str">
         <f aca="false">CONCATENATE(D41,"_vs_",C41)</f>
         <v>carey_641_vs_mbio_H37Rv</v>
       </c>
-      <c r="F41" s="4"/>
+      <c r="F41" s="4" t="s">
+        <v>234</v>
+      </c>
       <c r="G41" s="5" t="n">
         <v>14</v>
       </c>
@@ -6225,25 +6273,25 @@
         <v>2</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="J41" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="P41" s="5" t="s">
         <v>35</v>
@@ -6322,7 +6370,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B42" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -6332,13 +6380,15 @@
         <v>42</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E42" s="4" t="str">
         <f aca="false">CONCATENATE(D42,"_vs_",C42)</f>
         <v>carey_662_vs_mbio_H37Rv</v>
       </c>
-      <c r="F42" s="4"/>
+      <c r="F42" s="4" t="s">
+        <v>237</v>
+      </c>
       <c r="G42" s="5" t="n">
         <v>14</v>
       </c>
@@ -6346,25 +6396,25 @@
         <v>2</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="J42" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="N42" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="O42" s="5" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="P42" s="5" t="s">
         <v>35</v>
@@ -6443,7 +6493,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B43" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -6453,13 +6503,15 @@
         <v>42</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E43" s="4" t="str">
         <f aca="false">CONCATENATE(D43,"_vs_",C43)</f>
         <v>carey_663_vs_mbio_H37Rv</v>
       </c>
-      <c r="F43" s="4"/>
+      <c r="F43" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="G43" s="5" t="n">
         <v>14</v>
       </c>
@@ -6467,25 +6519,25 @@
         <v>2</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="J43" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="O43" s="5" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="P43" s="5" t="s">
         <v>35</v>
@@ -6564,7 +6616,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B44" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -6574,13 +6626,15 @@
         <v>42</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="E44" s="4" t="str">
         <f aca="false">CONCATENATE(D44,"_vs_",C44)</f>
         <v>carey_667_vs_mbio_H37Rv</v>
       </c>
-      <c r="F44" s="4"/>
+      <c r="F44" s="4" t="s">
+        <v>243</v>
+      </c>
       <c r="G44" s="5" t="n">
         <v>14</v>
       </c>
@@ -6588,25 +6642,25 @@
         <v>2</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="J44" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="N44" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="P44" s="5" t="s">
         <v>35</v>
@@ -6685,23 +6739,25 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B45" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="E45" s="4" t="str">
         <f aca="false">CONCATENATE(D45,"_vs_",C45)</f>
         <v>ritterhaus_hypoxia_H3_vs_ritterhaus_hypoxia_input</v>
       </c>
-      <c r="F45" s="4"/>
+      <c r="F45" s="4" t="s">
+        <v>249</v>
+      </c>
       <c r="G45" s="5" t="n">
         <v>8</v>
       </c>
@@ -6709,22 +6765,22 @@
         <v>8</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="J45" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="O45" s="5" t="s">
         <v>34</v>
@@ -6733,13 +6789,13 @@
         <v>35</v>
       </c>
       <c r="Q45" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="R45" s="5" t="s">
         <v>48</v>
       </c>
       <c r="S45" s="5" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="T45" s="5"/>
       <c r="U45" s="5"/>
@@ -6747,7 +6803,7 @@
         <v>39</v>
       </c>
       <c r="W45" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X45" s="5"/>
       <c r="Y45" s="5"/>
@@ -6810,23 +6866,25 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="B46" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="E46" s="4" t="str">
         <f aca="false">CONCATENATE(D46,"_vs_",C46)</f>
         <v>ritterhaus_hypoxia_H6_vs_ritterhaus_hypoxia_input</v>
       </c>
-      <c r="F46" s="4"/>
+      <c r="F46" s="4" t="s">
+        <v>258</v>
+      </c>
       <c r="G46" s="5" t="n">
         <v>8</v>
       </c>
@@ -6834,22 +6892,22 @@
         <v>6</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="J46" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="L46" s="7" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="O46" s="5" t="s">
         <v>34</v>
@@ -6858,13 +6916,13 @@
         <v>35</v>
       </c>
       <c r="Q46" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="R46" s="5" t="s">
         <v>48</v>
       </c>
       <c r="S46" s="5" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="T46" s="5"/>
       <c r="U46" s="5"/>
@@ -6872,7 +6930,7 @@
         <v>39</v>
       </c>
       <c r="W46" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X46" s="5"/>
       <c r="Y46" s="5"/>
@@ -6935,17 +6993,17 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="B47" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="E47" s="4" t="str">
         <f aca="false">CONCATENATE(D47,"_vs_",C47)</f>
@@ -6963,16 +7021,16 @@
         <v>2019</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="L47" s="18" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="O47" s="5" t="s">
         <v>34</v>
@@ -6989,10 +7047,10 @@
         <v>39</v>
       </c>
       <c r="W47" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X47" s="5" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="Y47" s="5"/>
       <c r="Z47" s="5" t="s">
@@ -7054,17 +7112,17 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="B48" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E48" s="4" t="str">
         <f aca="false">CONCATENATE(D48,"_vs_",C48)</f>
@@ -7082,16 +7140,16 @@
         <v>2019</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="L48" s="18" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="O48" s="5" t="s">
         <v>34</v>
@@ -7108,10 +7166,10 @@
         <v>39</v>
       </c>
       <c r="W48" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X48" s="5" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="Y48" s="5"/>
       <c r="Z48" s="5" t="s">
@@ -7173,17 +7231,17 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="B49" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E49" s="4" t="str">
         <f aca="false">CONCATENATE(D49,"_vs_",C49)</f>
@@ -7201,16 +7259,16 @@
         <v>2019</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="L49" s="18" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="O49" s="5" t="s">
         <v>34</v>
@@ -7227,10 +7285,10 @@
         <v>39</v>
       </c>
       <c r="W49" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X49" s="5" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="Y49" s="5"/>
       <c r="Z49" s="5" t="s">
@@ -7292,17 +7350,17 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="B50" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="E50" s="4" t="str">
         <f aca="false">CONCATENATE(D50,"_vs_",C50)</f>
@@ -7320,28 +7378,28 @@
         <v>2019</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="L50" s="18" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q50" s="5" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="R50" s="5" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
@@ -7350,7 +7408,7 @@
         <v>39</v>
       </c>
       <c r="W50" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X50" s="5"/>
       <c r="Y50" s="5"/>
@@ -7411,17 +7469,17 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B51" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="E51" s="4" t="str">
         <f aca="false">CONCATENATE(D51,"_vs_",C51)</f>
@@ -7435,19 +7493,19 @@
         <v>3</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N51" s="5" t="s">
         <v>46</v>
@@ -7466,14 +7524,14 @@
       </c>
       <c r="S51" s="5"/>
       <c r="T51" s="5" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="U51" s="5"/>
       <c r="V51" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W51" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X51" s="5"/>
       <c r="Y51" s="5"/>
@@ -7536,17 +7594,17 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="B52" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="E52" s="4" t="str">
         <f aca="false">CONCATENATE(D52,"_vs_",C52)</f>
@@ -7560,19 +7618,19 @@
         <v>2</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N52" s="5" t="s">
         <v>46</v>
@@ -7591,14 +7649,14 @@
       </c>
       <c r="S52" s="5"/>
       <c r="T52" s="5" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="U52" s="5"/>
       <c r="V52" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W52" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X52" s="5"/>
       <c r="Y52" s="5"/>
@@ -7661,17 +7719,17 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="B53" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="E53" s="4" t="str">
         <f aca="false">CONCATENATE(D53,"_vs_",C53)</f>
@@ -7685,17 +7743,17 @@
         <v>1</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="J53" s="5"/>
       <c r="K53" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
@@ -7710,16 +7768,16 @@
       </c>
       <c r="S53" s="5"/>
       <c r="T53" s="5" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="U53" s="5" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="V53" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W53" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X53" s="5"/>
       <c r="Y53" s="5"/>
@@ -7782,17 +7840,17 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="B54" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="E54" s="4" t="str">
         <f aca="false">CONCATENATE(D54,"_vs_",C54)</f>
@@ -7806,17 +7864,17 @@
         <v>2</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
@@ -7831,16 +7889,16 @@
       </c>
       <c r="S54" s="5"/>
       <c r="T54" s="5" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="U54" s="5" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="V54" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W54" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X54" s="5"/>
       <c r="Y54" s="5"/>
@@ -7903,17 +7961,17 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="B55" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="E55" s="4" t="str">
         <f aca="false">CONCATENATE(D55,"_vs_",C55)</f>
@@ -7927,17 +7985,17 @@
         <v>1</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="J55" s="5"/>
       <c r="K55" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
@@ -7952,16 +8010,16 @@
       </c>
       <c r="S55" s="5"/>
       <c r="T55" s="5" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="U55" s="5" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="V55" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W55" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X55" s="5"/>
       <c r="Y55" s="5"/>
@@ -8024,17 +8082,17 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="B56" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="E56" s="4" t="str">
         <f aca="false">CONCATENATE(D56,"_vs_",C56)</f>
@@ -8048,17 +8106,17 @@
         <v>2</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M56" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N56" s="5"/>
       <c r="O56" s="5"/>
@@ -8073,16 +8131,16 @@
       </c>
       <c r="S56" s="5"/>
       <c r="T56" s="5" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="U56" s="5" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="V56" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W56" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X56" s="5"/>
       <c r="Y56" s="5"/>
@@ -8145,17 +8203,17 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B57" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="E57" s="4" t="str">
         <f aca="false">CONCATENATE(D57,"_vs_",C57)</f>
@@ -8169,17 +8227,17 @@
         <v>1</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="J57" s="5"/>
       <c r="K57" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L57" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M57" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
@@ -8194,16 +8252,16 @@
       </c>
       <c r="S57" s="5"/>
       <c r="T57" s="5" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="U57" s="5" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="V57" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W57" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X57" s="5"/>
       <c r="Y57" s="5"/>
@@ -8266,17 +8324,17 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B58" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="E58" s="4" t="str">
         <f aca="false">CONCATENATE(D58,"_vs_",C58)</f>
@@ -8290,17 +8348,17 @@
         <v>1</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="J58" s="5"/>
       <c r="K58" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M58" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
@@ -8315,16 +8373,16 @@
       </c>
       <c r="S58" s="5"/>
       <c r="T58" s="5" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="U58" s="5" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="V58" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W58" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X58" s="5"/>
       <c r="Y58" s="5"/>
@@ -8387,17 +8445,17 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="B59" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="E59" s="4" t="str">
         <f aca="false">CONCATENATE(D59,"_vs_",C59)</f>
@@ -8411,17 +8469,17 @@
         <v>1</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="J59" s="5"/>
       <c r="K59" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M59" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N59" s="5"/>
       <c r="O59" s="5"/>
@@ -8436,16 +8494,16 @@
       </c>
       <c r="S59" s="5"/>
       <c r="T59" s="5" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="U59" s="5" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="V59" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W59" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X59" s="5"/>
       <c r="Y59" s="5"/>
@@ -8508,17 +8566,17 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="B60" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="E60" s="4" t="str">
         <f aca="false">CONCATENATE(D60,"_vs_",C60)</f>
@@ -8532,17 +8590,17 @@
         <v>1</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="J60" s="5"/>
       <c r="K60" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M60" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N60" s="5"/>
       <c r="O60" s="5"/>
@@ -8557,16 +8615,16 @@
       </c>
       <c r="S60" s="5"/>
       <c r="T60" s="5" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="U60" s="5" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="V60" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W60" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X60" s="5"/>
       <c r="Y60" s="5"/>
@@ -8629,17 +8687,17 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="B61" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="E61" s="4" t="str">
         <f aca="false">CONCATENATE(D61,"_vs_",C61)</f>
@@ -8653,17 +8711,17 @@
         <v>4</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="J61" s="5"/>
       <c r="K61" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L61" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N61" s="5"/>
       <c r="O61" s="5"/>
@@ -8679,13 +8737,13 @@
       <c r="S61" s="5"/>
       <c r="T61" s="5"/>
       <c r="U61" s="5" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="V61" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W61" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X61" s="5"/>
       <c r="Y61" s="5"/>
@@ -8748,7 +8806,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="B62" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -8758,7 +8816,7 @@
         <v>42</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="E62" s="4" t="str">
         <f aca="false">CONCATENATE(D62,"_vs_",C62)</f>
@@ -8772,17 +8830,17 @@
         <v>1</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="J62" s="5"/>
       <c r="K62" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
@@ -8798,13 +8856,13 @@
       <c r="S62" s="5"/>
       <c r="T62" s="5"/>
       <c r="U62" s="5" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="V62" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W62" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X62" s="5"/>
       <c r="Y62" s="5"/>
@@ -8867,7 +8925,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="B63" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -8877,7 +8935,7 @@
         <v>42</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="E63" s="4" t="str">
         <f aca="false">CONCATENATE(D63,"_vs_",C63)</f>
@@ -8891,17 +8949,17 @@
         <v>1</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="J63" s="5"/>
       <c r="K63" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N63" s="5"/>
       <c r="O63" s="5"/>
@@ -8917,13 +8975,13 @@
       <c r="S63" s="5"/>
       <c r="T63" s="5"/>
       <c r="U63" s="5" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="V63" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W63" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X63" s="5"/>
       <c r="Y63" s="5"/>
@@ -8986,7 +9044,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="B64" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -8996,7 +9054,7 @@
         <v>42</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="E64" s="4" t="str">
         <f aca="false">CONCATENATE(D64,"_vs_",C64)</f>
@@ -9010,17 +9068,17 @@
         <v>1</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="J64" s="5"/>
       <c r="K64" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L64" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M64" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N64" s="5"/>
       <c r="O64" s="5"/>
@@ -9036,13 +9094,13 @@
       <c r="S64" s="5"/>
       <c r="T64" s="5"/>
       <c r="U64" s="5" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="V64" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W64" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X64" s="5"/>
       <c r="Y64" s="5"/>
@@ -9105,7 +9163,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="B65" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -9115,7 +9173,7 @@
         <v>42</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="E65" s="4" t="str">
         <f aca="false">CONCATENATE(D65,"_vs_",C65)</f>
@@ -9129,17 +9187,17 @@
         <v>1</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="J65" s="5"/>
       <c r="K65" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L65" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="M65" s="5" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
@@ -9155,13 +9213,13 @@
       <c r="S65" s="5"/>
       <c r="T65" s="5"/>
       <c r="U65" s="5" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="V65" s="5" t="s">
         <v>39</v>
       </c>
       <c r="W65" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="X65" s="5"/>
       <c r="Y65" s="5"/>

</xml_diff>

<commit_message>
fixed carey column names in metadata spreadsheet
</commit_message>
<xml_diff>
--- a/data/column_descriptors_standardized.xlsx
+++ b/data/column_descriptors_standardized.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="393">
   <si>
     <t xml:space="preserve">column_ID</t>
   </si>
@@ -803,6 +803,9 @@
   </si>
   <si>
     <t xml:space="preserve">2018_Carey_1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carey_rv</t>
   </si>
   <si>
     <t xml:space="preserve">carey_621</t>
@@ -1326,7 +1329,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1363,10 +1366,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1380,31 +1379,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1491,11 +1470,11 @@
   <dimension ref="A1:CA74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I23" activeCellId="0" sqref="I23"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="D55" activeCellId="0" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2434,14 +2413,14 @@
         <f aca="false">CONCATENATE(D9,"_vs_",C9)</f>
         <v>griffin_glycerol_vs_mbio_H37Rv</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="5" t="n">
         <v>14</v>
       </c>
       <c r="H9" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="5" t="n">
         <v>2013</v>
       </c>
@@ -2918,7 +2897,7 @@
         <f aca="false">CONCATENATE(D13,"_vs_",C13)</f>
         <v>zhang_mhcii_mouse_d45_vs_zhang_wt_mouse_d45</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>95</v>
       </c>
       <c r="G13" s="5" t="n">
@@ -3277,17 +3256,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>108</v>
       </c>
       <c r="E16" s="4" t="str">
         <f aca="false">CONCATENATE(D16,"_vs_",C16)</f>
         <v>zhang_DETA-NO_pH_7.0_vs_zhang_pH_7.0_no_NO_control</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>106</v>
       </c>
       <c r="G16" s="5" t="n">
@@ -3564,7 +3543,7 @@
       <c r="P18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q18" s="12" t="s">
+      <c r="Q18" s="11" t="s">
         <v>33</v>
       </c>
       <c r="R18" s="5" t="s">
@@ -3685,7 +3664,7 @@
       <c r="P19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q19" s="12" t="s">
+      <c r="Q19" s="11" t="s">
         <v>33</v>
       </c>
       <c r="R19" s="5" t="s">
@@ -4378,10 +4357,10 @@
       <c r="P25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q25" s="12" t="s">
+      <c r="Q25" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="R25" s="12" t="s">
+      <c r="R25" s="11" t="s">
         <v>34</v>
       </c>
       <c r="S25" s="5"/>
@@ -4452,1197 +4431,1197 @@
       <c r="BZ25" s="5"/>
       <c r="CA25" s="5"/>
     </row>
-    <row r="26" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B26" s="13" t="n">
+      <c r="B26" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="E26" s="9" t="str">
+      <c r="E26" s="4" t="str">
         <f aca="false">CONCATENATE(D26,"_vs_",C26)</f>
         <v>dejesus_H37Rv_day32_vs_dejesus_H37Rv_day0</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="13" t="n">
+      <c r="F26" s="4"/>
+      <c r="G26" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H26" s="13" t="n">
+      <c r="H26" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="13" t="n">
+      <c r="I26" s="12"/>
+      <c r="J26" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K26" s="9" t="s">
+      <c r="K26" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L26" s="15" t="s">
+      <c r="L26" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M26" s="13" t="s">
+      <c r="M26" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N26" s="13" t="s">
+      <c r="N26" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O26" s="13" t="s">
+      <c r="O26" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P26" s="13" t="s">
+      <c r="P26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13" t="s">
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W26" s="13" t="s">
+      <c r="W26" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X26" s="13"/>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="13"/>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="13"/>
-      <c r="AC26" s="13"/>
-      <c r="AD26" s="13"/>
-      <c r="AE26" s="13"/>
-      <c r="AF26" s="13"/>
-      <c r="AG26" s="13"/>
-      <c r="AH26" s="13"/>
-      <c r="AI26" s="13"/>
-      <c r="AJ26" s="13"/>
-      <c r="AK26" s="13"/>
-      <c r="AL26" s="13"/>
-      <c r="AM26" s="13"/>
-      <c r="AN26" s="13"/>
-      <c r="AO26" s="13"/>
-      <c r="AP26" s="13"/>
-      <c r="AQ26" s="13"/>
-      <c r="AR26" s="13"/>
-      <c r="AS26" s="13"/>
-      <c r="AT26" s="13"/>
-      <c r="AU26" s="13"/>
-      <c r="AV26" s="13"/>
-      <c r="AW26" s="13"/>
-      <c r="AX26" s="13"/>
-      <c r="AY26" s="13"/>
-      <c r="AZ26" s="13"/>
-      <c r="BA26" s="13"/>
-      <c r="BB26" s="13"/>
-      <c r="BC26" s="13"/>
-      <c r="BD26" s="13"/>
-      <c r="BE26" s="13"/>
-      <c r="BF26" s="13"/>
-      <c r="BG26" s="13"/>
-      <c r="BH26" s="13"/>
-      <c r="BI26" s="13"/>
-      <c r="BJ26" s="13"/>
-      <c r="BK26" s="13"/>
-      <c r="BL26" s="13"/>
-      <c r="BM26" s="13"/>
-      <c r="BN26" s="13"/>
-      <c r="BO26" s="13"/>
-      <c r="BP26" s="13"/>
-      <c r="BQ26" s="13"/>
-      <c r="BR26" s="13"/>
-      <c r="BS26" s="13"/>
-      <c r="BT26" s="13"/>
-      <c r="BU26" s="13"/>
-      <c r="BV26" s="13"/>
-      <c r="BW26" s="13"/>
-      <c r="BX26" s="13"/>
-      <c r="BY26" s="13"/>
-      <c r="BZ26" s="13"/>
-      <c r="CA26" s="13"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="5"/>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="5"/>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="5"/>
+      <c r="AL26" s="5"/>
+      <c r="AM26" s="5"/>
+      <c r="AN26" s="5"/>
+      <c r="AO26" s="5"/>
+      <c r="AP26" s="5"/>
+      <c r="AQ26" s="5"/>
+      <c r="AR26" s="5"/>
+      <c r="AS26" s="5"/>
+      <c r="AT26" s="5"/>
+      <c r="AU26" s="5"/>
+      <c r="AV26" s="5"/>
+      <c r="AW26" s="5"/>
+      <c r="AX26" s="5"/>
+      <c r="AY26" s="5"/>
+      <c r="AZ26" s="5"/>
+      <c r="BA26" s="5"/>
+      <c r="BB26" s="5"/>
+      <c r="BC26" s="5"/>
+      <c r="BD26" s="5"/>
+      <c r="BE26" s="5"/>
+      <c r="BF26" s="5"/>
+      <c r="BG26" s="5"/>
+      <c r="BH26" s="5"/>
+      <c r="BI26" s="5"/>
+      <c r="BJ26" s="5"/>
+      <c r="BK26" s="5"/>
+      <c r="BL26" s="5"/>
+      <c r="BM26" s="5"/>
+      <c r="BN26" s="5"/>
+      <c r="BO26" s="5"/>
+      <c r="BP26" s="5"/>
+      <c r="BQ26" s="5"/>
+      <c r="BR26" s="5"/>
+      <c r="BS26" s="5"/>
+      <c r="BT26" s="5"/>
+      <c r="BU26" s="5"/>
+      <c r="BV26" s="5"/>
+      <c r="BW26" s="5"/>
+      <c r="BX26" s="5"/>
+      <c r="BY26" s="5"/>
+      <c r="BZ26" s="5"/>
+      <c r="CA26" s="5"/>
     </row>
-    <row r="27" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B27" s="13" t="n">
+      <c r="B27" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E27" s="9" t="str">
+      <c r="E27" s="4" t="str">
         <f aca="false">CONCATENATE(D27,"_vs_",C27)</f>
         <v>dejesus_Rv1432_day0_vs_dejesus_H37Rv_day0</v>
       </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="13" t="n">
+      <c r="F27" s="4"/>
+      <c r="G27" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H27" s="13" t="n">
+      <c r="H27" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="J27" s="13" t="n">
+      <c r="J27" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K27" s="9" t="s">
+      <c r="K27" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L27" s="18" t="s">
+      <c r="L27" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="M27" s="13" t="s">
+      <c r="M27" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N27" s="13" t="s">
+      <c r="N27" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O27" s="13" t="s">
+      <c r="O27" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P27" s="13" t="s">
+      <c r="P27" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13" t="s">
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13" t="s">
+      <c r="U27" s="5"/>
+      <c r="V27" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W27" s="13" t="s">
+      <c r="W27" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
-      <c r="AA27" s="16"/>
-      <c r="AB27" s="13"/>
-      <c r="AC27" s="13"/>
-      <c r="AD27" s="13"/>
-      <c r="AE27" s="13"/>
-      <c r="AF27" s="13"/>
-      <c r="AG27" s="13"/>
-      <c r="AH27" s="13"/>
-      <c r="AI27" s="13"/>
-      <c r="AJ27" s="13"/>
-      <c r="AK27" s="13"/>
-      <c r="AL27" s="13"/>
-      <c r="AM27" s="13"/>
-      <c r="AN27" s="13"/>
-      <c r="AO27" s="13"/>
-      <c r="AP27" s="13"/>
-      <c r="AQ27" s="13"/>
-      <c r="AR27" s="13"/>
-      <c r="AS27" s="13"/>
-      <c r="AT27" s="13"/>
-      <c r="AU27" s="13"/>
-      <c r="AV27" s="13"/>
-      <c r="AW27" s="13"/>
-      <c r="AX27" s="13"/>
-      <c r="AY27" s="13"/>
-      <c r="AZ27" s="13"/>
-      <c r="BA27" s="13"/>
-      <c r="BB27" s="13"/>
-      <c r="BC27" s="13"/>
-      <c r="BD27" s="13"/>
-      <c r="BE27" s="13"/>
-      <c r="BF27" s="13"/>
-      <c r="BG27" s="13"/>
-      <c r="BH27" s="13"/>
-      <c r="BI27" s="13"/>
-      <c r="BJ27" s="13"/>
-      <c r="BK27" s="13"/>
-      <c r="BL27" s="13"/>
-      <c r="BM27" s="13"/>
-      <c r="BN27" s="13"/>
-      <c r="BO27" s="13"/>
-      <c r="BP27" s="13"/>
-      <c r="BQ27" s="13"/>
-      <c r="BR27" s="13"/>
-      <c r="BS27" s="13"/>
-      <c r="BT27" s="13"/>
-      <c r="BU27" s="13"/>
-      <c r="BV27" s="13"/>
-      <c r="BW27" s="13"/>
-      <c r="BX27" s="13"/>
-      <c r="BY27" s="13"/>
-      <c r="BZ27" s="13"/>
-      <c r="CA27" s="13"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="5"/>
+      <c r="AG27" s="5"/>
+      <c r="AH27" s="5"/>
+      <c r="AI27" s="5"/>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="5"/>
+      <c r="AL27" s="5"/>
+      <c r="AM27" s="5"/>
+      <c r="AN27" s="5"/>
+      <c r="AO27" s="5"/>
+      <c r="AP27" s="5"/>
+      <c r="AQ27" s="5"/>
+      <c r="AR27" s="5"/>
+      <c r="AS27" s="5"/>
+      <c r="AT27" s="5"/>
+      <c r="AU27" s="5"/>
+      <c r="AV27" s="5"/>
+      <c r="AW27" s="5"/>
+      <c r="AX27" s="5"/>
+      <c r="AY27" s="5"/>
+      <c r="AZ27" s="5"/>
+      <c r="BA27" s="5"/>
+      <c r="BB27" s="5"/>
+      <c r="BC27" s="5"/>
+      <c r="BD27" s="5"/>
+      <c r="BE27" s="5"/>
+      <c r="BF27" s="5"/>
+      <c r="BG27" s="5"/>
+      <c r="BH27" s="5"/>
+      <c r="BI27" s="5"/>
+      <c r="BJ27" s="5"/>
+      <c r="BK27" s="5"/>
+      <c r="BL27" s="5"/>
+      <c r="BM27" s="5"/>
+      <c r="BN27" s="5"/>
+      <c r="BO27" s="5"/>
+      <c r="BP27" s="5"/>
+      <c r="BQ27" s="5"/>
+      <c r="BR27" s="5"/>
+      <c r="BS27" s="5"/>
+      <c r="BT27" s="5"/>
+      <c r="BU27" s="5"/>
+      <c r="BV27" s="5"/>
+      <c r="BW27" s="5"/>
+      <c r="BX27" s="5"/>
+      <c r="BY27" s="5"/>
+      <c r="BZ27" s="5"/>
+      <c r="CA27" s="5"/>
     </row>
-    <row r="28" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B28" s="13" t="n">
+      <c r="B28" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E28" s="9" t="str">
+      <c r="E28" s="4" t="str">
         <f aca="false">CONCATENATE(D28,"_vs_",C28)</f>
         <v>dejesus_Rv1432_day32_vs_dejesus_Rv1432_day0</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="13" t="n">
+      <c r="F28" s="4"/>
+      <c r="G28" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H28" s="13" t="n">
+      <c r="H28" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I28" s="9" t="s">
+      <c r="I28" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="J28" s="13" t="n">
+      <c r="J28" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="K28" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L28" s="15" t="s">
+      <c r="L28" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M28" s="13" t="s">
+      <c r="M28" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N28" s="13" t="s">
+      <c r="N28" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O28" s="13" t="s">
+      <c r="O28" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P28" s="13" t="s">
+      <c r="P28" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13" t="s">
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13" t="s">
+      <c r="U28" s="5"/>
+      <c r="V28" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W28" s="13" t="s">
+      <c r="W28" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X28" s="13"/>
-      <c r="Y28" s="13"/>
-      <c r="Z28" s="13"/>
-      <c r="AA28" s="16"/>
-      <c r="AB28" s="13"/>
-      <c r="AC28" s="13"/>
-      <c r="AD28" s="13"/>
-      <c r="AE28" s="13"/>
-      <c r="AF28" s="13"/>
-      <c r="AG28" s="13"/>
-      <c r="AH28" s="13"/>
-      <c r="AI28" s="13"/>
-      <c r="AJ28" s="13"/>
-      <c r="AK28" s="13"/>
-      <c r="AL28" s="13"/>
-      <c r="AM28" s="13"/>
-      <c r="AN28" s="13"/>
-      <c r="AO28" s="13"/>
-      <c r="AP28" s="13"/>
-      <c r="AQ28" s="13"/>
-      <c r="AR28" s="13"/>
-      <c r="AS28" s="13"/>
-      <c r="AT28" s="13"/>
-      <c r="AU28" s="13"/>
-      <c r="AV28" s="13"/>
-      <c r="AW28" s="13"/>
-      <c r="AX28" s="13"/>
-      <c r="AY28" s="13"/>
-      <c r="AZ28" s="13"/>
-      <c r="BA28" s="13"/>
-      <c r="BB28" s="13"/>
-      <c r="BC28" s="13"/>
-      <c r="BD28" s="13"/>
-      <c r="BE28" s="13"/>
-      <c r="BF28" s="13"/>
-      <c r="BG28" s="13"/>
-      <c r="BH28" s="13"/>
-      <c r="BI28" s="13"/>
-      <c r="BJ28" s="13"/>
-      <c r="BK28" s="13"/>
-      <c r="BL28" s="13"/>
-      <c r="BM28" s="13"/>
-      <c r="BN28" s="13"/>
-      <c r="BO28" s="13"/>
-      <c r="BP28" s="13"/>
-      <c r="BQ28" s="13"/>
-      <c r="BR28" s="13"/>
-      <c r="BS28" s="13"/>
-      <c r="BT28" s="13"/>
-      <c r="BU28" s="13"/>
-      <c r="BV28" s="13"/>
-      <c r="BW28" s="13"/>
-      <c r="BX28" s="13"/>
-      <c r="BY28" s="13"/>
-      <c r="BZ28" s="13"/>
-      <c r="CA28" s="13"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="5"/>
+      <c r="AG28" s="5"/>
+      <c r="AH28" s="5"/>
+      <c r="AI28" s="5"/>
+      <c r="AJ28" s="5"/>
+      <c r="AK28" s="5"/>
+      <c r="AL28" s="5"/>
+      <c r="AM28" s="5"/>
+      <c r="AN28" s="5"/>
+      <c r="AO28" s="5"/>
+      <c r="AP28" s="5"/>
+      <c r="AQ28" s="5"/>
+      <c r="AR28" s="5"/>
+      <c r="AS28" s="5"/>
+      <c r="AT28" s="5"/>
+      <c r="AU28" s="5"/>
+      <c r="AV28" s="5"/>
+      <c r="AW28" s="5"/>
+      <c r="AX28" s="5"/>
+      <c r="AY28" s="5"/>
+      <c r="AZ28" s="5"/>
+      <c r="BA28" s="5"/>
+      <c r="BB28" s="5"/>
+      <c r="BC28" s="5"/>
+      <c r="BD28" s="5"/>
+      <c r="BE28" s="5"/>
+      <c r="BF28" s="5"/>
+      <c r="BG28" s="5"/>
+      <c r="BH28" s="5"/>
+      <c r="BI28" s="5"/>
+      <c r="BJ28" s="5"/>
+      <c r="BK28" s="5"/>
+      <c r="BL28" s="5"/>
+      <c r="BM28" s="5"/>
+      <c r="BN28" s="5"/>
+      <c r="BO28" s="5"/>
+      <c r="BP28" s="5"/>
+      <c r="BQ28" s="5"/>
+      <c r="BR28" s="5"/>
+      <c r="BS28" s="5"/>
+      <c r="BT28" s="5"/>
+      <c r="BU28" s="5"/>
+      <c r="BV28" s="5"/>
+      <c r="BW28" s="5"/>
+      <c r="BX28" s="5"/>
+      <c r="BY28" s="5"/>
+      <c r="BZ28" s="5"/>
+      <c r="CA28" s="5"/>
     </row>
-    <row r="29" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B29" s="13" t="n">
+      <c r="B29" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E29" s="11" t="str">
+      <c r="E29" s="10" t="str">
         <f aca="false">CONCATENATE(D29,"_vs_",C29)</f>
         <v>dejesus_Rv1432_day32_vs_dejesus_H37Rv_day32</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="G29" s="13" t="n">
+      <c r="G29" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H29" s="13" t="n">
+      <c r="H29" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="I29" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="J29" s="13" t="n">
+      <c r="J29" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K29" s="9" t="s">
+      <c r="K29" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L29" s="15" t="s">
+      <c r="L29" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M29" s="13" t="s">
+      <c r="M29" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N29" s="13" t="s">
+      <c r="N29" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O29" s="13" t="s">
+      <c r="O29" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P29" s="13" t="s">
+      <c r="P29" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13" t="s">
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="U29" s="13"/>
-      <c r="V29" s="13" t="s">
+      <c r="U29" s="5"/>
+      <c r="V29" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W29" s="13" t="s">
+      <c r="W29" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X29" s="13"/>
-      <c r="Y29" s="13"/>
-      <c r="Z29" s="13"/>
-      <c r="AA29" s="16"/>
-      <c r="AB29" s="13"/>
-      <c r="AC29" s="13"/>
-      <c r="AD29" s="13"/>
-      <c r="AE29" s="13"/>
-      <c r="AF29" s="13"/>
-      <c r="AG29" s="13"/>
-      <c r="AH29" s="13"/>
-      <c r="AI29" s="13"/>
-      <c r="AJ29" s="13"/>
-      <c r="AK29" s="13"/>
-      <c r="AL29" s="13"/>
-      <c r="AM29" s="13"/>
-      <c r="AN29" s="13"/>
-      <c r="AO29" s="13"/>
-      <c r="AP29" s="13"/>
-      <c r="AQ29" s="13"/>
-      <c r="AR29" s="13"/>
-      <c r="AS29" s="13"/>
-      <c r="AT29" s="13"/>
-      <c r="AU29" s="13"/>
-      <c r="AV29" s="13"/>
-      <c r="AW29" s="13"/>
-      <c r="AX29" s="13"/>
-      <c r="AY29" s="13"/>
-      <c r="AZ29" s="13"/>
-      <c r="BA29" s="13"/>
-      <c r="BB29" s="13"/>
-      <c r="BC29" s="13"/>
-      <c r="BD29" s="13"/>
-      <c r="BE29" s="13"/>
-      <c r="BF29" s="13"/>
-      <c r="BG29" s="13"/>
-      <c r="BH29" s="13"/>
-      <c r="BI29" s="13"/>
-      <c r="BJ29" s="13"/>
-      <c r="BK29" s="13"/>
-      <c r="BL29" s="13"/>
-      <c r="BM29" s="13"/>
-      <c r="BN29" s="13"/>
-      <c r="BO29" s="13"/>
-      <c r="BP29" s="13"/>
-      <c r="BQ29" s="13"/>
-      <c r="BR29" s="13"/>
-      <c r="BS29" s="13"/>
-      <c r="BT29" s="13"/>
-      <c r="BU29" s="13"/>
-      <c r="BV29" s="13"/>
-      <c r="BW29" s="13"/>
-      <c r="BX29" s="13"/>
-      <c r="BY29" s="13"/>
-      <c r="BZ29" s="13"/>
-      <c r="CA29" s="13"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
+      <c r="AH29" s="5"/>
+      <c r="AI29" s="5"/>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="5"/>
+      <c r="AL29" s="5"/>
+      <c r="AM29" s="5"/>
+      <c r="AN29" s="5"/>
+      <c r="AO29" s="5"/>
+      <c r="AP29" s="5"/>
+      <c r="AQ29" s="5"/>
+      <c r="AR29" s="5"/>
+      <c r="AS29" s="5"/>
+      <c r="AT29" s="5"/>
+      <c r="AU29" s="5"/>
+      <c r="AV29" s="5"/>
+      <c r="AW29" s="5"/>
+      <c r="AX29" s="5"/>
+      <c r="AY29" s="5"/>
+      <c r="AZ29" s="5"/>
+      <c r="BA29" s="5"/>
+      <c r="BB29" s="5"/>
+      <c r="BC29" s="5"/>
+      <c r="BD29" s="5"/>
+      <c r="BE29" s="5"/>
+      <c r="BF29" s="5"/>
+      <c r="BG29" s="5"/>
+      <c r="BH29" s="5"/>
+      <c r="BI29" s="5"/>
+      <c r="BJ29" s="5"/>
+      <c r="BK29" s="5"/>
+      <c r="BL29" s="5"/>
+      <c r="BM29" s="5"/>
+      <c r="BN29" s="5"/>
+      <c r="BO29" s="5"/>
+      <c r="BP29" s="5"/>
+      <c r="BQ29" s="5"/>
+      <c r="BR29" s="5"/>
+      <c r="BS29" s="5"/>
+      <c r="BT29" s="5"/>
+      <c r="BU29" s="5"/>
+      <c r="BV29" s="5"/>
+      <c r="BW29" s="5"/>
+      <c r="BX29" s="5"/>
+      <c r="BY29" s="5"/>
+      <c r="BZ29" s="5"/>
+      <c r="CA29" s="5"/>
     </row>
-    <row r="30" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B30" s="13" t="n">
+      <c r="B30" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E30" s="9" t="str">
+      <c r="E30" s="4" t="str">
         <f aca="false">CONCATENATE(D30,"_vs_",C30)</f>
         <v>dejesus_Rv1565c_day0_vs_dejesus_H37Rv_day0</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="13" t="n">
+      <c r="F30" s="4"/>
+      <c r="G30" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H30" s="13" t="n">
+      <c r="H30" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="J30" s="13" t="n">
+      <c r="J30" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="K30" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L30" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M30" s="13" t="s">
+      <c r="M30" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N30" s="13" t="s">
+      <c r="N30" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O30" s="13" t="s">
+      <c r="O30" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P30" s="13" t="s">
+      <c r="P30" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13" t="s">
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="U30" s="13"/>
-      <c r="V30" s="13" t="s">
+      <c r="U30" s="5"/>
+      <c r="V30" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W30" s="13" t="s">
+      <c r="W30" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X30" s="13"/>
-      <c r="Y30" s="13"/>
-      <c r="Z30" s="13"/>
-      <c r="AA30" s="16"/>
-      <c r="AB30" s="13"/>
-      <c r="AC30" s="13"/>
-      <c r="AD30" s="13"/>
-      <c r="AE30" s="13"/>
-      <c r="AF30" s="13"/>
-      <c r="AG30" s="13"/>
-      <c r="AH30" s="13"/>
-      <c r="AI30" s="13"/>
-      <c r="AJ30" s="13"/>
-      <c r="AK30" s="13"/>
-      <c r="AL30" s="13"/>
-      <c r="AM30" s="13"/>
-      <c r="AN30" s="13"/>
-      <c r="AO30" s="13"/>
-      <c r="AP30" s="13"/>
-      <c r="AQ30" s="13"/>
-      <c r="AR30" s="13"/>
-      <c r="AS30" s="13"/>
-      <c r="AT30" s="13"/>
-      <c r="AU30" s="13"/>
-      <c r="AV30" s="13"/>
-      <c r="AW30" s="13"/>
-      <c r="AX30" s="13"/>
-      <c r="AY30" s="13"/>
-      <c r="AZ30" s="13"/>
-      <c r="BA30" s="13"/>
-      <c r="BB30" s="13"/>
-      <c r="BC30" s="13"/>
-      <c r="BD30" s="13"/>
-      <c r="BE30" s="13"/>
-      <c r="BF30" s="13"/>
-      <c r="BG30" s="13"/>
-      <c r="BH30" s="13"/>
-      <c r="BI30" s="13"/>
-      <c r="BJ30" s="13"/>
-      <c r="BK30" s="13"/>
-      <c r="BL30" s="13"/>
-      <c r="BM30" s="13"/>
-      <c r="BN30" s="13"/>
-      <c r="BO30" s="13"/>
-      <c r="BP30" s="13"/>
-      <c r="BQ30" s="13"/>
-      <c r="BR30" s="13"/>
-      <c r="BS30" s="13"/>
-      <c r="BT30" s="13"/>
-      <c r="BU30" s="13"/>
-      <c r="BV30" s="13"/>
-      <c r="BW30" s="13"/>
-      <c r="BX30" s="13"/>
-      <c r="BY30" s="13"/>
-      <c r="BZ30" s="13"/>
-      <c r="CA30" s="13"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
+      <c r="AG30" s="5"/>
+      <c r="AH30" s="5"/>
+      <c r="AI30" s="5"/>
+      <c r="AJ30" s="5"/>
+      <c r="AK30" s="5"/>
+      <c r="AL30" s="5"/>
+      <c r="AM30" s="5"/>
+      <c r="AN30" s="5"/>
+      <c r="AO30" s="5"/>
+      <c r="AP30" s="5"/>
+      <c r="AQ30" s="5"/>
+      <c r="AR30" s="5"/>
+      <c r="AS30" s="5"/>
+      <c r="AT30" s="5"/>
+      <c r="AU30" s="5"/>
+      <c r="AV30" s="5"/>
+      <c r="AW30" s="5"/>
+      <c r="AX30" s="5"/>
+      <c r="AY30" s="5"/>
+      <c r="AZ30" s="5"/>
+      <c r="BA30" s="5"/>
+      <c r="BB30" s="5"/>
+      <c r="BC30" s="5"/>
+      <c r="BD30" s="5"/>
+      <c r="BE30" s="5"/>
+      <c r="BF30" s="5"/>
+      <c r="BG30" s="5"/>
+      <c r="BH30" s="5"/>
+      <c r="BI30" s="5"/>
+      <c r="BJ30" s="5"/>
+      <c r="BK30" s="5"/>
+      <c r="BL30" s="5"/>
+      <c r="BM30" s="5"/>
+      <c r="BN30" s="5"/>
+      <c r="BO30" s="5"/>
+      <c r="BP30" s="5"/>
+      <c r="BQ30" s="5"/>
+      <c r="BR30" s="5"/>
+      <c r="BS30" s="5"/>
+      <c r="BT30" s="5"/>
+      <c r="BU30" s="5"/>
+      <c r="BV30" s="5"/>
+      <c r="BW30" s="5"/>
+      <c r="BX30" s="5"/>
+      <c r="BY30" s="5"/>
+      <c r="BZ30" s="5"/>
+      <c r="CA30" s="5"/>
     </row>
-    <row r="31" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B31" s="13" t="n">
+      <c r="B31" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="E31" s="9" t="str">
+      <c r="E31" s="4" t="str">
         <f aca="false">CONCATENATE(D31,"_vs_",C31)</f>
         <v>dejesus_Rv1565c_day32_vs_dejesus_Rv1565c_day0</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="13" t="n">
+      <c r="F31" s="4"/>
+      <c r="G31" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H31" s="13" t="n">
+      <c r="H31" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="J31" s="13" t="n">
+      <c r="J31" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K31" s="9" t="s">
+      <c r="K31" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L31" s="15" t="s">
+      <c r="L31" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M31" s="13" t="s">
+      <c r="M31" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N31" s="13" t="s">
+      <c r="N31" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O31" s="13" t="s">
+      <c r="O31" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P31" s="13" t="s">
+      <c r="P31" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13" t="s">
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="U31" s="13"/>
-      <c r="V31" s="13" t="s">
+      <c r="U31" s="5"/>
+      <c r="V31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W31" s="13" t="s">
+      <c r="W31" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X31" s="13"/>
-      <c r="Y31" s="13"/>
-      <c r="Z31" s="13"/>
-      <c r="AA31" s="16"/>
-      <c r="AB31" s="13"/>
-      <c r="AC31" s="13"/>
-      <c r="AD31" s="13"/>
-      <c r="AE31" s="13"/>
-      <c r="AF31" s="13"/>
-      <c r="AG31" s="13"/>
-      <c r="AH31" s="13"/>
-      <c r="AI31" s="13"/>
-      <c r="AJ31" s="13"/>
-      <c r="AK31" s="13"/>
-      <c r="AL31" s="13"/>
-      <c r="AM31" s="13"/>
-      <c r="AN31" s="13"/>
-      <c r="AO31" s="13"/>
-      <c r="AP31" s="13"/>
-      <c r="AQ31" s="13"/>
-      <c r="AR31" s="13"/>
-      <c r="AS31" s="13"/>
-      <c r="AT31" s="13"/>
-      <c r="AU31" s="13"/>
-      <c r="AV31" s="13"/>
-      <c r="AW31" s="13"/>
-      <c r="AX31" s="13"/>
-      <c r="AY31" s="13"/>
-      <c r="AZ31" s="13"/>
-      <c r="BA31" s="13"/>
-      <c r="BB31" s="13"/>
-      <c r="BC31" s="13"/>
-      <c r="BD31" s="13"/>
-      <c r="BE31" s="13"/>
-      <c r="BF31" s="13"/>
-      <c r="BG31" s="13"/>
-      <c r="BH31" s="13"/>
-      <c r="BI31" s="13"/>
-      <c r="BJ31" s="13"/>
-      <c r="BK31" s="13"/>
-      <c r="BL31" s="13"/>
-      <c r="BM31" s="13"/>
-      <c r="BN31" s="13"/>
-      <c r="BO31" s="13"/>
-      <c r="BP31" s="13"/>
-      <c r="BQ31" s="13"/>
-      <c r="BR31" s="13"/>
-      <c r="BS31" s="13"/>
-      <c r="BT31" s="13"/>
-      <c r="BU31" s="13"/>
-      <c r="BV31" s="13"/>
-      <c r="BW31" s="13"/>
-      <c r="BX31" s="13"/>
-      <c r="BY31" s="13"/>
-      <c r="BZ31" s="13"/>
-      <c r="CA31" s="13"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="5"/>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="5"/>
+      <c r="AE31" s="5"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="5"/>
+      <c r="AH31" s="5"/>
+      <c r="AI31" s="5"/>
+      <c r="AJ31" s="5"/>
+      <c r="AK31" s="5"/>
+      <c r="AL31" s="5"/>
+      <c r="AM31" s="5"/>
+      <c r="AN31" s="5"/>
+      <c r="AO31" s="5"/>
+      <c r="AP31" s="5"/>
+      <c r="AQ31" s="5"/>
+      <c r="AR31" s="5"/>
+      <c r="AS31" s="5"/>
+      <c r="AT31" s="5"/>
+      <c r="AU31" s="5"/>
+      <c r="AV31" s="5"/>
+      <c r="AW31" s="5"/>
+      <c r="AX31" s="5"/>
+      <c r="AY31" s="5"/>
+      <c r="AZ31" s="5"/>
+      <c r="BA31" s="5"/>
+      <c r="BB31" s="5"/>
+      <c r="BC31" s="5"/>
+      <c r="BD31" s="5"/>
+      <c r="BE31" s="5"/>
+      <c r="BF31" s="5"/>
+      <c r="BG31" s="5"/>
+      <c r="BH31" s="5"/>
+      <c r="BI31" s="5"/>
+      <c r="BJ31" s="5"/>
+      <c r="BK31" s="5"/>
+      <c r="BL31" s="5"/>
+      <c r="BM31" s="5"/>
+      <c r="BN31" s="5"/>
+      <c r="BO31" s="5"/>
+      <c r="BP31" s="5"/>
+      <c r="BQ31" s="5"/>
+      <c r="BR31" s="5"/>
+      <c r="BS31" s="5"/>
+      <c r="BT31" s="5"/>
+      <c r="BU31" s="5"/>
+      <c r="BV31" s="5"/>
+      <c r="BW31" s="5"/>
+      <c r="BX31" s="5"/>
+      <c r="BY31" s="5"/>
+      <c r="BZ31" s="5"/>
+      <c r="CA31" s="5"/>
     </row>
-    <row r="32" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B32" s="13" t="n">
+      <c r="B32" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="E32" s="11" t="str">
+      <c r="E32" s="10" t="str">
         <f aca="false">CONCATENATE(D32,"_vs_",C32)</f>
         <v>dejesus_Rv1565c_day32_vs_dejesus_H37Rv_day32</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="G32" s="13" t="n">
+      <c r="G32" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H32" s="13" t="n">
+      <c r="H32" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="J32" s="13" t="n">
+      <c r="J32" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="K32" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L32" s="15" t="s">
+      <c r="L32" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M32" s="13" t="s">
+      <c r="M32" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N32" s="13" t="s">
+      <c r="N32" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O32" s="13" t="s">
+      <c r="O32" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P32" s="13" t="s">
+      <c r="P32" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="13" t="s">
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="U32" s="13"/>
-      <c r="V32" s="13" t="s">
+      <c r="U32" s="5"/>
+      <c r="V32" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W32" s="13" t="s">
+      <c r="W32" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X32" s="13"/>
-      <c r="Y32" s="13"/>
-      <c r="Z32" s="13"/>
-      <c r="AA32" s="16"/>
-      <c r="AB32" s="13"/>
-      <c r="AC32" s="13"/>
-      <c r="AD32" s="13"/>
-      <c r="AE32" s="13"/>
-      <c r="AF32" s="13"/>
-      <c r="AG32" s="13"/>
-      <c r="AH32" s="13"/>
-      <c r="AI32" s="13"/>
-      <c r="AJ32" s="13"/>
-      <c r="AK32" s="13"/>
-      <c r="AL32" s="13"/>
-      <c r="AM32" s="13"/>
-      <c r="AN32" s="13"/>
-      <c r="AO32" s="13"/>
-      <c r="AP32" s="13"/>
-      <c r="AQ32" s="13"/>
-      <c r="AR32" s="13"/>
-      <c r="AS32" s="13"/>
-      <c r="AT32" s="13"/>
-      <c r="AU32" s="13"/>
-      <c r="AV32" s="13"/>
-      <c r="AW32" s="13"/>
-      <c r="AX32" s="13"/>
-      <c r="AY32" s="13"/>
-      <c r="AZ32" s="13"/>
-      <c r="BA32" s="13"/>
-      <c r="BB32" s="13"/>
-      <c r="BC32" s="13"/>
-      <c r="BD32" s="13"/>
-      <c r="BE32" s="13"/>
-      <c r="BF32" s="13"/>
-      <c r="BG32" s="13"/>
-      <c r="BH32" s="13"/>
-      <c r="BI32" s="13"/>
-      <c r="BJ32" s="13"/>
-      <c r="BK32" s="13"/>
-      <c r="BL32" s="13"/>
-      <c r="BM32" s="13"/>
-      <c r="BN32" s="13"/>
-      <c r="BO32" s="13"/>
-      <c r="BP32" s="13"/>
-      <c r="BQ32" s="13"/>
-      <c r="BR32" s="13"/>
-      <c r="BS32" s="13"/>
-      <c r="BT32" s="13"/>
-      <c r="BU32" s="13"/>
-      <c r="BV32" s="13"/>
-      <c r="BW32" s="13"/>
-      <c r="BX32" s="13"/>
-      <c r="BY32" s="13"/>
-      <c r="BZ32" s="13"/>
-      <c r="CA32" s="13"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="5"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="5"/>
+      <c r="AG32" s="5"/>
+      <c r="AH32" s="5"/>
+      <c r="AI32" s="5"/>
+      <c r="AJ32" s="5"/>
+      <c r="AK32" s="5"/>
+      <c r="AL32" s="5"/>
+      <c r="AM32" s="5"/>
+      <c r="AN32" s="5"/>
+      <c r="AO32" s="5"/>
+      <c r="AP32" s="5"/>
+      <c r="AQ32" s="5"/>
+      <c r="AR32" s="5"/>
+      <c r="AS32" s="5"/>
+      <c r="AT32" s="5"/>
+      <c r="AU32" s="5"/>
+      <c r="AV32" s="5"/>
+      <c r="AW32" s="5"/>
+      <c r="AX32" s="5"/>
+      <c r="AY32" s="5"/>
+      <c r="AZ32" s="5"/>
+      <c r="BA32" s="5"/>
+      <c r="BB32" s="5"/>
+      <c r="BC32" s="5"/>
+      <c r="BD32" s="5"/>
+      <c r="BE32" s="5"/>
+      <c r="BF32" s="5"/>
+      <c r="BG32" s="5"/>
+      <c r="BH32" s="5"/>
+      <c r="BI32" s="5"/>
+      <c r="BJ32" s="5"/>
+      <c r="BK32" s="5"/>
+      <c r="BL32" s="5"/>
+      <c r="BM32" s="5"/>
+      <c r="BN32" s="5"/>
+      <c r="BO32" s="5"/>
+      <c r="BP32" s="5"/>
+      <c r="BQ32" s="5"/>
+      <c r="BR32" s="5"/>
+      <c r="BS32" s="5"/>
+      <c r="BT32" s="5"/>
+      <c r="BU32" s="5"/>
+      <c r="BV32" s="5"/>
+      <c r="BW32" s="5"/>
+      <c r="BX32" s="5"/>
+      <c r="BY32" s="5"/>
+      <c r="BZ32" s="5"/>
+      <c r="CA32" s="5"/>
     </row>
-    <row r="33" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="s">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B33" s="13" t="n">
+      <c r="B33" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E33" s="9" t="str">
+      <c r="E33" s="4" t="str">
         <f aca="false">CONCATENATE(D33,"_vs_",C33)</f>
         <v>dejesus_Rv2680_day0_vs_dejesus_H37Rv_day0</v>
       </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="13" t="n">
+      <c r="F33" s="4"/>
+      <c r="G33" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H33" s="13" t="n">
+      <c r="H33" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="J33" s="13" t="n">
+      <c r="J33" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K33" s="9" t="s">
+      <c r="K33" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L33" s="15" t="s">
+      <c r="L33" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M33" s="13" t="s">
+      <c r="M33" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N33" s="13" t="s">
+      <c r="N33" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O33" s="13" t="s">
+      <c r="O33" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P33" s="13" t="s">
+      <c r="P33" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="13"/>
-      <c r="S33" s="13"/>
-      <c r="T33" s="13" t="s">
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="U33" s="13"/>
-      <c r="V33" s="13" t="s">
+      <c r="U33" s="5"/>
+      <c r="V33" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W33" s="13" t="s">
+      <c r="W33" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X33" s="13"/>
-      <c r="Y33" s="13"/>
-      <c r="Z33" s="13"/>
-      <c r="AA33" s="16"/>
-      <c r="AB33" s="13"/>
-      <c r="AC33" s="13"/>
-      <c r="AD33" s="13"/>
-      <c r="AE33" s="13"/>
-      <c r="AF33" s="13"/>
-      <c r="AG33" s="13"/>
-      <c r="AH33" s="13"/>
-      <c r="AI33" s="13"/>
-      <c r="AJ33" s="13"/>
-      <c r="AK33" s="13"/>
-      <c r="AL33" s="13"/>
-      <c r="AM33" s="13"/>
-      <c r="AN33" s="13"/>
-      <c r="AO33" s="13"/>
-      <c r="AP33" s="13"/>
-      <c r="AQ33" s="13"/>
-      <c r="AR33" s="13"/>
-      <c r="AS33" s="13"/>
-      <c r="AT33" s="13"/>
-      <c r="AU33" s="13"/>
-      <c r="AV33" s="13"/>
-      <c r="AW33" s="13"/>
-      <c r="AX33" s="13"/>
-      <c r="AY33" s="13"/>
-      <c r="AZ33" s="13"/>
-      <c r="BA33" s="13"/>
-      <c r="BB33" s="13"/>
-      <c r="BC33" s="13"/>
-      <c r="BD33" s="13"/>
-      <c r="BE33" s="13"/>
-      <c r="BF33" s="13"/>
-      <c r="BG33" s="13"/>
-      <c r="BH33" s="13"/>
-      <c r="BI33" s="13"/>
-      <c r="BJ33" s="13"/>
-      <c r="BK33" s="13"/>
-      <c r="BL33" s="13"/>
-      <c r="BM33" s="13"/>
-      <c r="BN33" s="13"/>
-      <c r="BO33" s="13"/>
-      <c r="BP33" s="13"/>
-      <c r="BQ33" s="13"/>
-      <c r="BR33" s="13"/>
-      <c r="BS33" s="13"/>
-      <c r="BT33" s="13"/>
-      <c r="BU33" s="13"/>
-      <c r="BV33" s="13"/>
-      <c r="BW33" s="13"/>
-      <c r="BX33" s="13"/>
-      <c r="BY33" s="13"/>
-      <c r="BZ33" s="13"/>
-      <c r="CA33" s="13"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="5"/>
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="5"/>
+      <c r="AE33" s="5"/>
+      <c r="AF33" s="5"/>
+      <c r="AG33" s="5"/>
+      <c r="AH33" s="5"/>
+      <c r="AI33" s="5"/>
+      <c r="AJ33" s="5"/>
+      <c r="AK33" s="5"/>
+      <c r="AL33" s="5"/>
+      <c r="AM33" s="5"/>
+      <c r="AN33" s="5"/>
+      <c r="AO33" s="5"/>
+      <c r="AP33" s="5"/>
+      <c r="AQ33" s="5"/>
+      <c r="AR33" s="5"/>
+      <c r="AS33" s="5"/>
+      <c r="AT33" s="5"/>
+      <c r="AU33" s="5"/>
+      <c r="AV33" s="5"/>
+      <c r="AW33" s="5"/>
+      <c r="AX33" s="5"/>
+      <c r="AY33" s="5"/>
+      <c r="AZ33" s="5"/>
+      <c r="BA33" s="5"/>
+      <c r="BB33" s="5"/>
+      <c r="BC33" s="5"/>
+      <c r="BD33" s="5"/>
+      <c r="BE33" s="5"/>
+      <c r="BF33" s="5"/>
+      <c r="BG33" s="5"/>
+      <c r="BH33" s="5"/>
+      <c r="BI33" s="5"/>
+      <c r="BJ33" s="5"/>
+      <c r="BK33" s="5"/>
+      <c r="BL33" s="5"/>
+      <c r="BM33" s="5"/>
+      <c r="BN33" s="5"/>
+      <c r="BO33" s="5"/>
+      <c r="BP33" s="5"/>
+      <c r="BQ33" s="5"/>
+      <c r="BR33" s="5"/>
+      <c r="BS33" s="5"/>
+      <c r="BT33" s="5"/>
+      <c r="BU33" s="5"/>
+      <c r="BV33" s="5"/>
+      <c r="BW33" s="5"/>
+      <c r="BX33" s="5"/>
+      <c r="BY33" s="5"/>
+      <c r="BZ33" s="5"/>
+      <c r="CA33" s="5"/>
     </row>
-    <row r="34" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="s">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B34" s="13" t="n">
+      <c r="B34" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="E34" s="9" t="str">
+      <c r="E34" s="4" t="str">
         <f aca="false">CONCATENATE(D34,"_vs_",C34)</f>
         <v>dejesus_Rv2680_day32_vs_dejesus_Rv2680_day0</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="13" t="n">
+      <c r="F34" s="4"/>
+      <c r="G34" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H34" s="13" t="n">
+      <c r="H34" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I34" s="9" t="s">
+      <c r="I34" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="J34" s="13" t="n">
+      <c r="J34" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K34" s="9" t="s">
+      <c r="K34" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L34" s="15" t="s">
+      <c r="L34" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M34" s="13" t="s">
+      <c r="M34" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N34" s="13" t="s">
+      <c r="N34" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O34" s="13" t="s">
+      <c r="O34" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P34" s="13" t="s">
+      <c r="P34" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="13"/>
-      <c r="T34" s="13" t="s">
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="U34" s="13"/>
-      <c r="V34" s="13" t="s">
+      <c r="U34" s="5"/>
+      <c r="V34" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W34" s="13" t="s">
+      <c r="W34" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X34" s="13"/>
-      <c r="Y34" s="13"/>
-      <c r="Z34" s="13"/>
-      <c r="AA34" s="16"/>
-      <c r="AB34" s="13"/>
-      <c r="AC34" s="13"/>
-      <c r="AD34" s="13"/>
-      <c r="AE34" s="13"/>
-      <c r="AF34" s="13"/>
-      <c r="AG34" s="13"/>
-      <c r="AH34" s="13"/>
-      <c r="AI34" s="13"/>
-      <c r="AJ34" s="13"/>
-      <c r="AK34" s="13"/>
-      <c r="AL34" s="13"/>
-      <c r="AM34" s="13"/>
-      <c r="AN34" s="13"/>
-      <c r="AO34" s="13"/>
-      <c r="AP34" s="13"/>
-      <c r="AQ34" s="13"/>
-      <c r="AR34" s="13"/>
-      <c r="AS34" s="13"/>
-      <c r="AT34" s="13"/>
-      <c r="AU34" s="13"/>
-      <c r="AV34" s="13"/>
-      <c r="AW34" s="13"/>
-      <c r="AX34" s="13"/>
-      <c r="AY34" s="13"/>
-      <c r="AZ34" s="13"/>
-      <c r="BA34" s="13"/>
-      <c r="BB34" s="13"/>
-      <c r="BC34" s="13"/>
-      <c r="BD34" s="13"/>
-      <c r="BE34" s="13"/>
-      <c r="BF34" s="13"/>
-      <c r="BG34" s="13"/>
-      <c r="BH34" s="13"/>
-      <c r="BI34" s="13"/>
-      <c r="BJ34" s="13"/>
-      <c r="BK34" s="13"/>
-      <c r="BL34" s="13"/>
-      <c r="BM34" s="13"/>
-      <c r="BN34" s="13"/>
-      <c r="BO34" s="13"/>
-      <c r="BP34" s="13"/>
-      <c r="BQ34" s="13"/>
-      <c r="BR34" s="13"/>
-      <c r="BS34" s="13"/>
-      <c r="BT34" s="13"/>
-      <c r="BU34" s="13"/>
-      <c r="BV34" s="13"/>
-      <c r="BW34" s="13"/>
-      <c r="BX34" s="13"/>
-      <c r="BY34" s="13"/>
-      <c r="BZ34" s="13"/>
-      <c r="CA34" s="13"/>
+      <c r="X34" s="5"/>
+      <c r="Y34" s="5"/>
+      <c r="Z34" s="5"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="5"/>
+      <c r="AC34" s="5"/>
+      <c r="AD34" s="5"/>
+      <c r="AE34" s="5"/>
+      <c r="AF34" s="5"/>
+      <c r="AG34" s="5"/>
+      <c r="AH34" s="5"/>
+      <c r="AI34" s="5"/>
+      <c r="AJ34" s="5"/>
+      <c r="AK34" s="5"/>
+      <c r="AL34" s="5"/>
+      <c r="AM34" s="5"/>
+      <c r="AN34" s="5"/>
+      <c r="AO34" s="5"/>
+      <c r="AP34" s="5"/>
+      <c r="AQ34" s="5"/>
+      <c r="AR34" s="5"/>
+      <c r="AS34" s="5"/>
+      <c r="AT34" s="5"/>
+      <c r="AU34" s="5"/>
+      <c r="AV34" s="5"/>
+      <c r="AW34" s="5"/>
+      <c r="AX34" s="5"/>
+      <c r="AY34" s="5"/>
+      <c r="AZ34" s="5"/>
+      <c r="BA34" s="5"/>
+      <c r="BB34" s="5"/>
+      <c r="BC34" s="5"/>
+      <c r="BD34" s="5"/>
+      <c r="BE34" s="5"/>
+      <c r="BF34" s="5"/>
+      <c r="BG34" s="5"/>
+      <c r="BH34" s="5"/>
+      <c r="BI34" s="5"/>
+      <c r="BJ34" s="5"/>
+      <c r="BK34" s="5"/>
+      <c r="BL34" s="5"/>
+      <c r="BM34" s="5"/>
+      <c r="BN34" s="5"/>
+      <c r="BO34" s="5"/>
+      <c r="BP34" s="5"/>
+      <c r="BQ34" s="5"/>
+      <c r="BR34" s="5"/>
+      <c r="BS34" s="5"/>
+      <c r="BT34" s="5"/>
+      <c r="BU34" s="5"/>
+      <c r="BV34" s="5"/>
+      <c r="BW34" s="5"/>
+      <c r="BX34" s="5"/>
+      <c r="BY34" s="5"/>
+      <c r="BZ34" s="5"/>
+      <c r="CA34" s="5"/>
     </row>
-    <row r="35" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="s">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B35" s="13" t="n">
+      <c r="B35" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="E35" s="11" t="str">
+      <c r="E35" s="10" t="str">
         <f aca="false">CONCATENATE(D35,"_vs_",C35)</f>
         <v>dejesus_Rv2680_day32_vs_dejesus_H37Rv_day32</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="G35" s="13" t="n">
+      <c r="G35" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H35" s="13" t="n">
+      <c r="H35" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="J35" s="13" t="n">
+      <c r="J35" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K35" s="9" t="s">
+      <c r="K35" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L35" s="15" t="s">
+      <c r="L35" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M35" s="13" t="s">
+      <c r="M35" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N35" s="13" t="s">
+      <c r="N35" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O35" s="13" t="s">
+      <c r="O35" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P35" s="13" t="s">
+      <c r="P35" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="13" t="s">
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="U35" s="13"/>
-      <c r="V35" s="13" t="s">
+      <c r="U35" s="5"/>
+      <c r="V35" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W35" s="13" t="s">
+      <c r="W35" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X35" s="13"/>
-      <c r="Y35" s="13"/>
-      <c r="Z35" s="13"/>
-      <c r="AA35" s="16"/>
-      <c r="AB35" s="13"/>
-      <c r="AC35" s="13"/>
-      <c r="AD35" s="13"/>
-      <c r="AE35" s="13"/>
-      <c r="AF35" s="13"/>
-      <c r="AG35" s="13"/>
-      <c r="AH35" s="13"/>
-      <c r="AI35" s="13"/>
-      <c r="AJ35" s="13"/>
-      <c r="AK35" s="13"/>
-      <c r="AL35" s="13"/>
-      <c r="AM35" s="13"/>
-      <c r="AN35" s="13"/>
-      <c r="AO35" s="13"/>
-      <c r="AP35" s="13"/>
-      <c r="AQ35" s="13"/>
-      <c r="AR35" s="13"/>
-      <c r="AS35" s="13"/>
-      <c r="AT35" s="13"/>
-      <c r="AU35" s="13"/>
-      <c r="AV35" s="13"/>
-      <c r="AW35" s="13"/>
-      <c r="AX35" s="13"/>
-      <c r="AY35" s="13"/>
-      <c r="AZ35" s="13"/>
-      <c r="BA35" s="13"/>
-      <c r="BB35" s="13"/>
-      <c r="BC35" s="13"/>
-      <c r="BD35" s="13"/>
-      <c r="BE35" s="13"/>
-      <c r="BF35" s="13"/>
-      <c r="BG35" s="13"/>
-      <c r="BH35" s="13"/>
-      <c r="BI35" s="13"/>
-      <c r="BJ35" s="13"/>
-      <c r="BK35" s="13"/>
-      <c r="BL35" s="13"/>
-      <c r="BM35" s="13"/>
-      <c r="BN35" s="13"/>
-      <c r="BO35" s="13"/>
-      <c r="BP35" s="13"/>
-      <c r="BQ35" s="13"/>
-      <c r="BR35" s="13"/>
-      <c r="BS35" s="13"/>
-      <c r="BT35" s="13"/>
-      <c r="BU35" s="13"/>
-      <c r="BV35" s="13"/>
-      <c r="BW35" s="13"/>
-      <c r="BX35" s="13"/>
-      <c r="BY35" s="13"/>
-      <c r="BZ35" s="13"/>
-      <c r="CA35" s="13"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="5"/>
+      <c r="AC35" s="5"/>
+      <c r="AD35" s="5"/>
+      <c r="AE35" s="5"/>
+      <c r="AF35" s="5"/>
+      <c r="AG35" s="5"/>
+      <c r="AH35" s="5"/>
+      <c r="AI35" s="5"/>
+      <c r="AJ35" s="5"/>
+      <c r="AK35" s="5"/>
+      <c r="AL35" s="5"/>
+      <c r="AM35" s="5"/>
+      <c r="AN35" s="5"/>
+      <c r="AO35" s="5"/>
+      <c r="AP35" s="5"/>
+      <c r="AQ35" s="5"/>
+      <c r="AR35" s="5"/>
+      <c r="AS35" s="5"/>
+      <c r="AT35" s="5"/>
+      <c r="AU35" s="5"/>
+      <c r="AV35" s="5"/>
+      <c r="AW35" s="5"/>
+      <c r="AX35" s="5"/>
+      <c r="AY35" s="5"/>
+      <c r="AZ35" s="5"/>
+      <c r="BA35" s="5"/>
+      <c r="BB35" s="5"/>
+      <c r="BC35" s="5"/>
+      <c r="BD35" s="5"/>
+      <c r="BE35" s="5"/>
+      <c r="BF35" s="5"/>
+      <c r="BG35" s="5"/>
+      <c r="BH35" s="5"/>
+      <c r="BI35" s="5"/>
+      <c r="BJ35" s="5"/>
+      <c r="BK35" s="5"/>
+      <c r="BL35" s="5"/>
+      <c r="BM35" s="5"/>
+      <c r="BN35" s="5"/>
+      <c r="BO35" s="5"/>
+      <c r="BP35" s="5"/>
+      <c r="BQ35" s="5"/>
+      <c r="BR35" s="5"/>
+      <c r="BS35" s="5"/>
+      <c r="BT35" s="5"/>
+      <c r="BU35" s="5"/>
+      <c r="BV35" s="5"/>
+      <c r="BW35" s="5"/>
+      <c r="BX35" s="5"/>
+      <c r="BY35" s="5"/>
+      <c r="BZ35" s="5"/>
+      <c r="CA35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
@@ -5662,7 +5641,7 @@
         <f aca="false">CONCATENATE(D36,"_vs_",C36)</f>
         <v>xu_van_16_vs_xu_van_0</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="10" t="s">
         <v>211</v>
       </c>
       <c r="G36" s="5" t="n">
@@ -5785,7 +5764,7 @@
         <f aca="false">CONCATENATE(D37,"_vs_",C37)</f>
         <v>xu_rif_4_vs_xu_rif_0</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="10" t="s">
         <v>223</v>
       </c>
       <c r="G37" s="5" t="n">
@@ -5908,7 +5887,7 @@
         <f aca="false">CONCATENATE(D38,"_vs_",C38)</f>
         <v>xu_inh_02_vs_xu_inh_0</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="10" t="s">
         <v>229</v>
       </c>
       <c r="G38" s="5" t="n">
@@ -6031,7 +6010,7 @@
         <f aca="false">CONCATENATE(D39,"_vs_",C39)</f>
         <v>xu_inh_025_vs_xu_inh_0</v>
       </c>
-      <c r="F39" s="11"/>
+      <c r="F39" s="10"/>
       <c r="G39" s="5" t="n">
         <v>4</v>
       </c>
@@ -6152,7 +6131,7 @@
         <f aca="false">CONCATENATE(D40,"_vs_",C40)</f>
         <v>xu_emb_2.5_vs_xu_emb_0</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F40" s="10" t="s">
         <v>237</v>
       </c>
       <c r="G40" s="5" t="n">
@@ -6275,7 +6254,7 @@
         <f aca="false">CONCATENATE(D41,"_vs_",C41)</f>
         <v>xu_emb_3_vs_xu_emb_0</v>
       </c>
-      <c r="F41" s="11"/>
+      <c r="F41" s="10"/>
       <c r="G41" s="5" t="n">
         <v>3</v>
       </c>
@@ -6396,7 +6375,7 @@
         <f aca="false">CONCATENATE(D42,"_vs_",C42)</f>
         <v>xu_mero_2.5_vs_xu_mero_0</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="10" t="s">
         <v>242</v>
       </c>
       <c r="G42" s="5" t="n">
@@ -6509,10 +6488,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="12" t="s">
         <v>249</v>
       </c>
       <c r="E43" s="4" t="str">
@@ -6628,10 +6607,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="12" t="s">
         <v>256</v>
       </c>
       <c r="E44" s="4" t="str">
@@ -6747,10 +6726,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="12" t="s">
         <v>256</v>
       </c>
       <c r="E45" s="4" t="str">
@@ -6865,14 +6844,14 @@
         <v>1</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E46" s="4" t="str">
         <f aca="false">CONCATENATE(D46,"_vs_",C46)</f>
-        <v>carey_621_vs_mbio_H37Rv</v>
+        <v>carey_621_vs_carey_rv</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>260</v>
@@ -6884,25 +6863,25 @@
         <v>2</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="J46" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P46" s="5" t="s">
         <v>32</v>
@@ -6981,24 +6960,24 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B47" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E47" s="4" t="str">
         <f aca="false">CONCATENATE(D47,"_vs_",C47)</f>
-        <v>carey_630_vs_mbio_H37Rv</v>
+        <v>carey_630_vs_carey_rv</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G47" s="5" t="n">
         <v>14</v>
@@ -7007,25 +6986,25 @@
         <v>2</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J47" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>32</v>
@@ -7104,24 +7083,24 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B48" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E48" s="4" t="str">
         <f aca="false">CONCATENATE(D48,"_vs_",C48)</f>
-        <v>carey_631_vs_mbio_H37Rv</v>
+        <v>carey_631_vs_carey_rv</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G48" s="5" t="n">
         <v>14</v>
@@ -7130,25 +7109,25 @@
         <v>2</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="J48" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>32</v>
@@ -7227,24 +7206,24 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B49" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E49" s="4" t="str">
         <f aca="false">CONCATENATE(D49,"_vs_",C49)</f>
-        <v>carey_632_vs_mbio_H37Rv</v>
+        <v>carey_632_vs_carey_rv</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G49" s="5" t="n">
         <v>14</v>
@@ -7253,25 +7232,25 @@
         <v>2</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="J49" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>32</v>
@@ -7350,24 +7329,24 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B50" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E50" s="4" t="str">
         <f aca="false">CONCATENATE(D50,"_vs_",C50)</f>
-        <v>carey_641_vs_mbio_H37Rv</v>
+        <v>carey_641_vs_carey_rv</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G50" s="5" t="n">
         <v>14</v>
@@ -7376,25 +7355,25 @@
         <v>2</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="J50" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>32</v>
@@ -7473,24 +7452,24 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B51" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E51" s="4" t="str">
         <f aca="false">CONCATENATE(D51,"_vs_",C51)</f>
-        <v>carey_662_vs_mbio_H37Rv</v>
+        <v>carey_662_vs_carey_rv</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G51" s="5" t="n">
         <v>14</v>
@@ -7499,25 +7478,25 @@
         <v>2</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="J51" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P51" s="5" t="s">
         <v>32</v>
@@ -7596,24 +7575,24 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B52" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E52" s="4" t="str">
         <f aca="false">CONCATENATE(D52,"_vs_",C52)</f>
-        <v>carey_663_vs_mbio_H37Rv</v>
+        <v>carey_663_vs_carey_rv</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G52" s="5" t="n">
         <v>14</v>
@@ -7622,25 +7601,25 @@
         <v>2</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J52" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P52" s="5" t="s">
         <v>32</v>
@@ -7719,24 +7698,24 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B53" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E53" s="4" t="str">
         <f aca="false">CONCATENATE(D53,"_vs_",C53)</f>
-        <v>carey_667_vs_mbio_H37Rv</v>
+        <v>carey_667_vs_carey_rv</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G53" s="5" t="n">
         <v>14</v>
@@ -7745,25 +7724,25 @@
         <v>2</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="J53" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>32</v>
@@ -7842,24 +7821,24 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B54" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E54" s="4" t="str">
         <f aca="false">CONCATENATE(D54,"_vs_",C54)</f>
         <v>ritterhaus_hypoxia_H3_vs_ritterhaus_hypoxia_input</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G54" s="5" t="n">
         <v>8</v>
@@ -7868,22 +7847,22 @@
         <v>8</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="J54" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="O54" s="5" t="s">
         <v>30</v>
@@ -7898,7 +7877,7 @@
         <v>34</v>
       </c>
       <c r="S54" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="T54" s="5"/>
       <c r="U54" s="5"/>
@@ -7969,24 +7948,24 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B55" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E55" s="4" t="str">
         <f aca="false">CONCATENATE(D55,"_vs_",C55)</f>
         <v>ritterhaus_hypoxia_H6_vs_ritterhaus_hypoxia_input</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="G55" s="5" t="n">
         <v>8</v>
@@ -7995,22 +7974,22 @@
         <v>6</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="J55" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="O55" s="5" t="s">
         <v>30</v>
@@ -8025,7 +8004,7 @@
         <v>34</v>
       </c>
       <c r="S55" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="T55" s="5"/>
       <c r="U55" s="5"/>
@@ -8096,17 +8075,17 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B56" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E56" s="4" t="str">
         <f aca="false">CONCATENATE(D56,"_vs_",C56)</f>
@@ -8124,16 +8103,16 @@
         <v>2019</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="L56" s="20" t="s">
         <v>308</v>
       </c>
+      <c r="L56" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="M56" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O56" s="5" t="s">
         <v>30</v>
@@ -8153,7 +8132,7 @@
         <v>179</v>
       </c>
       <c r="X56" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="Y56" s="5"/>
       <c r="Z56" s="5" t="s">
@@ -8215,17 +8194,17 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B57" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E57" s="4" t="str">
         <f aca="false">CONCATENATE(D57,"_vs_",C57)</f>
@@ -8243,16 +8222,16 @@
         <v>2019</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="L57" s="20" t="s">
         <v>308</v>
       </c>
+      <c r="L57" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="M57" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O57" s="5" t="s">
         <v>30</v>
@@ -8272,7 +8251,7 @@
         <v>179</v>
       </c>
       <c r="X57" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="Y57" s="5"/>
       <c r="Z57" s="5" t="s">
@@ -8334,17 +8313,17 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B58" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E58" s="4" t="str">
         <f aca="false">CONCATENATE(D58,"_vs_",C58)</f>
@@ -8362,16 +8341,16 @@
         <v>2019</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="L58" s="20" t="s">
         <v>308</v>
       </c>
+      <c r="L58" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="M58" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O58" s="5" t="s">
         <v>30</v>
@@ -8391,7 +8370,7 @@
         <v>179</v>
       </c>
       <c r="X58" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="Y58" s="5"/>
       <c r="Z58" s="5" t="s">
@@ -8453,17 +8432,17 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B59" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E59" s="4" t="str">
         <f aca="false">CONCATENATE(D59,"_vs_",C59)</f>
@@ -8481,28 +8460,28 @@
         <v>2019</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="L59" s="20" t="s">
         <v>319</v>
       </c>
+      <c r="L59" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="M59" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="O59" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="P59" s="5" t="s">
         <v>32</v>
       </c>
       <c r="Q59" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="R59" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="S59" s="5"/>
       <c r="T59" s="5"/>
@@ -8572,17 +8551,17 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B60" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E60" s="4" t="str">
         <f aca="false">CONCATENATE(D60,"_vs_",C60)</f>
@@ -8596,19 +8575,19 @@
         <v>3</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M60" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N60" s="5" t="s">
         <v>76</v>
@@ -8627,7 +8606,7 @@
       </c>
       <c r="S60" s="5"/>
       <c r="T60" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="U60" s="5"/>
       <c r="V60" s="5" t="s">
@@ -8697,17 +8676,17 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B61" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E61" s="4" t="str">
         <f aca="false">CONCATENATE(D61,"_vs_",C61)</f>
@@ -8721,19 +8700,19 @@
         <v>2</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L61" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N61" s="5" t="s">
         <v>76</v>
@@ -8752,7 +8731,7 @@
       </c>
       <c r="S61" s="5"/>
       <c r="T61" s="5" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="U61" s="5"/>
       <c r="V61" s="5" t="s">
@@ -8822,17 +8801,17 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B62" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="D62" s="19" t="s">
         <v>338</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>339</v>
       </c>
       <c r="E62" s="4" t="str">
         <f aca="false">CONCATENATE(D62,"_vs_",C62)</f>
@@ -8846,17 +8825,17 @@
         <v>1</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="J62" s="5"/>
       <c r="K62" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
@@ -8871,10 +8850,10 @@
       </c>
       <c r="S62" s="5"/>
       <c r="T62" s="5" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="U62" s="5" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="V62" s="5" t="s">
         <v>64</v>
@@ -8943,17 +8922,17 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B63" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="D63" s="19" t="s">
         <v>343</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>344</v>
       </c>
       <c r="E63" s="4" t="str">
         <f aca="false">CONCATENATE(D63,"_vs_",C63)</f>
@@ -8967,17 +8946,17 @@
         <v>2</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="J63" s="5"/>
       <c r="K63" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N63" s="5"/>
       <c r="O63" s="5"/>
@@ -8992,10 +8971,10 @@
       </c>
       <c r="S63" s="5"/>
       <c r="T63" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="U63" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="V63" s="5" t="s">
         <v>64</v>
@@ -9064,17 +9043,17 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B64" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="D64" s="19" t="s">
-        <v>347</v>
+        <v>338</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>348</v>
       </c>
       <c r="E64" s="4" t="str">
         <f aca="false">CONCATENATE(D64,"_vs_",C64)</f>
@@ -9088,17 +9067,17 @@
         <v>1</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="J64" s="5"/>
       <c r="K64" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L64" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M64" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N64" s="5"/>
       <c r="O64" s="5"/>
@@ -9113,10 +9092,10 @@
       </c>
       <c r="S64" s="5"/>
       <c r="T64" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="U64" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="V64" s="5" t="s">
         <v>64</v>
@@ -9185,17 +9164,17 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B65" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D65" s="19" t="s">
-        <v>351</v>
+      <c r="D65" s="12" t="s">
+        <v>352</v>
       </c>
       <c r="E65" s="4" t="str">
         <f aca="false">CONCATENATE(D65,"_vs_",C65)</f>
@@ -9209,17 +9188,17 @@
         <v>2</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="J65" s="5"/>
       <c r="K65" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L65" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M65" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
@@ -9234,10 +9213,10 @@
       </c>
       <c r="S65" s="5"/>
       <c r="T65" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="U65" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="V65" s="5" t="s">
         <v>64</v>
@@ -9306,17 +9285,17 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B66" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="D66" s="19" t="s">
         <v>356</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>357</v>
       </c>
       <c r="E66" s="4" t="str">
         <f aca="false">CONCATENATE(D66,"_vs_",C66)</f>
@@ -9330,17 +9309,17 @@
         <v>1</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="J66" s="5"/>
       <c r="K66" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M66" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
@@ -9355,10 +9334,10 @@
       </c>
       <c r="S66" s="5"/>
       <c r="T66" s="5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="U66" s="5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="V66" s="5" t="s">
         <v>64</v>
@@ -9427,17 +9406,17 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B67" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="D67" s="19" t="s">
-        <v>360</v>
+        <v>338</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>361</v>
       </c>
       <c r="E67" s="4" t="str">
         <f aca="false">CONCATENATE(D67,"_vs_",C67)</f>
@@ -9451,17 +9430,17 @@
         <v>1</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="J67" s="5"/>
       <c r="K67" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M67" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
@@ -9476,10 +9455,10 @@
       </c>
       <c r="S67" s="5"/>
       <c r="T67" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="U67" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="V67" s="5" t="s">
         <v>64</v>
@@ -9548,17 +9527,17 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B68" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="D68" s="19" t="s">
-        <v>364</v>
+        <v>356</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>365</v>
       </c>
       <c r="E68" s="4" t="str">
         <f aca="false">CONCATENATE(D68,"_vs_",C68)</f>
@@ -9572,17 +9551,17 @@
         <v>1</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="J68" s="5"/>
       <c r="K68" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L68" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M68" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
@@ -9597,10 +9576,10 @@
       </c>
       <c r="S68" s="5"/>
       <c r="T68" s="5" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="U68" s="5" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="V68" s="5" t="s">
         <v>64</v>
@@ -9669,17 +9648,17 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B69" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>368</v>
+        <v>356</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>369</v>
       </c>
       <c r="E69" s="4" t="str">
         <f aca="false">CONCATENATE(D69,"_vs_",C69)</f>
@@ -9693,17 +9672,17 @@
         <v>1</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L69" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M69" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
@@ -9718,10 +9697,10 @@
       </c>
       <c r="S69" s="5"/>
       <c r="T69" s="5" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="U69" s="5" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="V69" s="5" t="s">
         <v>64</v>
@@ -9790,17 +9769,17 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B70" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C70" s="19" t="s">
-        <v>372</v>
-      </c>
-      <c r="D70" s="19" t="s">
+      <c r="C70" s="12" t="s">
         <v>373</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>374</v>
       </c>
       <c r="E70" s="4" t="str">
         <f aca="false">CONCATENATE(D70,"_vs_",C70)</f>
@@ -9814,17 +9793,17 @@
         <v>4</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="J70" s="5"/>
       <c r="K70" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L70" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M70" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N70" s="5"/>
       <c r="O70" s="5"/>
@@ -9840,7 +9819,7 @@
       <c r="S70" s="5"/>
       <c r="T70" s="5"/>
       <c r="U70" s="5" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="V70" s="5" t="s">
         <v>64</v>
@@ -9909,7 +9888,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B71" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -9918,8 +9897,8 @@
       <c r="C71" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D71" s="19" t="s">
-        <v>377</v>
+      <c r="D71" s="12" t="s">
+        <v>378</v>
       </c>
       <c r="E71" s="4" t="str">
         <f aca="false">CONCATENATE(D71,"_vs_",C71)</f>
@@ -9933,17 +9912,17 @@
         <v>1</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="J71" s="5"/>
       <c r="K71" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L71" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M71" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N71" s="5"/>
       <c r="O71" s="5"/>
@@ -9959,7 +9938,7 @@
       <c r="S71" s="5"/>
       <c r="T71" s="5"/>
       <c r="U71" s="5" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="V71" s="5" t="s">
         <v>64</v>
@@ -10028,7 +10007,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B72" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -10037,8 +10016,8 @@
       <c r="C72" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D72" s="19" t="s">
-        <v>381</v>
+      <c r="D72" s="12" t="s">
+        <v>382</v>
       </c>
       <c r="E72" s="4" t="str">
         <f aca="false">CONCATENATE(D72,"_vs_",C72)</f>
@@ -10052,17 +10031,17 @@
         <v>1</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="J72" s="5"/>
       <c r="K72" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L72" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M72" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N72" s="5"/>
       <c r="O72" s="5"/>
@@ -10078,7 +10057,7 @@
       <c r="S72" s="5"/>
       <c r="T72" s="5"/>
       <c r="U72" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="V72" s="5" t="s">
         <v>64</v>
@@ -10147,7 +10126,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B73" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -10156,8 +10135,8 @@
       <c r="C73" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D73" s="19" t="s">
-        <v>385</v>
+      <c r="D73" s="12" t="s">
+        <v>386</v>
       </c>
       <c r="E73" s="4" t="str">
         <f aca="false">CONCATENATE(D73,"_vs_",C73)</f>
@@ -10171,17 +10150,17 @@
         <v>1</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="J73" s="5"/>
       <c r="K73" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L73" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M73" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N73" s="5"/>
       <c r="O73" s="5"/>
@@ -10197,7 +10176,7 @@
       <c r="S73" s="5"/>
       <c r="T73" s="5"/>
       <c r="U73" s="5" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="V73" s="5" t="s">
         <v>64</v>
@@ -10266,7 +10245,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B74" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -10275,8 +10254,8 @@
       <c r="C74" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D74" s="19" t="s">
-        <v>389</v>
+      <c r="D74" s="12" t="s">
+        <v>390</v>
       </c>
       <c r="E74" s="4" t="str">
         <f aca="false">CONCATENATE(D74,"_vs_",C74)</f>
@@ -10290,17 +10269,17 @@
         <v>1</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="J74" s="5"/>
       <c r="K74" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M74" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N74" s="5"/>
       <c r="O74" s="5"/>
@@ -10316,7 +10295,7 @@
       <c r="S74" s="5"/>
       <c r="T74" s="5"/>
       <c r="U74" s="5" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="V74" s="5" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
made new dash data
</commit_message>
<xml_diff>
--- a/data/column_descriptors_standardized.xlsx
+++ b/data/column_descriptors_standardized.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="393">
   <si>
     <t xml:space="preserve">column_ID</t>
   </si>
@@ -803,6 +803,9 @@
   </si>
   <si>
     <t xml:space="preserve">2018_Carey_1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carey_rv</t>
   </si>
   <si>
     <t xml:space="preserve">carey_621</t>
@@ -1326,7 +1329,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1363,10 +1366,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1380,31 +1379,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1491,11 +1470,11 @@
   <dimension ref="A1:CA74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I23" activeCellId="0" sqref="I23"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="D55" activeCellId="0" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2434,14 +2413,14 @@
         <f aca="false">CONCATENATE(D9,"_vs_",C9)</f>
         <v>griffin_glycerol_vs_mbio_H37Rv</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="5" t="n">
         <v>14</v>
       </c>
       <c r="H9" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="5" t="n">
         <v>2013</v>
       </c>
@@ -2918,7 +2897,7 @@
         <f aca="false">CONCATENATE(D13,"_vs_",C13)</f>
         <v>zhang_mhcii_mouse_d45_vs_zhang_wt_mouse_d45</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>95</v>
       </c>
       <c r="G13" s="5" t="n">
@@ -3277,17 +3256,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>108</v>
       </c>
       <c r="E16" s="4" t="str">
         <f aca="false">CONCATENATE(D16,"_vs_",C16)</f>
         <v>zhang_DETA-NO_pH_7.0_vs_zhang_pH_7.0_no_NO_control</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>106</v>
       </c>
       <c r="G16" s="5" t="n">
@@ -3564,7 +3543,7 @@
       <c r="P18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q18" s="12" t="s">
+      <c r="Q18" s="11" t="s">
         <v>33</v>
       </c>
       <c r="R18" s="5" t="s">
@@ -3685,7 +3664,7 @@
       <c r="P19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q19" s="12" t="s">
+      <c r="Q19" s="11" t="s">
         <v>33</v>
       </c>
       <c r="R19" s="5" t="s">
@@ -4378,10 +4357,10 @@
       <c r="P25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q25" s="12" t="s">
+      <c r="Q25" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="R25" s="12" t="s">
+      <c r="R25" s="11" t="s">
         <v>34</v>
       </c>
       <c r="S25" s="5"/>
@@ -4452,1197 +4431,1197 @@
       <c r="BZ25" s="5"/>
       <c r="CA25" s="5"/>
     </row>
-    <row r="26" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B26" s="13" t="n">
+      <c r="B26" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="E26" s="9" t="str">
+      <c r="E26" s="4" t="str">
         <f aca="false">CONCATENATE(D26,"_vs_",C26)</f>
         <v>dejesus_H37Rv_day32_vs_dejesus_H37Rv_day0</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="13" t="n">
+      <c r="F26" s="4"/>
+      <c r="G26" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H26" s="13" t="n">
+      <c r="H26" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="13" t="n">
+      <c r="I26" s="12"/>
+      <c r="J26" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K26" s="9" t="s">
+      <c r="K26" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L26" s="15" t="s">
+      <c r="L26" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M26" s="13" t="s">
+      <c r="M26" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N26" s="13" t="s">
+      <c r="N26" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O26" s="13" t="s">
+      <c r="O26" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P26" s="13" t="s">
+      <c r="P26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13" t="s">
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W26" s="13" t="s">
+      <c r="W26" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X26" s="13"/>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="13"/>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="13"/>
-      <c r="AC26" s="13"/>
-      <c r="AD26" s="13"/>
-      <c r="AE26" s="13"/>
-      <c r="AF26" s="13"/>
-      <c r="AG26" s="13"/>
-      <c r="AH26" s="13"/>
-      <c r="AI26" s="13"/>
-      <c r="AJ26" s="13"/>
-      <c r="AK26" s="13"/>
-      <c r="AL26" s="13"/>
-      <c r="AM26" s="13"/>
-      <c r="AN26" s="13"/>
-      <c r="AO26" s="13"/>
-      <c r="AP26" s="13"/>
-      <c r="AQ26" s="13"/>
-      <c r="AR26" s="13"/>
-      <c r="AS26" s="13"/>
-      <c r="AT26" s="13"/>
-      <c r="AU26" s="13"/>
-      <c r="AV26" s="13"/>
-      <c r="AW26" s="13"/>
-      <c r="AX26" s="13"/>
-      <c r="AY26" s="13"/>
-      <c r="AZ26" s="13"/>
-      <c r="BA26" s="13"/>
-      <c r="BB26" s="13"/>
-      <c r="BC26" s="13"/>
-      <c r="BD26" s="13"/>
-      <c r="BE26" s="13"/>
-      <c r="BF26" s="13"/>
-      <c r="BG26" s="13"/>
-      <c r="BH26" s="13"/>
-      <c r="BI26" s="13"/>
-      <c r="BJ26" s="13"/>
-      <c r="BK26" s="13"/>
-      <c r="BL26" s="13"/>
-      <c r="BM26" s="13"/>
-      <c r="BN26" s="13"/>
-      <c r="BO26" s="13"/>
-      <c r="BP26" s="13"/>
-      <c r="BQ26" s="13"/>
-      <c r="BR26" s="13"/>
-      <c r="BS26" s="13"/>
-      <c r="BT26" s="13"/>
-      <c r="BU26" s="13"/>
-      <c r="BV26" s="13"/>
-      <c r="BW26" s="13"/>
-      <c r="BX26" s="13"/>
-      <c r="BY26" s="13"/>
-      <c r="BZ26" s="13"/>
-      <c r="CA26" s="13"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="5"/>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="5"/>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="5"/>
+      <c r="AL26" s="5"/>
+      <c r="AM26" s="5"/>
+      <c r="AN26" s="5"/>
+      <c r="AO26" s="5"/>
+      <c r="AP26" s="5"/>
+      <c r="AQ26" s="5"/>
+      <c r="AR26" s="5"/>
+      <c r="AS26" s="5"/>
+      <c r="AT26" s="5"/>
+      <c r="AU26" s="5"/>
+      <c r="AV26" s="5"/>
+      <c r="AW26" s="5"/>
+      <c r="AX26" s="5"/>
+      <c r="AY26" s="5"/>
+      <c r="AZ26" s="5"/>
+      <c r="BA26" s="5"/>
+      <c r="BB26" s="5"/>
+      <c r="BC26" s="5"/>
+      <c r="BD26" s="5"/>
+      <c r="BE26" s="5"/>
+      <c r="BF26" s="5"/>
+      <c r="BG26" s="5"/>
+      <c r="BH26" s="5"/>
+      <c r="BI26" s="5"/>
+      <c r="BJ26" s="5"/>
+      <c r="BK26" s="5"/>
+      <c r="BL26" s="5"/>
+      <c r="BM26" s="5"/>
+      <c r="BN26" s="5"/>
+      <c r="BO26" s="5"/>
+      <c r="BP26" s="5"/>
+      <c r="BQ26" s="5"/>
+      <c r="BR26" s="5"/>
+      <c r="BS26" s="5"/>
+      <c r="BT26" s="5"/>
+      <c r="BU26" s="5"/>
+      <c r="BV26" s="5"/>
+      <c r="BW26" s="5"/>
+      <c r="BX26" s="5"/>
+      <c r="BY26" s="5"/>
+      <c r="BZ26" s="5"/>
+      <c r="CA26" s="5"/>
     </row>
-    <row r="27" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B27" s="13" t="n">
+      <c r="B27" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E27" s="9" t="str">
+      <c r="E27" s="4" t="str">
         <f aca="false">CONCATENATE(D27,"_vs_",C27)</f>
         <v>dejesus_Rv1432_day0_vs_dejesus_H37Rv_day0</v>
       </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="13" t="n">
+      <c r="F27" s="4"/>
+      <c r="G27" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H27" s="13" t="n">
+      <c r="H27" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="J27" s="13" t="n">
+      <c r="J27" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K27" s="9" t="s">
+      <c r="K27" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L27" s="18" t="s">
+      <c r="L27" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="M27" s="13" t="s">
+      <c r="M27" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N27" s="13" t="s">
+      <c r="N27" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O27" s="13" t="s">
+      <c r="O27" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P27" s="13" t="s">
+      <c r="P27" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13" t="s">
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13" t="s">
+      <c r="U27" s="5"/>
+      <c r="V27" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W27" s="13" t="s">
+      <c r="W27" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
-      <c r="AA27" s="16"/>
-      <c r="AB27" s="13"/>
-      <c r="AC27" s="13"/>
-      <c r="AD27" s="13"/>
-      <c r="AE27" s="13"/>
-      <c r="AF27" s="13"/>
-      <c r="AG27" s="13"/>
-      <c r="AH27" s="13"/>
-      <c r="AI27" s="13"/>
-      <c r="AJ27" s="13"/>
-      <c r="AK27" s="13"/>
-      <c r="AL27" s="13"/>
-      <c r="AM27" s="13"/>
-      <c r="AN27" s="13"/>
-      <c r="AO27" s="13"/>
-      <c r="AP27" s="13"/>
-      <c r="AQ27" s="13"/>
-      <c r="AR27" s="13"/>
-      <c r="AS27" s="13"/>
-      <c r="AT27" s="13"/>
-      <c r="AU27" s="13"/>
-      <c r="AV27" s="13"/>
-      <c r="AW27" s="13"/>
-      <c r="AX27" s="13"/>
-      <c r="AY27" s="13"/>
-      <c r="AZ27" s="13"/>
-      <c r="BA27" s="13"/>
-      <c r="BB27" s="13"/>
-      <c r="BC27" s="13"/>
-      <c r="BD27" s="13"/>
-      <c r="BE27" s="13"/>
-      <c r="BF27" s="13"/>
-      <c r="BG27" s="13"/>
-      <c r="BH27" s="13"/>
-      <c r="BI27" s="13"/>
-      <c r="BJ27" s="13"/>
-      <c r="BK27" s="13"/>
-      <c r="BL27" s="13"/>
-      <c r="BM27" s="13"/>
-      <c r="BN27" s="13"/>
-      <c r="BO27" s="13"/>
-      <c r="BP27" s="13"/>
-      <c r="BQ27" s="13"/>
-      <c r="BR27" s="13"/>
-      <c r="BS27" s="13"/>
-      <c r="BT27" s="13"/>
-      <c r="BU27" s="13"/>
-      <c r="BV27" s="13"/>
-      <c r="BW27" s="13"/>
-      <c r="BX27" s="13"/>
-      <c r="BY27" s="13"/>
-      <c r="BZ27" s="13"/>
-      <c r="CA27" s="13"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="5"/>
+      <c r="AG27" s="5"/>
+      <c r="AH27" s="5"/>
+      <c r="AI27" s="5"/>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="5"/>
+      <c r="AL27" s="5"/>
+      <c r="AM27" s="5"/>
+      <c r="AN27" s="5"/>
+      <c r="AO27" s="5"/>
+      <c r="AP27" s="5"/>
+      <c r="AQ27" s="5"/>
+      <c r="AR27" s="5"/>
+      <c r="AS27" s="5"/>
+      <c r="AT27" s="5"/>
+      <c r="AU27" s="5"/>
+      <c r="AV27" s="5"/>
+      <c r="AW27" s="5"/>
+      <c r="AX27" s="5"/>
+      <c r="AY27" s="5"/>
+      <c r="AZ27" s="5"/>
+      <c r="BA27" s="5"/>
+      <c r="BB27" s="5"/>
+      <c r="BC27" s="5"/>
+      <c r="BD27" s="5"/>
+      <c r="BE27" s="5"/>
+      <c r="BF27" s="5"/>
+      <c r="BG27" s="5"/>
+      <c r="BH27" s="5"/>
+      <c r="BI27" s="5"/>
+      <c r="BJ27" s="5"/>
+      <c r="BK27" s="5"/>
+      <c r="BL27" s="5"/>
+      <c r="BM27" s="5"/>
+      <c r="BN27" s="5"/>
+      <c r="BO27" s="5"/>
+      <c r="BP27" s="5"/>
+      <c r="BQ27" s="5"/>
+      <c r="BR27" s="5"/>
+      <c r="BS27" s="5"/>
+      <c r="BT27" s="5"/>
+      <c r="BU27" s="5"/>
+      <c r="BV27" s="5"/>
+      <c r="BW27" s="5"/>
+      <c r="BX27" s="5"/>
+      <c r="BY27" s="5"/>
+      <c r="BZ27" s="5"/>
+      <c r="CA27" s="5"/>
     </row>
-    <row r="28" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B28" s="13" t="n">
+      <c r="B28" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E28" s="9" t="str">
+      <c r="E28" s="4" t="str">
         <f aca="false">CONCATENATE(D28,"_vs_",C28)</f>
         <v>dejesus_Rv1432_day32_vs_dejesus_Rv1432_day0</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="13" t="n">
+      <c r="F28" s="4"/>
+      <c r="G28" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H28" s="13" t="n">
+      <c r="H28" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I28" s="9" t="s">
+      <c r="I28" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="J28" s="13" t="n">
+      <c r="J28" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="K28" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L28" s="15" t="s">
+      <c r="L28" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M28" s="13" t="s">
+      <c r="M28" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N28" s="13" t="s">
+      <c r="N28" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O28" s="13" t="s">
+      <c r="O28" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P28" s="13" t="s">
+      <c r="P28" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13" t="s">
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13" t="s">
+      <c r="U28" s="5"/>
+      <c r="V28" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W28" s="13" t="s">
+      <c r="W28" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X28" s="13"/>
-      <c r="Y28" s="13"/>
-      <c r="Z28" s="13"/>
-      <c r="AA28" s="16"/>
-      <c r="AB28" s="13"/>
-      <c r="AC28" s="13"/>
-      <c r="AD28" s="13"/>
-      <c r="AE28" s="13"/>
-      <c r="AF28" s="13"/>
-      <c r="AG28" s="13"/>
-      <c r="AH28" s="13"/>
-      <c r="AI28" s="13"/>
-      <c r="AJ28" s="13"/>
-      <c r="AK28" s="13"/>
-      <c r="AL28" s="13"/>
-      <c r="AM28" s="13"/>
-      <c r="AN28" s="13"/>
-      <c r="AO28" s="13"/>
-      <c r="AP28" s="13"/>
-      <c r="AQ28" s="13"/>
-      <c r="AR28" s="13"/>
-      <c r="AS28" s="13"/>
-      <c r="AT28" s="13"/>
-      <c r="AU28" s="13"/>
-      <c r="AV28" s="13"/>
-      <c r="AW28" s="13"/>
-      <c r="AX28" s="13"/>
-      <c r="AY28" s="13"/>
-      <c r="AZ28" s="13"/>
-      <c r="BA28" s="13"/>
-      <c r="BB28" s="13"/>
-      <c r="BC28" s="13"/>
-      <c r="BD28" s="13"/>
-      <c r="BE28" s="13"/>
-      <c r="BF28" s="13"/>
-      <c r="BG28" s="13"/>
-      <c r="BH28" s="13"/>
-      <c r="BI28" s="13"/>
-      <c r="BJ28" s="13"/>
-      <c r="BK28" s="13"/>
-      <c r="BL28" s="13"/>
-      <c r="BM28" s="13"/>
-      <c r="BN28" s="13"/>
-      <c r="BO28" s="13"/>
-      <c r="BP28" s="13"/>
-      <c r="BQ28" s="13"/>
-      <c r="BR28" s="13"/>
-      <c r="BS28" s="13"/>
-      <c r="BT28" s="13"/>
-      <c r="BU28" s="13"/>
-      <c r="BV28" s="13"/>
-      <c r="BW28" s="13"/>
-      <c r="BX28" s="13"/>
-      <c r="BY28" s="13"/>
-      <c r="BZ28" s="13"/>
-      <c r="CA28" s="13"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="5"/>
+      <c r="AG28" s="5"/>
+      <c r="AH28" s="5"/>
+      <c r="AI28" s="5"/>
+      <c r="AJ28" s="5"/>
+      <c r="AK28" s="5"/>
+      <c r="AL28" s="5"/>
+      <c r="AM28" s="5"/>
+      <c r="AN28" s="5"/>
+      <c r="AO28" s="5"/>
+      <c r="AP28" s="5"/>
+      <c r="AQ28" s="5"/>
+      <c r="AR28" s="5"/>
+      <c r="AS28" s="5"/>
+      <c r="AT28" s="5"/>
+      <c r="AU28" s="5"/>
+      <c r="AV28" s="5"/>
+      <c r="AW28" s="5"/>
+      <c r="AX28" s="5"/>
+      <c r="AY28" s="5"/>
+      <c r="AZ28" s="5"/>
+      <c r="BA28" s="5"/>
+      <c r="BB28" s="5"/>
+      <c r="BC28" s="5"/>
+      <c r="BD28" s="5"/>
+      <c r="BE28" s="5"/>
+      <c r="BF28" s="5"/>
+      <c r="BG28" s="5"/>
+      <c r="BH28" s="5"/>
+      <c r="BI28" s="5"/>
+      <c r="BJ28" s="5"/>
+      <c r="BK28" s="5"/>
+      <c r="BL28" s="5"/>
+      <c r="BM28" s="5"/>
+      <c r="BN28" s="5"/>
+      <c r="BO28" s="5"/>
+      <c r="BP28" s="5"/>
+      <c r="BQ28" s="5"/>
+      <c r="BR28" s="5"/>
+      <c r="BS28" s="5"/>
+      <c r="BT28" s="5"/>
+      <c r="BU28" s="5"/>
+      <c r="BV28" s="5"/>
+      <c r="BW28" s="5"/>
+      <c r="BX28" s="5"/>
+      <c r="BY28" s="5"/>
+      <c r="BZ28" s="5"/>
+      <c r="CA28" s="5"/>
     </row>
-    <row r="29" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B29" s="13" t="n">
+      <c r="B29" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E29" s="11" t="str">
+      <c r="E29" s="10" t="str">
         <f aca="false">CONCATENATE(D29,"_vs_",C29)</f>
         <v>dejesus_Rv1432_day32_vs_dejesus_H37Rv_day32</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="G29" s="13" t="n">
+      <c r="G29" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H29" s="13" t="n">
+      <c r="H29" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="I29" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="J29" s="13" t="n">
+      <c r="J29" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K29" s="9" t="s">
+      <c r="K29" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L29" s="15" t="s">
+      <c r="L29" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M29" s="13" t="s">
+      <c r="M29" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N29" s="13" t="s">
+      <c r="N29" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O29" s="13" t="s">
+      <c r="O29" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P29" s="13" t="s">
+      <c r="P29" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13" t="s">
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="U29" s="13"/>
-      <c r="V29" s="13" t="s">
+      <c r="U29" s="5"/>
+      <c r="V29" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W29" s="13" t="s">
+      <c r="W29" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X29" s="13"/>
-      <c r="Y29" s="13"/>
-      <c r="Z29" s="13"/>
-      <c r="AA29" s="16"/>
-      <c r="AB29" s="13"/>
-      <c r="AC29" s="13"/>
-      <c r="AD29" s="13"/>
-      <c r="AE29" s="13"/>
-      <c r="AF29" s="13"/>
-      <c r="AG29" s="13"/>
-      <c r="AH29" s="13"/>
-      <c r="AI29" s="13"/>
-      <c r="AJ29" s="13"/>
-      <c r="AK29" s="13"/>
-      <c r="AL29" s="13"/>
-      <c r="AM29" s="13"/>
-      <c r="AN29" s="13"/>
-      <c r="AO29" s="13"/>
-      <c r="AP29" s="13"/>
-      <c r="AQ29" s="13"/>
-      <c r="AR29" s="13"/>
-      <c r="AS29" s="13"/>
-      <c r="AT29" s="13"/>
-      <c r="AU29" s="13"/>
-      <c r="AV29" s="13"/>
-      <c r="AW29" s="13"/>
-      <c r="AX29" s="13"/>
-      <c r="AY29" s="13"/>
-      <c r="AZ29" s="13"/>
-      <c r="BA29" s="13"/>
-      <c r="BB29" s="13"/>
-      <c r="BC29" s="13"/>
-      <c r="BD29" s="13"/>
-      <c r="BE29" s="13"/>
-      <c r="BF29" s="13"/>
-      <c r="BG29" s="13"/>
-      <c r="BH29" s="13"/>
-      <c r="BI29" s="13"/>
-      <c r="BJ29" s="13"/>
-      <c r="BK29" s="13"/>
-      <c r="BL29" s="13"/>
-      <c r="BM29" s="13"/>
-      <c r="BN29" s="13"/>
-      <c r="BO29" s="13"/>
-      <c r="BP29" s="13"/>
-      <c r="BQ29" s="13"/>
-      <c r="BR29" s="13"/>
-      <c r="BS29" s="13"/>
-      <c r="BT29" s="13"/>
-      <c r="BU29" s="13"/>
-      <c r="BV29" s="13"/>
-      <c r="BW29" s="13"/>
-      <c r="BX29" s="13"/>
-      <c r="BY29" s="13"/>
-      <c r="BZ29" s="13"/>
-      <c r="CA29" s="13"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
+      <c r="AH29" s="5"/>
+      <c r="AI29" s="5"/>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="5"/>
+      <c r="AL29" s="5"/>
+      <c r="AM29" s="5"/>
+      <c r="AN29" s="5"/>
+      <c r="AO29" s="5"/>
+      <c r="AP29" s="5"/>
+      <c r="AQ29" s="5"/>
+      <c r="AR29" s="5"/>
+      <c r="AS29" s="5"/>
+      <c r="AT29" s="5"/>
+      <c r="AU29" s="5"/>
+      <c r="AV29" s="5"/>
+      <c r="AW29" s="5"/>
+      <c r="AX29" s="5"/>
+      <c r="AY29" s="5"/>
+      <c r="AZ29" s="5"/>
+      <c r="BA29" s="5"/>
+      <c r="BB29" s="5"/>
+      <c r="BC29" s="5"/>
+      <c r="BD29" s="5"/>
+      <c r="BE29" s="5"/>
+      <c r="BF29" s="5"/>
+      <c r="BG29" s="5"/>
+      <c r="BH29" s="5"/>
+      <c r="BI29" s="5"/>
+      <c r="BJ29" s="5"/>
+      <c r="BK29" s="5"/>
+      <c r="BL29" s="5"/>
+      <c r="BM29" s="5"/>
+      <c r="BN29" s="5"/>
+      <c r="BO29" s="5"/>
+      <c r="BP29" s="5"/>
+      <c r="BQ29" s="5"/>
+      <c r="BR29" s="5"/>
+      <c r="BS29" s="5"/>
+      <c r="BT29" s="5"/>
+      <c r="BU29" s="5"/>
+      <c r="BV29" s="5"/>
+      <c r="BW29" s="5"/>
+      <c r="BX29" s="5"/>
+      <c r="BY29" s="5"/>
+      <c r="BZ29" s="5"/>
+      <c r="CA29" s="5"/>
     </row>
-    <row r="30" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B30" s="13" t="n">
+      <c r="B30" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E30" s="9" t="str">
+      <c r="E30" s="4" t="str">
         <f aca="false">CONCATENATE(D30,"_vs_",C30)</f>
         <v>dejesus_Rv1565c_day0_vs_dejesus_H37Rv_day0</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="13" t="n">
+      <c r="F30" s="4"/>
+      <c r="G30" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H30" s="13" t="n">
+      <c r="H30" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="J30" s="13" t="n">
+      <c r="J30" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="K30" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L30" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M30" s="13" t="s">
+      <c r="M30" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N30" s="13" t="s">
+      <c r="N30" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O30" s="13" t="s">
+      <c r="O30" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P30" s="13" t="s">
+      <c r="P30" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13" t="s">
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="U30" s="13"/>
-      <c r="V30" s="13" t="s">
+      <c r="U30" s="5"/>
+      <c r="V30" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W30" s="13" t="s">
+      <c r="W30" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X30" s="13"/>
-      <c r="Y30" s="13"/>
-      <c r="Z30" s="13"/>
-      <c r="AA30" s="16"/>
-      <c r="AB30" s="13"/>
-      <c r="AC30" s="13"/>
-      <c r="AD30" s="13"/>
-      <c r="AE30" s="13"/>
-      <c r="AF30" s="13"/>
-      <c r="AG30" s="13"/>
-      <c r="AH30" s="13"/>
-      <c r="AI30" s="13"/>
-      <c r="AJ30" s="13"/>
-      <c r="AK30" s="13"/>
-      <c r="AL30" s="13"/>
-      <c r="AM30" s="13"/>
-      <c r="AN30" s="13"/>
-      <c r="AO30" s="13"/>
-      <c r="AP30" s="13"/>
-      <c r="AQ30" s="13"/>
-      <c r="AR30" s="13"/>
-      <c r="AS30" s="13"/>
-      <c r="AT30" s="13"/>
-      <c r="AU30" s="13"/>
-      <c r="AV30" s="13"/>
-      <c r="AW30" s="13"/>
-      <c r="AX30" s="13"/>
-      <c r="AY30" s="13"/>
-      <c r="AZ30" s="13"/>
-      <c r="BA30" s="13"/>
-      <c r="BB30" s="13"/>
-      <c r="BC30" s="13"/>
-      <c r="BD30" s="13"/>
-      <c r="BE30" s="13"/>
-      <c r="BF30" s="13"/>
-      <c r="BG30" s="13"/>
-      <c r="BH30" s="13"/>
-      <c r="BI30" s="13"/>
-      <c r="BJ30" s="13"/>
-      <c r="BK30" s="13"/>
-      <c r="BL30" s="13"/>
-      <c r="BM30" s="13"/>
-      <c r="BN30" s="13"/>
-      <c r="BO30" s="13"/>
-      <c r="BP30" s="13"/>
-      <c r="BQ30" s="13"/>
-      <c r="BR30" s="13"/>
-      <c r="BS30" s="13"/>
-      <c r="BT30" s="13"/>
-      <c r="BU30" s="13"/>
-      <c r="BV30" s="13"/>
-      <c r="BW30" s="13"/>
-      <c r="BX30" s="13"/>
-      <c r="BY30" s="13"/>
-      <c r="BZ30" s="13"/>
-      <c r="CA30" s="13"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
+      <c r="AG30" s="5"/>
+      <c r="AH30" s="5"/>
+      <c r="AI30" s="5"/>
+      <c r="AJ30" s="5"/>
+      <c r="AK30" s="5"/>
+      <c r="AL30" s="5"/>
+      <c r="AM30" s="5"/>
+      <c r="AN30" s="5"/>
+      <c r="AO30" s="5"/>
+      <c r="AP30" s="5"/>
+      <c r="AQ30" s="5"/>
+      <c r="AR30" s="5"/>
+      <c r="AS30" s="5"/>
+      <c r="AT30" s="5"/>
+      <c r="AU30" s="5"/>
+      <c r="AV30" s="5"/>
+      <c r="AW30" s="5"/>
+      <c r="AX30" s="5"/>
+      <c r="AY30" s="5"/>
+      <c r="AZ30" s="5"/>
+      <c r="BA30" s="5"/>
+      <c r="BB30" s="5"/>
+      <c r="BC30" s="5"/>
+      <c r="BD30" s="5"/>
+      <c r="BE30" s="5"/>
+      <c r="BF30" s="5"/>
+      <c r="BG30" s="5"/>
+      <c r="BH30" s="5"/>
+      <c r="BI30" s="5"/>
+      <c r="BJ30" s="5"/>
+      <c r="BK30" s="5"/>
+      <c r="BL30" s="5"/>
+      <c r="BM30" s="5"/>
+      <c r="BN30" s="5"/>
+      <c r="BO30" s="5"/>
+      <c r="BP30" s="5"/>
+      <c r="BQ30" s="5"/>
+      <c r="BR30" s="5"/>
+      <c r="BS30" s="5"/>
+      <c r="BT30" s="5"/>
+      <c r="BU30" s="5"/>
+      <c r="BV30" s="5"/>
+      <c r="BW30" s="5"/>
+      <c r="BX30" s="5"/>
+      <c r="BY30" s="5"/>
+      <c r="BZ30" s="5"/>
+      <c r="CA30" s="5"/>
     </row>
-    <row r="31" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B31" s="13" t="n">
+      <c r="B31" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="E31" s="9" t="str">
+      <c r="E31" s="4" t="str">
         <f aca="false">CONCATENATE(D31,"_vs_",C31)</f>
         <v>dejesus_Rv1565c_day32_vs_dejesus_Rv1565c_day0</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="13" t="n">
+      <c r="F31" s="4"/>
+      <c r="G31" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H31" s="13" t="n">
+      <c r="H31" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="J31" s="13" t="n">
+      <c r="J31" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K31" s="9" t="s">
+      <c r="K31" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L31" s="15" t="s">
+      <c r="L31" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M31" s="13" t="s">
+      <c r="M31" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N31" s="13" t="s">
+      <c r="N31" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O31" s="13" t="s">
+      <c r="O31" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P31" s="13" t="s">
+      <c r="P31" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13" t="s">
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="U31" s="13"/>
-      <c r="V31" s="13" t="s">
+      <c r="U31" s="5"/>
+      <c r="V31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W31" s="13" t="s">
+      <c r="W31" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X31" s="13"/>
-      <c r="Y31" s="13"/>
-      <c r="Z31" s="13"/>
-      <c r="AA31" s="16"/>
-      <c r="AB31" s="13"/>
-      <c r="AC31" s="13"/>
-      <c r="AD31" s="13"/>
-      <c r="AE31" s="13"/>
-      <c r="AF31" s="13"/>
-      <c r="AG31" s="13"/>
-      <c r="AH31" s="13"/>
-      <c r="AI31" s="13"/>
-      <c r="AJ31" s="13"/>
-      <c r="AK31" s="13"/>
-      <c r="AL31" s="13"/>
-      <c r="AM31" s="13"/>
-      <c r="AN31" s="13"/>
-      <c r="AO31" s="13"/>
-      <c r="AP31" s="13"/>
-      <c r="AQ31" s="13"/>
-      <c r="AR31" s="13"/>
-      <c r="AS31" s="13"/>
-      <c r="AT31" s="13"/>
-      <c r="AU31" s="13"/>
-      <c r="AV31" s="13"/>
-      <c r="AW31" s="13"/>
-      <c r="AX31" s="13"/>
-      <c r="AY31" s="13"/>
-      <c r="AZ31" s="13"/>
-      <c r="BA31" s="13"/>
-      <c r="BB31" s="13"/>
-      <c r="BC31" s="13"/>
-      <c r="BD31" s="13"/>
-      <c r="BE31" s="13"/>
-      <c r="BF31" s="13"/>
-      <c r="BG31" s="13"/>
-      <c r="BH31" s="13"/>
-      <c r="BI31" s="13"/>
-      <c r="BJ31" s="13"/>
-      <c r="BK31" s="13"/>
-      <c r="BL31" s="13"/>
-      <c r="BM31" s="13"/>
-      <c r="BN31" s="13"/>
-      <c r="BO31" s="13"/>
-      <c r="BP31" s="13"/>
-      <c r="BQ31" s="13"/>
-      <c r="BR31" s="13"/>
-      <c r="BS31" s="13"/>
-      <c r="BT31" s="13"/>
-      <c r="BU31" s="13"/>
-      <c r="BV31" s="13"/>
-      <c r="BW31" s="13"/>
-      <c r="BX31" s="13"/>
-      <c r="BY31" s="13"/>
-      <c r="BZ31" s="13"/>
-      <c r="CA31" s="13"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="5"/>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="5"/>
+      <c r="AE31" s="5"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="5"/>
+      <c r="AH31" s="5"/>
+      <c r="AI31" s="5"/>
+      <c r="AJ31" s="5"/>
+      <c r="AK31" s="5"/>
+      <c r="AL31" s="5"/>
+      <c r="AM31" s="5"/>
+      <c r="AN31" s="5"/>
+      <c r="AO31" s="5"/>
+      <c r="AP31" s="5"/>
+      <c r="AQ31" s="5"/>
+      <c r="AR31" s="5"/>
+      <c r="AS31" s="5"/>
+      <c r="AT31" s="5"/>
+      <c r="AU31" s="5"/>
+      <c r="AV31" s="5"/>
+      <c r="AW31" s="5"/>
+      <c r="AX31" s="5"/>
+      <c r="AY31" s="5"/>
+      <c r="AZ31" s="5"/>
+      <c r="BA31" s="5"/>
+      <c r="BB31" s="5"/>
+      <c r="BC31" s="5"/>
+      <c r="BD31" s="5"/>
+      <c r="BE31" s="5"/>
+      <c r="BF31" s="5"/>
+      <c r="BG31" s="5"/>
+      <c r="BH31" s="5"/>
+      <c r="BI31" s="5"/>
+      <c r="BJ31" s="5"/>
+      <c r="BK31" s="5"/>
+      <c r="BL31" s="5"/>
+      <c r="BM31" s="5"/>
+      <c r="BN31" s="5"/>
+      <c r="BO31" s="5"/>
+      <c r="BP31" s="5"/>
+      <c r="BQ31" s="5"/>
+      <c r="BR31" s="5"/>
+      <c r="BS31" s="5"/>
+      <c r="BT31" s="5"/>
+      <c r="BU31" s="5"/>
+      <c r="BV31" s="5"/>
+      <c r="BW31" s="5"/>
+      <c r="BX31" s="5"/>
+      <c r="BY31" s="5"/>
+      <c r="BZ31" s="5"/>
+      <c r="CA31" s="5"/>
     </row>
-    <row r="32" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B32" s="13" t="n">
+      <c r="B32" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="E32" s="11" t="str">
+      <c r="E32" s="10" t="str">
         <f aca="false">CONCATENATE(D32,"_vs_",C32)</f>
         <v>dejesus_Rv1565c_day32_vs_dejesus_H37Rv_day32</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="G32" s="13" t="n">
+      <c r="G32" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H32" s="13" t="n">
+      <c r="H32" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="J32" s="13" t="n">
+      <c r="J32" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="K32" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L32" s="15" t="s">
+      <c r="L32" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M32" s="13" t="s">
+      <c r="M32" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N32" s="13" t="s">
+      <c r="N32" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O32" s="13" t="s">
+      <c r="O32" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P32" s="13" t="s">
+      <c r="P32" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="13" t="s">
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="U32" s="13"/>
-      <c r="V32" s="13" t="s">
+      <c r="U32" s="5"/>
+      <c r="V32" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W32" s="13" t="s">
+      <c r="W32" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X32" s="13"/>
-      <c r="Y32" s="13"/>
-      <c r="Z32" s="13"/>
-      <c r="AA32" s="16"/>
-      <c r="AB32" s="13"/>
-      <c r="AC32" s="13"/>
-      <c r="AD32" s="13"/>
-      <c r="AE32" s="13"/>
-      <c r="AF32" s="13"/>
-      <c r="AG32" s="13"/>
-      <c r="AH32" s="13"/>
-      <c r="AI32" s="13"/>
-      <c r="AJ32" s="13"/>
-      <c r="AK32" s="13"/>
-      <c r="AL32" s="13"/>
-      <c r="AM32" s="13"/>
-      <c r="AN32" s="13"/>
-      <c r="AO32" s="13"/>
-      <c r="AP32" s="13"/>
-      <c r="AQ32" s="13"/>
-      <c r="AR32" s="13"/>
-      <c r="AS32" s="13"/>
-      <c r="AT32" s="13"/>
-      <c r="AU32" s="13"/>
-      <c r="AV32" s="13"/>
-      <c r="AW32" s="13"/>
-      <c r="AX32" s="13"/>
-      <c r="AY32" s="13"/>
-      <c r="AZ32" s="13"/>
-      <c r="BA32" s="13"/>
-      <c r="BB32" s="13"/>
-      <c r="BC32" s="13"/>
-      <c r="BD32" s="13"/>
-      <c r="BE32" s="13"/>
-      <c r="BF32" s="13"/>
-      <c r="BG32" s="13"/>
-      <c r="BH32" s="13"/>
-      <c r="BI32" s="13"/>
-      <c r="BJ32" s="13"/>
-      <c r="BK32" s="13"/>
-      <c r="BL32" s="13"/>
-      <c r="BM32" s="13"/>
-      <c r="BN32" s="13"/>
-      <c r="BO32" s="13"/>
-      <c r="BP32" s="13"/>
-      <c r="BQ32" s="13"/>
-      <c r="BR32" s="13"/>
-      <c r="BS32" s="13"/>
-      <c r="BT32" s="13"/>
-      <c r="BU32" s="13"/>
-      <c r="BV32" s="13"/>
-      <c r="BW32" s="13"/>
-      <c r="BX32" s="13"/>
-      <c r="BY32" s="13"/>
-      <c r="BZ32" s="13"/>
-      <c r="CA32" s="13"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="5"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="5"/>
+      <c r="AG32" s="5"/>
+      <c r="AH32" s="5"/>
+      <c r="AI32" s="5"/>
+      <c r="AJ32" s="5"/>
+      <c r="AK32" s="5"/>
+      <c r="AL32" s="5"/>
+      <c r="AM32" s="5"/>
+      <c r="AN32" s="5"/>
+      <c r="AO32" s="5"/>
+      <c r="AP32" s="5"/>
+      <c r="AQ32" s="5"/>
+      <c r="AR32" s="5"/>
+      <c r="AS32" s="5"/>
+      <c r="AT32" s="5"/>
+      <c r="AU32" s="5"/>
+      <c r="AV32" s="5"/>
+      <c r="AW32" s="5"/>
+      <c r="AX32" s="5"/>
+      <c r="AY32" s="5"/>
+      <c r="AZ32" s="5"/>
+      <c r="BA32" s="5"/>
+      <c r="BB32" s="5"/>
+      <c r="BC32" s="5"/>
+      <c r="BD32" s="5"/>
+      <c r="BE32" s="5"/>
+      <c r="BF32" s="5"/>
+      <c r="BG32" s="5"/>
+      <c r="BH32" s="5"/>
+      <c r="BI32" s="5"/>
+      <c r="BJ32" s="5"/>
+      <c r="BK32" s="5"/>
+      <c r="BL32" s="5"/>
+      <c r="BM32" s="5"/>
+      <c r="BN32" s="5"/>
+      <c r="BO32" s="5"/>
+      <c r="BP32" s="5"/>
+      <c r="BQ32" s="5"/>
+      <c r="BR32" s="5"/>
+      <c r="BS32" s="5"/>
+      <c r="BT32" s="5"/>
+      <c r="BU32" s="5"/>
+      <c r="BV32" s="5"/>
+      <c r="BW32" s="5"/>
+      <c r="BX32" s="5"/>
+      <c r="BY32" s="5"/>
+      <c r="BZ32" s="5"/>
+      <c r="CA32" s="5"/>
     </row>
-    <row r="33" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="s">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B33" s="13" t="n">
+      <c r="B33" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E33" s="9" t="str">
+      <c r="E33" s="4" t="str">
         <f aca="false">CONCATENATE(D33,"_vs_",C33)</f>
         <v>dejesus_Rv2680_day0_vs_dejesus_H37Rv_day0</v>
       </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="13" t="n">
+      <c r="F33" s="4"/>
+      <c r="G33" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H33" s="13" t="n">
+      <c r="H33" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="J33" s="13" t="n">
+      <c r="J33" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K33" s="9" t="s">
+      <c r="K33" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L33" s="15" t="s">
+      <c r="L33" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M33" s="13" t="s">
+      <c r="M33" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N33" s="13" t="s">
+      <c r="N33" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O33" s="13" t="s">
+      <c r="O33" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P33" s="13" t="s">
+      <c r="P33" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="13"/>
-      <c r="S33" s="13"/>
-      <c r="T33" s="13" t="s">
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="U33" s="13"/>
-      <c r="V33" s="13" t="s">
+      <c r="U33" s="5"/>
+      <c r="V33" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W33" s="13" t="s">
+      <c r="W33" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X33" s="13"/>
-      <c r="Y33" s="13"/>
-      <c r="Z33" s="13"/>
-      <c r="AA33" s="16"/>
-      <c r="AB33" s="13"/>
-      <c r="AC33" s="13"/>
-      <c r="AD33" s="13"/>
-      <c r="AE33" s="13"/>
-      <c r="AF33" s="13"/>
-      <c r="AG33" s="13"/>
-      <c r="AH33" s="13"/>
-      <c r="AI33" s="13"/>
-      <c r="AJ33" s="13"/>
-      <c r="AK33" s="13"/>
-      <c r="AL33" s="13"/>
-      <c r="AM33" s="13"/>
-      <c r="AN33" s="13"/>
-      <c r="AO33" s="13"/>
-      <c r="AP33" s="13"/>
-      <c r="AQ33" s="13"/>
-      <c r="AR33" s="13"/>
-      <c r="AS33" s="13"/>
-      <c r="AT33" s="13"/>
-      <c r="AU33" s="13"/>
-      <c r="AV33" s="13"/>
-      <c r="AW33" s="13"/>
-      <c r="AX33" s="13"/>
-      <c r="AY33" s="13"/>
-      <c r="AZ33" s="13"/>
-      <c r="BA33" s="13"/>
-      <c r="BB33" s="13"/>
-      <c r="BC33" s="13"/>
-      <c r="BD33" s="13"/>
-      <c r="BE33" s="13"/>
-      <c r="BF33" s="13"/>
-      <c r="BG33" s="13"/>
-      <c r="BH33" s="13"/>
-      <c r="BI33" s="13"/>
-      <c r="BJ33" s="13"/>
-      <c r="BK33" s="13"/>
-      <c r="BL33" s="13"/>
-      <c r="BM33" s="13"/>
-      <c r="BN33" s="13"/>
-      <c r="BO33" s="13"/>
-      <c r="BP33" s="13"/>
-      <c r="BQ33" s="13"/>
-      <c r="BR33" s="13"/>
-      <c r="BS33" s="13"/>
-      <c r="BT33" s="13"/>
-      <c r="BU33" s="13"/>
-      <c r="BV33" s="13"/>
-      <c r="BW33" s="13"/>
-      <c r="BX33" s="13"/>
-      <c r="BY33" s="13"/>
-      <c r="BZ33" s="13"/>
-      <c r="CA33" s="13"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="5"/>
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="5"/>
+      <c r="AE33" s="5"/>
+      <c r="AF33" s="5"/>
+      <c r="AG33" s="5"/>
+      <c r="AH33" s="5"/>
+      <c r="AI33" s="5"/>
+      <c r="AJ33" s="5"/>
+      <c r="AK33" s="5"/>
+      <c r="AL33" s="5"/>
+      <c r="AM33" s="5"/>
+      <c r="AN33" s="5"/>
+      <c r="AO33" s="5"/>
+      <c r="AP33" s="5"/>
+      <c r="AQ33" s="5"/>
+      <c r="AR33" s="5"/>
+      <c r="AS33" s="5"/>
+      <c r="AT33" s="5"/>
+      <c r="AU33" s="5"/>
+      <c r="AV33" s="5"/>
+      <c r="AW33" s="5"/>
+      <c r="AX33" s="5"/>
+      <c r="AY33" s="5"/>
+      <c r="AZ33" s="5"/>
+      <c r="BA33" s="5"/>
+      <c r="BB33" s="5"/>
+      <c r="BC33" s="5"/>
+      <c r="BD33" s="5"/>
+      <c r="BE33" s="5"/>
+      <c r="BF33" s="5"/>
+      <c r="BG33" s="5"/>
+      <c r="BH33" s="5"/>
+      <c r="BI33" s="5"/>
+      <c r="BJ33" s="5"/>
+      <c r="BK33" s="5"/>
+      <c r="BL33" s="5"/>
+      <c r="BM33" s="5"/>
+      <c r="BN33" s="5"/>
+      <c r="BO33" s="5"/>
+      <c r="BP33" s="5"/>
+      <c r="BQ33" s="5"/>
+      <c r="BR33" s="5"/>
+      <c r="BS33" s="5"/>
+      <c r="BT33" s="5"/>
+      <c r="BU33" s="5"/>
+      <c r="BV33" s="5"/>
+      <c r="BW33" s="5"/>
+      <c r="BX33" s="5"/>
+      <c r="BY33" s="5"/>
+      <c r="BZ33" s="5"/>
+      <c r="CA33" s="5"/>
     </row>
-    <row r="34" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="s">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B34" s="13" t="n">
+      <c r="B34" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="E34" s="9" t="str">
+      <c r="E34" s="4" t="str">
         <f aca="false">CONCATENATE(D34,"_vs_",C34)</f>
         <v>dejesus_Rv2680_day32_vs_dejesus_Rv2680_day0</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="13" t="n">
+      <c r="F34" s="4"/>
+      <c r="G34" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H34" s="13" t="n">
+      <c r="H34" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I34" s="9" t="s">
+      <c r="I34" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="J34" s="13" t="n">
+      <c r="J34" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K34" s="9" t="s">
+      <c r="K34" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L34" s="15" t="s">
+      <c r="L34" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M34" s="13" t="s">
+      <c r="M34" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N34" s="13" t="s">
+      <c r="N34" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O34" s="13" t="s">
+      <c r="O34" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P34" s="13" t="s">
+      <c r="P34" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="13"/>
-      <c r="T34" s="13" t="s">
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="U34" s="13"/>
-      <c r="V34" s="13" t="s">
+      <c r="U34" s="5"/>
+      <c r="V34" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W34" s="13" t="s">
+      <c r="W34" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X34" s="13"/>
-      <c r="Y34" s="13"/>
-      <c r="Z34" s="13"/>
-      <c r="AA34" s="16"/>
-      <c r="AB34" s="13"/>
-      <c r="AC34" s="13"/>
-      <c r="AD34" s="13"/>
-      <c r="AE34" s="13"/>
-      <c r="AF34" s="13"/>
-      <c r="AG34" s="13"/>
-      <c r="AH34" s="13"/>
-      <c r="AI34" s="13"/>
-      <c r="AJ34" s="13"/>
-      <c r="AK34" s="13"/>
-      <c r="AL34" s="13"/>
-      <c r="AM34" s="13"/>
-      <c r="AN34" s="13"/>
-      <c r="AO34" s="13"/>
-      <c r="AP34" s="13"/>
-      <c r="AQ34" s="13"/>
-      <c r="AR34" s="13"/>
-      <c r="AS34" s="13"/>
-      <c r="AT34" s="13"/>
-      <c r="AU34" s="13"/>
-      <c r="AV34" s="13"/>
-      <c r="AW34" s="13"/>
-      <c r="AX34" s="13"/>
-      <c r="AY34" s="13"/>
-      <c r="AZ34" s="13"/>
-      <c r="BA34" s="13"/>
-      <c r="BB34" s="13"/>
-      <c r="BC34" s="13"/>
-      <c r="BD34" s="13"/>
-      <c r="BE34" s="13"/>
-      <c r="BF34" s="13"/>
-      <c r="BG34" s="13"/>
-      <c r="BH34" s="13"/>
-      <c r="BI34" s="13"/>
-      <c r="BJ34" s="13"/>
-      <c r="BK34" s="13"/>
-      <c r="BL34" s="13"/>
-      <c r="BM34" s="13"/>
-      <c r="BN34" s="13"/>
-      <c r="BO34" s="13"/>
-      <c r="BP34" s="13"/>
-      <c r="BQ34" s="13"/>
-      <c r="BR34" s="13"/>
-      <c r="BS34" s="13"/>
-      <c r="BT34" s="13"/>
-      <c r="BU34" s="13"/>
-      <c r="BV34" s="13"/>
-      <c r="BW34" s="13"/>
-      <c r="BX34" s="13"/>
-      <c r="BY34" s="13"/>
-      <c r="BZ34" s="13"/>
-      <c r="CA34" s="13"/>
+      <c r="X34" s="5"/>
+      <c r="Y34" s="5"/>
+      <c r="Z34" s="5"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="5"/>
+      <c r="AC34" s="5"/>
+      <c r="AD34" s="5"/>
+      <c r="AE34" s="5"/>
+      <c r="AF34" s="5"/>
+      <c r="AG34" s="5"/>
+      <c r="AH34" s="5"/>
+      <c r="AI34" s="5"/>
+      <c r="AJ34" s="5"/>
+      <c r="AK34" s="5"/>
+      <c r="AL34" s="5"/>
+      <c r="AM34" s="5"/>
+      <c r="AN34" s="5"/>
+      <c r="AO34" s="5"/>
+      <c r="AP34" s="5"/>
+      <c r="AQ34" s="5"/>
+      <c r="AR34" s="5"/>
+      <c r="AS34" s="5"/>
+      <c r="AT34" s="5"/>
+      <c r="AU34" s="5"/>
+      <c r="AV34" s="5"/>
+      <c r="AW34" s="5"/>
+      <c r="AX34" s="5"/>
+      <c r="AY34" s="5"/>
+      <c r="AZ34" s="5"/>
+      <c r="BA34" s="5"/>
+      <c r="BB34" s="5"/>
+      <c r="BC34" s="5"/>
+      <c r="BD34" s="5"/>
+      <c r="BE34" s="5"/>
+      <c r="BF34" s="5"/>
+      <c r="BG34" s="5"/>
+      <c r="BH34" s="5"/>
+      <c r="BI34" s="5"/>
+      <c r="BJ34" s="5"/>
+      <c r="BK34" s="5"/>
+      <c r="BL34" s="5"/>
+      <c r="BM34" s="5"/>
+      <c r="BN34" s="5"/>
+      <c r="BO34" s="5"/>
+      <c r="BP34" s="5"/>
+      <c r="BQ34" s="5"/>
+      <c r="BR34" s="5"/>
+      <c r="BS34" s="5"/>
+      <c r="BT34" s="5"/>
+      <c r="BU34" s="5"/>
+      <c r="BV34" s="5"/>
+      <c r="BW34" s="5"/>
+      <c r="BX34" s="5"/>
+      <c r="BY34" s="5"/>
+      <c r="BZ34" s="5"/>
+      <c r="CA34" s="5"/>
     </row>
-    <row r="35" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="s">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B35" s="13" t="n">
+      <c r="B35" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="E35" s="11" t="str">
+      <c r="E35" s="10" t="str">
         <f aca="false">CONCATENATE(D35,"_vs_",C35)</f>
         <v>dejesus_Rv2680_day32_vs_dejesus_H37Rv_day32</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="G35" s="13" t="n">
+      <c r="G35" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H35" s="13" t="n">
+      <c r="H35" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="J35" s="13" t="n">
+      <c r="J35" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="K35" s="9" t="s">
+      <c r="K35" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L35" s="15" t="s">
+      <c r="L35" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="M35" s="13" t="s">
+      <c r="M35" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="N35" s="13" t="s">
+      <c r="N35" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O35" s="13" t="s">
+      <c r="O35" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P35" s="13" t="s">
+      <c r="P35" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="13" t="s">
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="U35" s="13"/>
-      <c r="V35" s="13" t="s">
+      <c r="U35" s="5"/>
+      <c r="V35" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W35" s="13" t="s">
+      <c r="W35" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X35" s="13"/>
-      <c r="Y35" s="13"/>
-      <c r="Z35" s="13"/>
-      <c r="AA35" s="16"/>
-      <c r="AB35" s="13"/>
-      <c r="AC35" s="13"/>
-      <c r="AD35" s="13"/>
-      <c r="AE35" s="13"/>
-      <c r="AF35" s="13"/>
-      <c r="AG35" s="13"/>
-      <c r="AH35" s="13"/>
-      <c r="AI35" s="13"/>
-      <c r="AJ35" s="13"/>
-      <c r="AK35" s="13"/>
-      <c r="AL35" s="13"/>
-      <c r="AM35" s="13"/>
-      <c r="AN35" s="13"/>
-      <c r="AO35" s="13"/>
-      <c r="AP35" s="13"/>
-      <c r="AQ35" s="13"/>
-      <c r="AR35" s="13"/>
-      <c r="AS35" s="13"/>
-      <c r="AT35" s="13"/>
-      <c r="AU35" s="13"/>
-      <c r="AV35" s="13"/>
-      <c r="AW35" s="13"/>
-      <c r="AX35" s="13"/>
-      <c r="AY35" s="13"/>
-      <c r="AZ35" s="13"/>
-      <c r="BA35" s="13"/>
-      <c r="BB35" s="13"/>
-      <c r="BC35" s="13"/>
-      <c r="BD35" s="13"/>
-      <c r="BE35" s="13"/>
-      <c r="BF35" s="13"/>
-      <c r="BG35" s="13"/>
-      <c r="BH35" s="13"/>
-      <c r="BI35" s="13"/>
-      <c r="BJ35" s="13"/>
-      <c r="BK35" s="13"/>
-      <c r="BL35" s="13"/>
-      <c r="BM35" s="13"/>
-      <c r="BN35" s="13"/>
-      <c r="BO35" s="13"/>
-      <c r="BP35" s="13"/>
-      <c r="BQ35" s="13"/>
-      <c r="BR35" s="13"/>
-      <c r="BS35" s="13"/>
-      <c r="BT35" s="13"/>
-      <c r="BU35" s="13"/>
-      <c r="BV35" s="13"/>
-      <c r="BW35" s="13"/>
-      <c r="BX35" s="13"/>
-      <c r="BY35" s="13"/>
-      <c r="BZ35" s="13"/>
-      <c r="CA35" s="13"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="5"/>
+      <c r="AC35" s="5"/>
+      <c r="AD35" s="5"/>
+      <c r="AE35" s="5"/>
+      <c r="AF35" s="5"/>
+      <c r="AG35" s="5"/>
+      <c r="AH35" s="5"/>
+      <c r="AI35" s="5"/>
+      <c r="AJ35" s="5"/>
+      <c r="AK35" s="5"/>
+      <c r="AL35" s="5"/>
+      <c r="AM35" s="5"/>
+      <c r="AN35" s="5"/>
+      <c r="AO35" s="5"/>
+      <c r="AP35" s="5"/>
+      <c r="AQ35" s="5"/>
+      <c r="AR35" s="5"/>
+      <c r="AS35" s="5"/>
+      <c r="AT35" s="5"/>
+      <c r="AU35" s="5"/>
+      <c r="AV35" s="5"/>
+      <c r="AW35" s="5"/>
+      <c r="AX35" s="5"/>
+      <c r="AY35" s="5"/>
+      <c r="AZ35" s="5"/>
+      <c r="BA35" s="5"/>
+      <c r="BB35" s="5"/>
+      <c r="BC35" s="5"/>
+      <c r="BD35" s="5"/>
+      <c r="BE35" s="5"/>
+      <c r="BF35" s="5"/>
+      <c r="BG35" s="5"/>
+      <c r="BH35" s="5"/>
+      <c r="BI35" s="5"/>
+      <c r="BJ35" s="5"/>
+      <c r="BK35" s="5"/>
+      <c r="BL35" s="5"/>
+      <c r="BM35" s="5"/>
+      <c r="BN35" s="5"/>
+      <c r="BO35" s="5"/>
+      <c r="BP35" s="5"/>
+      <c r="BQ35" s="5"/>
+      <c r="BR35" s="5"/>
+      <c r="BS35" s="5"/>
+      <c r="BT35" s="5"/>
+      <c r="BU35" s="5"/>
+      <c r="BV35" s="5"/>
+      <c r="BW35" s="5"/>
+      <c r="BX35" s="5"/>
+      <c r="BY35" s="5"/>
+      <c r="BZ35" s="5"/>
+      <c r="CA35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
@@ -5662,7 +5641,7 @@
         <f aca="false">CONCATENATE(D36,"_vs_",C36)</f>
         <v>xu_van_16_vs_xu_van_0</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="10" t="s">
         <v>211</v>
       </c>
       <c r="G36" s="5" t="n">
@@ -5785,7 +5764,7 @@
         <f aca="false">CONCATENATE(D37,"_vs_",C37)</f>
         <v>xu_rif_4_vs_xu_rif_0</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="10" t="s">
         <v>223</v>
       </c>
       <c r="G37" s="5" t="n">
@@ -5908,7 +5887,7 @@
         <f aca="false">CONCATENATE(D38,"_vs_",C38)</f>
         <v>xu_inh_02_vs_xu_inh_0</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="10" t="s">
         <v>229</v>
       </c>
       <c r="G38" s="5" t="n">
@@ -6031,7 +6010,7 @@
         <f aca="false">CONCATENATE(D39,"_vs_",C39)</f>
         <v>xu_inh_025_vs_xu_inh_0</v>
       </c>
-      <c r="F39" s="11"/>
+      <c r="F39" s="10"/>
       <c r="G39" s="5" t="n">
         <v>4</v>
       </c>
@@ -6152,7 +6131,7 @@
         <f aca="false">CONCATENATE(D40,"_vs_",C40)</f>
         <v>xu_emb_2.5_vs_xu_emb_0</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F40" s="10" t="s">
         <v>237</v>
       </c>
       <c r="G40" s="5" t="n">
@@ -6275,7 +6254,7 @@
         <f aca="false">CONCATENATE(D41,"_vs_",C41)</f>
         <v>xu_emb_3_vs_xu_emb_0</v>
       </c>
-      <c r="F41" s="11"/>
+      <c r="F41" s="10"/>
       <c r="G41" s="5" t="n">
         <v>3</v>
       </c>
@@ -6396,7 +6375,7 @@
         <f aca="false">CONCATENATE(D42,"_vs_",C42)</f>
         <v>xu_mero_2.5_vs_xu_mero_0</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="10" t="s">
         <v>242</v>
       </c>
       <c r="G42" s="5" t="n">
@@ -6509,10 +6488,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="12" t="s">
         <v>249</v>
       </c>
       <c r="E43" s="4" t="str">
@@ -6628,10 +6607,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="12" t="s">
         <v>256</v>
       </c>
       <c r="E44" s="4" t="str">
@@ -6747,10 +6726,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="12" t="s">
         <v>256</v>
       </c>
       <c r="E45" s="4" t="str">
@@ -6865,14 +6844,14 @@
         <v>1</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E46" s="4" t="str">
         <f aca="false">CONCATENATE(D46,"_vs_",C46)</f>
-        <v>carey_621_vs_mbio_H37Rv</v>
+        <v>carey_621_vs_carey_rv</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>260</v>
@@ -6884,25 +6863,25 @@
         <v>2</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="J46" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P46" s="5" t="s">
         <v>32</v>
@@ -6981,24 +6960,24 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B47" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E47" s="4" t="str">
         <f aca="false">CONCATENATE(D47,"_vs_",C47)</f>
-        <v>carey_630_vs_mbio_H37Rv</v>
+        <v>carey_630_vs_carey_rv</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G47" s="5" t="n">
         <v>14</v>
@@ -7007,25 +6986,25 @@
         <v>2</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J47" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>32</v>
@@ -7104,24 +7083,24 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B48" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E48" s="4" t="str">
         <f aca="false">CONCATENATE(D48,"_vs_",C48)</f>
-        <v>carey_631_vs_mbio_H37Rv</v>
+        <v>carey_631_vs_carey_rv</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G48" s="5" t="n">
         <v>14</v>
@@ -7130,25 +7109,25 @@
         <v>2</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="J48" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>32</v>
@@ -7227,24 +7206,24 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B49" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E49" s="4" t="str">
         <f aca="false">CONCATENATE(D49,"_vs_",C49)</f>
-        <v>carey_632_vs_mbio_H37Rv</v>
+        <v>carey_632_vs_carey_rv</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G49" s="5" t="n">
         <v>14</v>
@@ -7253,25 +7232,25 @@
         <v>2</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="J49" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>32</v>
@@ -7350,24 +7329,24 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B50" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E50" s="4" t="str">
         <f aca="false">CONCATENATE(D50,"_vs_",C50)</f>
-        <v>carey_641_vs_mbio_H37Rv</v>
+        <v>carey_641_vs_carey_rv</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G50" s="5" t="n">
         <v>14</v>
@@ -7376,25 +7355,25 @@
         <v>2</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="J50" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>32</v>
@@ -7473,24 +7452,24 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B51" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E51" s="4" t="str">
         <f aca="false">CONCATENATE(D51,"_vs_",C51)</f>
-        <v>carey_662_vs_mbio_H37Rv</v>
+        <v>carey_662_vs_carey_rv</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G51" s="5" t="n">
         <v>14</v>
@@ -7499,25 +7478,25 @@
         <v>2</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="J51" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P51" s="5" t="s">
         <v>32</v>
@@ -7596,24 +7575,24 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B52" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E52" s="4" t="str">
         <f aca="false">CONCATENATE(D52,"_vs_",C52)</f>
-        <v>carey_663_vs_mbio_H37Rv</v>
+        <v>carey_663_vs_carey_rv</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G52" s="5" t="n">
         <v>14</v>
@@ -7622,25 +7601,25 @@
         <v>2</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J52" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P52" s="5" t="s">
         <v>32</v>
@@ -7719,24 +7698,24 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B53" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>72</v>
+        <v>261</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E53" s="4" t="str">
         <f aca="false">CONCATENATE(D53,"_vs_",C53)</f>
-        <v>carey_667_vs_mbio_H37Rv</v>
+        <v>carey_667_vs_carey_rv</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G53" s="5" t="n">
         <v>14</v>
@@ -7745,25 +7724,25 @@
         <v>2</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="J53" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>32</v>
@@ -7842,24 +7821,24 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B54" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E54" s="4" t="str">
         <f aca="false">CONCATENATE(D54,"_vs_",C54)</f>
         <v>ritterhaus_hypoxia_H3_vs_ritterhaus_hypoxia_input</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G54" s="5" t="n">
         <v>8</v>
@@ -7868,22 +7847,22 @@
         <v>8</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="J54" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="O54" s="5" t="s">
         <v>30</v>
@@ -7898,7 +7877,7 @@
         <v>34</v>
       </c>
       <c r="S54" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="T54" s="5"/>
       <c r="U54" s="5"/>
@@ -7969,24 +7948,24 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B55" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E55" s="4" t="str">
         <f aca="false">CONCATENATE(D55,"_vs_",C55)</f>
         <v>ritterhaus_hypoxia_H6_vs_ritterhaus_hypoxia_input</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="G55" s="5" t="n">
         <v>8</v>
@@ -7995,22 +7974,22 @@
         <v>6</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="J55" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="O55" s="5" t="s">
         <v>30</v>
@@ -8025,7 +8004,7 @@
         <v>34</v>
       </c>
       <c r="S55" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="T55" s="5"/>
       <c r="U55" s="5"/>
@@ -8096,17 +8075,17 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B56" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E56" s="4" t="str">
         <f aca="false">CONCATENATE(D56,"_vs_",C56)</f>
@@ -8124,16 +8103,16 @@
         <v>2019</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="L56" s="20" t="s">
         <v>308</v>
       </c>
+      <c r="L56" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="M56" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O56" s="5" t="s">
         <v>30</v>
@@ -8153,7 +8132,7 @@
         <v>179</v>
       </c>
       <c r="X56" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="Y56" s="5"/>
       <c r="Z56" s="5" t="s">
@@ -8215,17 +8194,17 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B57" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E57" s="4" t="str">
         <f aca="false">CONCATENATE(D57,"_vs_",C57)</f>
@@ -8243,16 +8222,16 @@
         <v>2019</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="L57" s="20" t="s">
         <v>308</v>
       </c>
+      <c r="L57" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="M57" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O57" s="5" t="s">
         <v>30</v>
@@ -8272,7 +8251,7 @@
         <v>179</v>
       </c>
       <c r="X57" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="Y57" s="5"/>
       <c r="Z57" s="5" t="s">
@@ -8334,17 +8313,17 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B58" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E58" s="4" t="str">
         <f aca="false">CONCATENATE(D58,"_vs_",C58)</f>
@@ -8362,16 +8341,16 @@
         <v>2019</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="L58" s="20" t="s">
         <v>308</v>
       </c>
+      <c r="L58" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="M58" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O58" s="5" t="s">
         <v>30</v>
@@ -8391,7 +8370,7 @@
         <v>179</v>
       </c>
       <c r="X58" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="Y58" s="5"/>
       <c r="Z58" s="5" t="s">
@@ -8453,17 +8432,17 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B59" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E59" s="4" t="str">
         <f aca="false">CONCATENATE(D59,"_vs_",C59)</f>
@@ -8481,28 +8460,28 @@
         <v>2019</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="L59" s="20" t="s">
         <v>319</v>
       </c>
+      <c r="L59" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="M59" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="O59" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="P59" s="5" t="s">
         <v>32</v>
       </c>
       <c r="Q59" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="R59" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="S59" s="5"/>
       <c r="T59" s="5"/>
@@ -8572,17 +8551,17 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B60" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E60" s="4" t="str">
         <f aca="false">CONCATENATE(D60,"_vs_",C60)</f>
@@ -8596,19 +8575,19 @@
         <v>3</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M60" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N60" s="5" t="s">
         <v>76</v>
@@ -8627,7 +8606,7 @@
       </c>
       <c r="S60" s="5"/>
       <c r="T60" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="U60" s="5"/>
       <c r="V60" s="5" t="s">
@@ -8697,17 +8676,17 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B61" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E61" s="4" t="str">
         <f aca="false">CONCATENATE(D61,"_vs_",C61)</f>
@@ -8721,19 +8700,19 @@
         <v>2</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L61" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N61" s="5" t="s">
         <v>76</v>
@@ -8752,7 +8731,7 @@
       </c>
       <c r="S61" s="5"/>
       <c r="T61" s="5" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="U61" s="5"/>
       <c r="V61" s="5" t="s">
@@ -8822,17 +8801,17 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B62" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="D62" s="19" t="s">
         <v>338</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>339</v>
       </c>
       <c r="E62" s="4" t="str">
         <f aca="false">CONCATENATE(D62,"_vs_",C62)</f>
@@ -8846,17 +8825,17 @@
         <v>1</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="J62" s="5"/>
       <c r="K62" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
@@ -8871,10 +8850,10 @@
       </c>
       <c r="S62" s="5"/>
       <c r="T62" s="5" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="U62" s="5" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="V62" s="5" t="s">
         <v>64</v>
@@ -8943,17 +8922,17 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B63" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="D63" s="19" t="s">
         <v>343</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>344</v>
       </c>
       <c r="E63" s="4" t="str">
         <f aca="false">CONCATENATE(D63,"_vs_",C63)</f>
@@ -8967,17 +8946,17 @@
         <v>2</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="J63" s="5"/>
       <c r="K63" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N63" s="5"/>
       <c r="O63" s="5"/>
@@ -8992,10 +8971,10 @@
       </c>
       <c r="S63" s="5"/>
       <c r="T63" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="U63" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="V63" s="5" t="s">
         <v>64</v>
@@ -9064,17 +9043,17 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B64" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="D64" s="19" t="s">
-        <v>347</v>
+        <v>338</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>348</v>
       </c>
       <c r="E64" s="4" t="str">
         <f aca="false">CONCATENATE(D64,"_vs_",C64)</f>
@@ -9088,17 +9067,17 @@
         <v>1</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="J64" s="5"/>
       <c r="K64" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L64" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M64" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N64" s="5"/>
       <c r="O64" s="5"/>
@@ -9113,10 +9092,10 @@
       </c>
       <c r="S64" s="5"/>
       <c r="T64" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="U64" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="V64" s="5" t="s">
         <v>64</v>
@@ -9185,17 +9164,17 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B65" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D65" s="19" t="s">
-        <v>351</v>
+      <c r="D65" s="12" t="s">
+        <v>352</v>
       </c>
       <c r="E65" s="4" t="str">
         <f aca="false">CONCATENATE(D65,"_vs_",C65)</f>
@@ -9209,17 +9188,17 @@
         <v>2</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="J65" s="5"/>
       <c r="K65" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L65" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M65" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
@@ -9234,10 +9213,10 @@
       </c>
       <c r="S65" s="5"/>
       <c r="T65" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="U65" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="V65" s="5" t="s">
         <v>64</v>
@@ -9306,17 +9285,17 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B66" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="D66" s="19" t="s">
         <v>356</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>357</v>
       </c>
       <c r="E66" s="4" t="str">
         <f aca="false">CONCATENATE(D66,"_vs_",C66)</f>
@@ -9330,17 +9309,17 @@
         <v>1</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="J66" s="5"/>
       <c r="K66" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M66" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
@@ -9355,10 +9334,10 @@
       </c>
       <c r="S66" s="5"/>
       <c r="T66" s="5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="U66" s="5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="V66" s="5" t="s">
         <v>64</v>
@@ -9427,17 +9406,17 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B67" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="D67" s="19" t="s">
-        <v>360</v>
+        <v>338</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>361</v>
       </c>
       <c r="E67" s="4" t="str">
         <f aca="false">CONCATENATE(D67,"_vs_",C67)</f>
@@ -9451,17 +9430,17 @@
         <v>1</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="J67" s="5"/>
       <c r="K67" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M67" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
@@ -9476,10 +9455,10 @@
       </c>
       <c r="S67" s="5"/>
       <c r="T67" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="U67" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="V67" s="5" t="s">
         <v>64</v>
@@ -9548,17 +9527,17 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B68" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="D68" s="19" t="s">
-        <v>364</v>
+        <v>356</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>365</v>
       </c>
       <c r="E68" s="4" t="str">
         <f aca="false">CONCATENATE(D68,"_vs_",C68)</f>
@@ -9572,17 +9551,17 @@
         <v>1</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="J68" s="5"/>
       <c r="K68" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L68" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M68" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
@@ -9597,10 +9576,10 @@
       </c>
       <c r="S68" s="5"/>
       <c r="T68" s="5" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="U68" s="5" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="V68" s="5" t="s">
         <v>64</v>
@@ -9669,17 +9648,17 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B69" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>368</v>
+        <v>356</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>369</v>
       </c>
       <c r="E69" s="4" t="str">
         <f aca="false">CONCATENATE(D69,"_vs_",C69)</f>
@@ -9693,17 +9672,17 @@
         <v>1</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L69" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M69" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
@@ -9718,10 +9697,10 @@
       </c>
       <c r="S69" s="5"/>
       <c r="T69" s="5" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="U69" s="5" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="V69" s="5" t="s">
         <v>64</v>
@@ -9790,17 +9769,17 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B70" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C70" s="19" t="s">
-        <v>372</v>
-      </c>
-      <c r="D70" s="19" t="s">
+      <c r="C70" s="12" t="s">
         <v>373</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>374</v>
       </c>
       <c r="E70" s="4" t="str">
         <f aca="false">CONCATENATE(D70,"_vs_",C70)</f>
@@ -9814,17 +9793,17 @@
         <v>4</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="J70" s="5"/>
       <c r="K70" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L70" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M70" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N70" s="5"/>
       <c r="O70" s="5"/>
@@ -9840,7 +9819,7 @@
       <c r="S70" s="5"/>
       <c r="T70" s="5"/>
       <c r="U70" s="5" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="V70" s="5" t="s">
         <v>64</v>
@@ -9909,7 +9888,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B71" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -9918,8 +9897,8 @@
       <c r="C71" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D71" s="19" t="s">
-        <v>377</v>
+      <c r="D71" s="12" t="s">
+        <v>378</v>
       </c>
       <c r="E71" s="4" t="str">
         <f aca="false">CONCATENATE(D71,"_vs_",C71)</f>
@@ -9933,17 +9912,17 @@
         <v>1</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="J71" s="5"/>
       <c r="K71" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L71" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M71" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N71" s="5"/>
       <c r="O71" s="5"/>
@@ -9959,7 +9938,7 @@
       <c r="S71" s="5"/>
       <c r="T71" s="5"/>
       <c r="U71" s="5" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="V71" s="5" t="s">
         <v>64</v>
@@ -10028,7 +10007,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B72" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -10037,8 +10016,8 @@
       <c r="C72" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D72" s="19" t="s">
-        <v>381</v>
+      <c r="D72" s="12" t="s">
+        <v>382</v>
       </c>
       <c r="E72" s="4" t="str">
         <f aca="false">CONCATENATE(D72,"_vs_",C72)</f>
@@ -10052,17 +10031,17 @@
         <v>1</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="J72" s="5"/>
       <c r="K72" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L72" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M72" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N72" s="5"/>
       <c r="O72" s="5"/>
@@ -10078,7 +10057,7 @@
       <c r="S72" s="5"/>
       <c r="T72" s="5"/>
       <c r="U72" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="V72" s="5" t="s">
         <v>64</v>
@@ -10147,7 +10126,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B73" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -10156,8 +10135,8 @@
       <c r="C73" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D73" s="19" t="s">
-        <v>385</v>
+      <c r="D73" s="12" t="s">
+        <v>386</v>
       </c>
       <c r="E73" s="4" t="str">
         <f aca="false">CONCATENATE(D73,"_vs_",C73)</f>
@@ -10171,17 +10150,17 @@
         <v>1</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="J73" s="5"/>
       <c r="K73" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L73" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M73" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N73" s="5"/>
       <c r="O73" s="5"/>
@@ -10197,7 +10176,7 @@
       <c r="S73" s="5"/>
       <c r="T73" s="5"/>
       <c r="U73" s="5" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="V73" s="5" t="s">
         <v>64</v>
@@ -10266,7 +10245,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B74" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -10275,8 +10254,8 @@
       <c r="C74" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D74" s="19" t="s">
-        <v>389</v>
+      <c r="D74" s="12" t="s">
+        <v>390</v>
       </c>
       <c r="E74" s="4" t="str">
         <f aca="false">CONCATENATE(D74,"_vs_",C74)</f>
@@ -10290,17 +10269,17 @@
         <v>1</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="J74" s="5"/>
       <c r="K74" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M74" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N74" s="5"/>
       <c r="O74" s="5"/>
@@ -10316,7 +10295,7 @@
       <c r="S74" s="5"/>
       <c r="T74" s="5"/>
       <c r="U74" s="5" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="V74" s="5" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
inverted log2FC values in 3 Zhang 2013 datasets
</commit_message>
<xml_diff>
--- a/data/column_descriptors_standardized.xlsx
+++ b/data/column_descriptors_standardized.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="396">
   <si>
     <t xml:space="preserve">column_ID</t>
   </si>
@@ -586,6 +586,9 @@
     <t xml:space="preserve">2017B_DeJesus_2C</t>
   </si>
   <si>
+    <t xml:space="preserve">2017B_DeJesus_GI_1A</t>
+  </si>
+  <si>
     <t xml:space="preserve">2017B_DeJesus_1A</t>
   </si>
   <si>
@@ -613,12 +616,15 @@
     <t xml:space="preserve">2017B_DeJesus_3C</t>
   </si>
   <si>
+    <t xml:space="preserve">Mutants exhibiting altered fitness in the absence of gene Rv1565c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017B_DeJesus_GI_1B</t>
+  </si>
+  <si>
     <t xml:space="preserve">2017B_DeJesus_1B</t>
   </si>
   <si>
-    <t xml:space="preserve">Mutants exhibiting altered fitness in the absence of gene Rv1565c</t>
-  </si>
-  <si>
     <t xml:space="preserve">2017B_DeJesus_4A</t>
   </si>
   <si>
@@ -641,6 +647,9 @@
   </si>
   <si>
     <t xml:space="preserve">2017B_DeJesus_4C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017B_DeJesus_GI_1C</t>
   </si>
   <si>
     <t xml:space="preserve">2017B_DeJesus_1C</t>
@@ -1329,7 +1338,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1384,6 +1393,14 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1467,14 +1484,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CA74"/>
+  <dimension ref="A1:CA77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
-      <selection pane="bottomRight" activeCell="D55" activeCellId="0" sqref="D55"/>
+      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4798,13 +4815,11 @@
       <c r="D29" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E29" s="10" t="str">
+      <c r="E29" s="14" t="str">
         <f aca="false">CONCATENATE(D29,"_vs_",C29)</f>
         <v>dejesus_Rv1432_day32_vs_dejesus_H37Rv_day32</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>188</v>
-      </c>
+      <c r="F29" s="15"/>
       <c r="G29" s="5" t="n">
         <v>3</v>
       </c>
@@ -4906,32 +4921,20 @@
       <c r="CA29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="B30" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="E30" s="4" t="str">
-        <f aca="false">CONCATENATE(D30,"_vs_",C30)</f>
-        <v>dejesus_Rv1565c_day0_vs_dejesus_H37Rv_day0</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H30" s="5" t="n">
-        <v>2</v>
-      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
       <c r="I30" s="4" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="J30" s="5" t="n">
         <v>2017</v>
@@ -4958,7 +4961,7 @@
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="5" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="U30" s="5"/>
       <c r="V30" s="5" t="s">
@@ -5025,32 +5028,32 @@
       <c r="CA30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>193</v>
+      <c r="A31" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="B31" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>190</v>
+      <c r="C31" s="12" t="s">
+        <v>174</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E31" s="4" t="str">
+        <v>191</v>
+      </c>
+      <c r="E31" s="14" t="str">
         <f aca="false">CONCATENATE(D31,"_vs_",C31)</f>
-        <v>dejesus_Rv1565c_day32_vs_dejesus_Rv1565c_day0</v>
-      </c>
-      <c r="F31" s="4"/>
+        <v>dejesus_Rv1565c_day0_vs_dejesus_H37Rv_day0</v>
+      </c>
+      <c r="F31" s="14"/>
       <c r="G31" s="5" t="n">
         <v>2</v>
       </c>
       <c r="H31" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J31" s="5" t="n">
         <v>2017</v>
@@ -5077,7 +5080,7 @@
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="U31" s="5"/>
       <c r="V31" s="5" t="s">
@@ -5144,34 +5147,32 @@
       <c r="CA31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>196</v>
+      <c r="A32" s="14" t="s">
+        <v>194</v>
       </c>
       <c r="B32" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>175</v>
+      <c r="C32" s="4" t="s">
+        <v>191</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E32" s="10" t="str">
+        <v>195</v>
+      </c>
+      <c r="E32" s="14" t="str">
         <f aca="false">CONCATENATE(D32,"_vs_",C32)</f>
-        <v>dejesus_Rv1565c_day32_vs_dejesus_H37Rv_day32</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>197</v>
-      </c>
+        <v>dejesus_Rv1565c_day32_vs_dejesus_Rv1565c_day0</v>
+      </c>
+      <c r="F32" s="14"/>
       <c r="G32" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H32" s="5" t="n">
         <v>3</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J32" s="5" t="n">
         <v>2017</v>
@@ -5198,7 +5199,7 @@
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
       <c r="T32" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="U32" s="5"/>
       <c r="V32" s="5" t="s">
@@ -5265,32 +5266,32 @@
       <c r="CA32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
-        <v>199</v>
+      <c r="A33" s="14" t="s">
+        <v>197</v>
       </c>
       <c r="B33" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E33" s="4" t="str">
+        <v>195</v>
+      </c>
+      <c r="E33" s="14" t="str">
         <f aca="false">CONCATENATE(D33,"_vs_",C33)</f>
-        <v>dejesus_Rv2680_day0_vs_dejesus_H37Rv_day0</v>
-      </c>
-      <c r="F33" s="4"/>
+        <v>dejesus_Rv1565c_day32_vs_dejesus_H37Rv_day32</v>
+      </c>
+      <c r="F33" s="15"/>
       <c r="G33" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H33" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J33" s="5" t="n">
         <v>2017</v>
@@ -5317,7 +5318,7 @@
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
       <c r="T33" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="U33" s="5"/>
       <c r="V33" s="5" t="s">
@@ -5384,32 +5385,20 @@
       <c r="CA33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="B34" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="A34" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E34" s="4" t="str">
-        <f aca="false">CONCATENATE(D34,"_vs_",C34)</f>
-        <v>dejesus_Rv2680_day32_vs_dejesus_Rv2680_day0</v>
-      </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H34" s="5" t="n">
-        <v>3</v>
-      </c>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
       <c r="I34" s="4" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="J34" s="5" t="n">
         <v>2017</v>
@@ -5436,7 +5425,7 @@
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
       <c r="T34" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="U34" s="5"/>
       <c r="V34" s="5" t="s">
@@ -5503,34 +5492,32 @@
       <c r="CA34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
-        <v>206</v>
+      <c r="A35" s="14" t="s">
+        <v>201</v>
       </c>
       <c r="B35" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E35" s="10" t="str">
+        <v>202</v>
+      </c>
+      <c r="E35" s="14" t="str">
         <f aca="false">CONCATENATE(D35,"_vs_",C35)</f>
-        <v>dejesus_Rv2680_day32_vs_dejesus_H37Rv_day32</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>207</v>
-      </c>
+        <v>dejesus_Rv2680_day0_vs_dejesus_H37Rv_day0</v>
+      </c>
+      <c r="F35" s="14"/>
       <c r="G35" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H35" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="J35" s="5" t="n">
         <v>2017</v>
@@ -5557,7 +5544,7 @@
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
       <c r="T35" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="U35" s="5"/>
       <c r="V35" s="5" t="s">
@@ -5624,71 +5611,67 @@
       <c r="CA35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
-        <v>208</v>
+      <c r="A36" s="14" t="s">
+        <v>205</v>
       </c>
       <c r="B36" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="E36" s="4" t="str">
+        <v>206</v>
+      </c>
+      <c r="E36" s="14" t="str">
         <f aca="false">CONCATENATE(D36,"_vs_",C36)</f>
-        <v>xu_van_16_vs_xu_van_0</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>211</v>
-      </c>
+        <v>dejesus_Rv2680_day32_vs_dejesus_Rv2680_day0</v>
+      </c>
+      <c r="F36" s="14"/>
       <c r="G36" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H36" s="5" t="n">
         <v>3</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J36" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>216</v>
+        <v>76</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>217</v>
+        <v>77</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q36" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="R36" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S36" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="T36" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="U36" s="5"/>
       <c r="V36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W36" s="5"/>
+      <c r="W36" s="5" t="s">
+        <v>179</v>
+      </c>
       <c r="X36" s="5"/>
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
@@ -5747,26 +5730,24 @@
       <c r="CA36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
-        <v>220</v>
+      <c r="A37" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="B37" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>221</v>
+      <c r="C37" s="12" t="s">
+        <v>175</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="E37" s="4" t="str">
+        <v>206</v>
+      </c>
+      <c r="E37" s="14" t="str">
         <f aca="false">CONCATENATE(D37,"_vs_",C37)</f>
-        <v>xu_rif_4_vs_xu_rif_0</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>223</v>
-      </c>
+        <v>dejesus_Rv2680_day32_vs_dejesus_H37Rv_day32</v>
+      </c>
+      <c r="F37" s="15"/>
       <c r="G37" s="5" t="n">
         <v>3</v>
       </c>
@@ -5774,44 +5755,42 @@
         <v>3</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="J37" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>216</v>
+        <v>76</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>217</v>
+        <v>77</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q37" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="R37" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S37" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="T37" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="U37" s="5"/>
       <c r="V37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W37" s="5"/>
+      <c r="W37" s="5" t="s">
+        <v>179</v>
+      </c>
       <c r="X37" s="5"/>
       <c r="Y37" s="5"/>
       <c r="Z37" s="5"/>
@@ -5870,71 +5849,55 @@
       <c r="CA37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="B38" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="E38" s="4" t="str">
-        <f aca="false">CONCATENATE(D38,"_vs_",C38)</f>
-        <v>xu_inh_02_vs_xu_inh_0</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="G38" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H38" s="5" t="n">
-        <v>3</v>
-      </c>
+      <c r="A38" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
       <c r="I38" s="4" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="J38" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>216</v>
+        <v>76</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>217</v>
+        <v>77</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q38" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="R38" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="S38" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="T38" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="U38" s="5"/>
       <c r="V38" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W38" s="5"/>
+      <c r="W38" s="5" t="s">
+        <v>179</v>
+      </c>
       <c r="X38" s="5"/>
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
@@ -5994,63 +5957,65 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="B39" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="E39" s="4" t="str">
         <f aca="false">CONCATENATE(D39,"_vs_",C39)</f>
-        <v>xu_inh_025_vs_xu_inh_0</v>
-      </c>
-      <c r="F39" s="10"/>
+        <v>xu_van_16_vs_xu_van_0</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>214</v>
+      </c>
       <c r="G39" s="5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H39" s="5" t="n">
         <v>3</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="J39" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="P39" s="5" t="s">
         <v>32</v>
       </c>
       <c r="Q39" s="5" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="R39" s="5" t="s">
         <v>34</v>
       </c>
       <c r="S39" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="T39" s="5"/>
+        <v>222</v>
+      </c>
+      <c r="T39" s="3"/>
       <c r="U39" s="5"/>
       <c r="V39" s="5" t="s">
         <v>64</v>
@@ -6115,24 +6080,24 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="B40" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E40" s="4" t="str">
         <f aca="false">CONCATENATE(D40,"_vs_",C40)</f>
-        <v>xu_emb_2.5_vs_xu_emb_0</v>
+        <v>xu_rif_4_vs_xu_rif_0</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="G40" s="5" t="n">
         <v>3</v>
@@ -6141,37 +6106,37 @@
         <v>3</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="J40" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="P40" s="5" t="s">
         <v>32</v>
       </c>
       <c r="Q40" s="5" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="R40" s="5" t="s">
         <v>34</v>
       </c>
       <c r="S40" s="5" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="T40" s="5"/>
       <c r="U40" s="5"/>
@@ -6238,61 +6203,63 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="B41" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="E41" s="4" t="str">
         <f aca="false">CONCATENATE(D41,"_vs_",C41)</f>
-        <v>xu_emb_3_vs_xu_emb_0</v>
-      </c>
-      <c r="F41" s="10"/>
+        <v>xu_inh_02_vs_xu_inh_0</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>232</v>
+      </c>
       <c r="G41" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H41" s="5" t="n">
         <v>3</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="J41" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="P41" s="5" t="s">
         <v>32</v>
       </c>
       <c r="Q41" s="5" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="R41" s="5" t="s">
         <v>34</v>
       </c>
       <c r="S41" s="5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="T41" s="5"/>
       <c r="U41" s="5"/>
@@ -6359,63 +6326,61 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B42" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E42" s="4" t="str">
         <f aca="false">CONCATENATE(D42,"_vs_",C42)</f>
-        <v>xu_mero_2.5_vs_xu_mero_0</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>242</v>
-      </c>
+        <v>xu_inh_025_vs_xu_inh_0</v>
+      </c>
+      <c r="F42" s="10"/>
       <c r="G42" s="5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H42" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="J42" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="N42" s="5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="O42" s="5" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="P42" s="5" t="s">
         <v>32</v>
       </c>
       <c r="Q42" s="5" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="R42" s="5" t="s">
         <v>34</v>
       </c>
       <c r="S42" s="5" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="T42" s="5"/>
       <c r="U42" s="5"/>
@@ -6480,71 +6445,75 @@
       <c r="BZ42" s="5"/>
       <c r="CA42" s="5"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B43" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>249</v>
+      <c r="C43" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>239</v>
       </c>
       <c r="E43" s="4" t="str">
         <f aca="false">CONCATENATE(D43,"_vs_",C43)</f>
-        <v>mishra_C3H_vs_mishra_B6</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>247</v>
+        <v>xu_emb_2.5_vs_xu_emb_0</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>240</v>
       </c>
       <c r="G43" s="5" t="n">
         <v>3</v>
       </c>
       <c r="H43" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I43" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="J43" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
       <c r="O43" s="5" t="s">
-        <v>30</v>
+        <v>220</v>
       </c>
       <c r="P43" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="Q43" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="R43" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S43" s="5" t="s">
+        <v>242</v>
+      </c>
       <c r="T43" s="5"/>
       <c r="U43" s="5"/>
       <c r="V43" s="5" t="s">
         <v>64</v>
       </c>
       <c r="W43" s="5"/>
-      <c r="X43" s="5" t="s">
-        <v>254</v>
-      </c>
+      <c r="X43" s="5"/>
       <c r="Y43" s="5"/>
-      <c r="Z43" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="Z43" s="5"/>
       <c r="AA43" s="3"/>
       <c r="AB43" s="5"/>
       <c r="AC43" s="5"/>
@@ -6599,71 +6568,73 @@
       <c r="BZ43" s="5"/>
       <c r="CA43" s="5"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B44" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>256</v>
+      <c r="C44" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>244</v>
       </c>
       <c r="E44" s="4" t="str">
         <f aca="false">CONCATENATE(D44,"_vs_",C44)</f>
-        <v>mishra_NOS2_vs_mishra_B6</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>255</v>
-      </c>
+        <v>xu_emb_3_vs_xu_emb_0</v>
+      </c>
+      <c r="F44" s="10"/>
       <c r="G44" s="5" t="n">
         <v>3</v>
       </c>
       <c r="H44" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I44" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="J44" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="N44" s="5" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>30</v>
+        <v>220</v>
       </c>
       <c r="P44" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="Q44" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="R44" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S44" s="5" t="s">
+        <v>242</v>
+      </c>
       <c r="T44" s="5"/>
       <c r="U44" s="5"/>
       <c r="V44" s="5" t="s">
         <v>64</v>
       </c>
       <c r="W44" s="5"/>
-      <c r="X44" s="5" t="s">
-        <v>257</v>
-      </c>
+      <c r="X44" s="5"/>
       <c r="Y44" s="5"/>
-      <c r="Z44" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="Z44" s="5"/>
       <c r="AA44" s="3"/>
       <c r="AB44" s="5"/>
       <c r="AC44" s="5"/>
@@ -6718,180 +6689,180 @@
       <c r="BZ44" s="5"/>
       <c r="CA44" s="5"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B45" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>256</v>
+      <c r="C45" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="E45" s="4" t="str">
         <f aca="false">CONCATENATE(D45,"_vs_",C45)</f>
-        <v>mishra_NOS2_vs_mishra_C3H</v>
-      </c>
-      <c r="F45" s="4"/>
+        <v>xu_mero_2.5_vs_xu_mero_0</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>245</v>
+      </c>
       <c r="G45" s="5" t="n">
         <v>2</v>
       </c>
       <c r="H45" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I45" s="4"/>
+      <c r="I45" s="4" t="s">
+        <v>248</v>
+      </c>
       <c r="J45" s="5" t="n">
         <v>2017</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>30</v>
+        <v>220</v>
       </c>
       <c r="P45" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="Q45" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="R45" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S45" s="5" t="s">
+        <v>249</v>
+      </c>
       <c r="T45" s="5"/>
       <c r="U45" s="5"/>
       <c r="V45" s="5" t="s">
         <v>64</v>
       </c>
       <c r="W45" s="5"/>
-      <c r="X45" s="5" t="s">
-        <v>259</v>
-      </c>
+      <c r="X45" s="5"/>
       <c r="Y45" s="5"/>
-      <c r="Z45" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="Z45" s="5"/>
       <c r="AA45" s="3"/>
-      <c r="AB45" s="3"/>
-      <c r="AC45" s="3"/>
-      <c r="AD45" s="3"/>
-      <c r="AE45" s="3"/>
-      <c r="AF45" s="3"/>
-      <c r="AG45" s="3"/>
-      <c r="AH45" s="3"/>
-      <c r="AI45" s="3"/>
-      <c r="AJ45" s="3"/>
-      <c r="AK45" s="3"/>
-      <c r="AL45" s="3"/>
-      <c r="AM45" s="3"/>
-      <c r="AN45" s="3"/>
-      <c r="AO45" s="3"/>
-      <c r="AP45" s="3"/>
-      <c r="AQ45" s="3"/>
-      <c r="AR45" s="3"/>
-      <c r="AS45" s="3"/>
-      <c r="AT45" s="3"/>
-      <c r="AU45" s="3"/>
-      <c r="AV45" s="3"/>
-      <c r="AW45" s="3"/>
-      <c r="AX45" s="3"/>
-      <c r="AY45" s="3"/>
-      <c r="AZ45" s="3"/>
-      <c r="BA45" s="3"/>
-      <c r="BB45" s="3"/>
-      <c r="BC45" s="3"/>
-      <c r="BD45" s="3"/>
-      <c r="BE45" s="3"/>
-      <c r="BF45" s="3"/>
-      <c r="BG45" s="3"/>
-      <c r="BH45" s="3"/>
-      <c r="BI45" s="3"/>
-      <c r="BJ45" s="3"/>
-      <c r="BK45" s="3"/>
-      <c r="BL45" s="3"/>
-      <c r="BM45" s="3"/>
-      <c r="BN45" s="3"/>
-      <c r="BO45" s="3"/>
-      <c r="BP45" s="3"/>
-      <c r="BQ45" s="3"/>
-      <c r="BR45" s="3"/>
-      <c r="BS45" s="3"/>
-      <c r="BT45" s="3"/>
-      <c r="BU45" s="3"/>
-      <c r="BV45" s="3"/>
-      <c r="BW45" s="3"/>
-      <c r="BX45" s="3"/>
-      <c r="BY45" s="3"/>
-      <c r="BZ45" s="3"/>
-      <c r="CA45" s="3"/>
+      <c r="AB45" s="5"/>
+      <c r="AC45" s="5"/>
+      <c r="AD45" s="5"/>
+      <c r="AE45" s="5"/>
+      <c r="AF45" s="5"/>
+      <c r="AG45" s="5"/>
+      <c r="AH45" s="5"/>
+      <c r="AI45" s="5"/>
+      <c r="AJ45" s="5"/>
+      <c r="AK45" s="5"/>
+      <c r="AL45" s="5"/>
+      <c r="AM45" s="5"/>
+      <c r="AN45" s="5"/>
+      <c r="AO45" s="5"/>
+      <c r="AP45" s="5"/>
+      <c r="AQ45" s="5"/>
+      <c r="AR45" s="5"/>
+      <c r="AS45" s="5"/>
+      <c r="AT45" s="5"/>
+      <c r="AU45" s="5"/>
+      <c r="AV45" s="5"/>
+      <c r="AW45" s="5"/>
+      <c r="AX45" s="5"/>
+      <c r="AY45" s="5"/>
+      <c r="AZ45" s="5"/>
+      <c r="BA45" s="5"/>
+      <c r="BB45" s="5"/>
+      <c r="BC45" s="5"/>
+      <c r="BD45" s="5"/>
+      <c r="BE45" s="5"/>
+      <c r="BF45" s="5"/>
+      <c r="BG45" s="5"/>
+      <c r="BH45" s="5"/>
+      <c r="BI45" s="5"/>
+      <c r="BJ45" s="5"/>
+      <c r="BK45" s="5"/>
+      <c r="BL45" s="5"/>
+      <c r="BM45" s="5"/>
+      <c r="BN45" s="5"/>
+      <c r="BO45" s="5"/>
+      <c r="BP45" s="5"/>
+      <c r="BQ45" s="5"/>
+      <c r="BR45" s="5"/>
+      <c r="BS45" s="5"/>
+      <c r="BT45" s="5"/>
+      <c r="BU45" s="5"/>
+      <c r="BV45" s="5"/>
+      <c r="BW45" s="5"/>
+      <c r="BX45" s="5"/>
+      <c r="BY45" s="5"/>
+      <c r="BZ45" s="5"/>
+      <c r="CA45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B46" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>262</v>
+      <c r="C46" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>252</v>
       </c>
       <c r="E46" s="4" t="str">
         <f aca="false">CONCATENATE(D46,"_vs_",C46)</f>
-        <v>carey_621_vs_carey_rv</v>
+        <v>mishra_C3H_vs_mishra_B6</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="G46" s="5" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="H46" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I46" s="4" t="s">
-        <v>263</v>
-      </c>
+      <c r="I46" s="4"/>
       <c r="J46" s="5" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>268</v>
+        <v>30</v>
       </c>
       <c r="P46" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q46" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="R46" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
       <c r="U46" s="5"/>
@@ -6899,10 +6870,12 @@
         <v>64</v>
       </c>
       <c r="W46" s="5"/>
-      <c r="X46" s="5"/>
+      <c r="X46" s="5" t="s">
+        <v>257</v>
+      </c>
       <c r="Y46" s="5"/>
-      <c r="Z46" s="5" t="n">
-        <v>621</v>
+      <c r="Z46" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="AA46" s="3"/>
       <c r="AB46" s="5"/>
@@ -6960,61 +6933,55 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B47" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>270</v>
+      <c r="C47" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>259</v>
       </c>
       <c r="E47" s="4" t="str">
         <f aca="false">CONCATENATE(D47,"_vs_",C47)</f>
-        <v>carey_630_vs_carey_rv</v>
+        <v>mishra_NOS2_vs_mishra_B6</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="G47" s="5" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="H47" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I47" s="4" t="s">
-        <v>271</v>
-      </c>
+      <c r="I47" s="4"/>
       <c r="J47" s="5" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>268</v>
+        <v>30</v>
       </c>
       <c r="P47" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q47" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="R47" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
       <c r="U47" s="5"/>
@@ -7022,10 +6989,12 @@
         <v>64</v>
       </c>
       <c r="W47" s="5"/>
-      <c r="X47" s="5"/>
+      <c r="X47" s="5" t="s">
+        <v>260</v>
+      </c>
       <c r="Y47" s="5"/>
-      <c r="Z47" s="5" t="n">
-        <v>630</v>
+      <c r="Z47" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="AA47" s="3"/>
       <c r="AB47" s="5"/>
@@ -7083,61 +7052,53 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B48" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>273</v>
+      <c r="C48" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>259</v>
       </c>
       <c r="E48" s="4" t="str">
         <f aca="false">CONCATENATE(D48,"_vs_",C48)</f>
-        <v>carey_631_vs_carey_rv</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>272</v>
-      </c>
+        <v>mishra_NOS2_vs_mishra_C3H</v>
+      </c>
+      <c r="F48" s="4"/>
       <c r="G48" s="5" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H48" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I48" s="4" t="s">
-        <v>274</v>
-      </c>
+      <c r="I48" s="4"/>
       <c r="J48" s="5" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>268</v>
+        <v>30</v>
       </c>
       <c r="P48" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q48" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="R48" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
       <c r="S48" s="5"/>
       <c r="T48" s="5"/>
       <c r="U48" s="5"/>
@@ -7145,85 +7106,87 @@
         <v>64</v>
       </c>
       <c r="W48" s="5"/>
-      <c r="X48" s="5"/>
+      <c r="X48" s="5" t="s">
+        <v>262</v>
+      </c>
       <c r="Y48" s="5"/>
-      <c r="Z48" s="5" t="n">
-        <v>631</v>
+      <c r="Z48" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="AA48" s="3"/>
-      <c r="AB48" s="5"/>
-      <c r="AC48" s="5"/>
-      <c r="AD48" s="5"/>
-      <c r="AE48" s="5"/>
-      <c r="AF48" s="5"/>
-      <c r="AG48" s="5"/>
-      <c r="AH48" s="5"/>
-      <c r="AI48" s="5"/>
-      <c r="AJ48" s="5"/>
-      <c r="AK48" s="5"/>
-      <c r="AL48" s="5"/>
-      <c r="AM48" s="5"/>
-      <c r="AN48" s="5"/>
-      <c r="AO48" s="5"/>
-      <c r="AP48" s="5"/>
-      <c r="AQ48" s="5"/>
-      <c r="AR48" s="5"/>
-      <c r="AS48" s="5"/>
-      <c r="AT48" s="5"/>
-      <c r="AU48" s="5"/>
-      <c r="AV48" s="5"/>
-      <c r="AW48" s="5"/>
-      <c r="AX48" s="5"/>
-      <c r="AY48" s="5"/>
-      <c r="AZ48" s="5"/>
-      <c r="BA48" s="5"/>
-      <c r="BB48" s="5"/>
-      <c r="BC48" s="5"/>
-      <c r="BD48" s="5"/>
-      <c r="BE48" s="5"/>
-      <c r="BF48" s="5"/>
-      <c r="BG48" s="5"/>
-      <c r="BH48" s="5"/>
-      <c r="BI48" s="5"/>
-      <c r="BJ48" s="5"/>
-      <c r="BK48" s="5"/>
-      <c r="BL48" s="5"/>
-      <c r="BM48" s="5"/>
-      <c r="BN48" s="5"/>
-      <c r="BO48" s="5"/>
-      <c r="BP48" s="5"/>
-      <c r="BQ48" s="5"/>
-      <c r="BR48" s="5"/>
-      <c r="BS48" s="5"/>
-      <c r="BT48" s="5"/>
-      <c r="BU48" s="5"/>
-      <c r="BV48" s="5"/>
-      <c r="BW48" s="5"/>
-      <c r="BX48" s="5"/>
-      <c r="BY48" s="5"/>
-      <c r="BZ48" s="5"/>
-      <c r="CA48" s="5"/>
+      <c r="AB48" s="3"/>
+      <c r="AC48" s="3"/>
+      <c r="AD48" s="3"/>
+      <c r="AE48" s="3"/>
+      <c r="AF48" s="3"/>
+      <c r="AG48" s="3"/>
+      <c r="AH48" s="3"/>
+      <c r="AI48" s="3"/>
+      <c r="AJ48" s="3"/>
+      <c r="AK48" s="3"/>
+      <c r="AL48" s="3"/>
+      <c r="AM48" s="3"/>
+      <c r="AN48" s="3"/>
+      <c r="AO48" s="3"/>
+      <c r="AP48" s="3"/>
+      <c r="AQ48" s="3"/>
+      <c r="AR48" s="3"/>
+      <c r="AS48" s="3"/>
+      <c r="AT48" s="3"/>
+      <c r="AU48" s="3"/>
+      <c r="AV48" s="3"/>
+      <c r="AW48" s="3"/>
+      <c r="AX48" s="3"/>
+      <c r="AY48" s="3"/>
+      <c r="AZ48" s="3"/>
+      <c r="BA48" s="3"/>
+      <c r="BB48" s="3"/>
+      <c r="BC48" s="3"/>
+      <c r="BD48" s="3"/>
+      <c r="BE48" s="3"/>
+      <c r="BF48" s="3"/>
+      <c r="BG48" s="3"/>
+      <c r="BH48" s="3"/>
+      <c r="BI48" s="3"/>
+      <c r="BJ48" s="3"/>
+      <c r="BK48" s="3"/>
+      <c r="BL48" s="3"/>
+      <c r="BM48" s="3"/>
+      <c r="BN48" s="3"/>
+      <c r="BO48" s="3"/>
+      <c r="BP48" s="3"/>
+      <c r="BQ48" s="3"/>
+      <c r="BR48" s="3"/>
+      <c r="BS48" s="3"/>
+      <c r="BT48" s="3"/>
+      <c r="BU48" s="3"/>
+      <c r="BV48" s="3"/>
+      <c r="BW48" s="3"/>
+      <c r="BX48" s="3"/>
+      <c r="BY48" s="3"/>
+      <c r="BZ48" s="3"/>
+      <c r="CA48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="B49" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="E49" s="4" t="str">
         <f aca="false">CONCATENATE(D49,"_vs_",C49)</f>
-        <v>carey_632_vs_carey_rv</v>
+        <v>carey_621_vs_carey_rv</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="G49" s="5" t="n">
         <v>14</v>
@@ -7232,25 +7195,25 @@
         <v>2</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="J49" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="P49" s="5" t="s">
         <v>32</v>
@@ -7271,7 +7234,7 @@
       <c r="X49" s="5"/>
       <c r="Y49" s="5"/>
       <c r="Z49" s="5" t="n">
-        <v>632</v>
+        <v>621</v>
       </c>
       <c r="AA49" s="3"/>
       <c r="AB49" s="5"/>
@@ -7329,24 +7292,24 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B50" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="E50" s="4" t="str">
         <f aca="false">CONCATENATE(D50,"_vs_",C50)</f>
-        <v>carey_641_vs_carey_rv</v>
+        <v>carey_630_vs_carey_rv</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="G50" s="5" t="n">
         <v>14</v>
@@ -7355,25 +7318,25 @@
         <v>2</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="J50" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="P50" s="5" t="s">
         <v>32</v>
@@ -7394,7 +7357,7 @@
       <c r="X50" s="5"/>
       <c r="Y50" s="5"/>
       <c r="Z50" s="5" t="n">
-        <v>641</v>
+        <v>630</v>
       </c>
       <c r="AA50" s="3"/>
       <c r="AB50" s="5"/>
@@ -7452,24 +7415,24 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B51" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="E51" s="4" t="str">
         <f aca="false">CONCATENATE(D51,"_vs_",C51)</f>
-        <v>carey_662_vs_carey_rv</v>
+        <v>carey_631_vs_carey_rv</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="G51" s="5" t="n">
         <v>14</v>
@@ -7478,25 +7441,25 @@
         <v>2</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="J51" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="P51" s="5" t="s">
         <v>32</v>
@@ -7517,7 +7480,7 @@
       <c r="X51" s="5"/>
       <c r="Y51" s="5"/>
       <c r="Z51" s="5" t="n">
-        <v>662</v>
+        <v>631</v>
       </c>
       <c r="AA51" s="3"/>
       <c r="AB51" s="5"/>
@@ -7575,24 +7538,24 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B52" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E52" s="4" t="str">
         <f aca="false">CONCATENATE(D52,"_vs_",C52)</f>
-        <v>carey_663_vs_carey_rv</v>
+        <v>carey_632_vs_carey_rv</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="G52" s="5" t="n">
         <v>14</v>
@@ -7601,25 +7564,25 @@
         <v>2</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="J52" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="P52" s="5" t="s">
         <v>32</v>
@@ -7640,7 +7603,7 @@
       <c r="X52" s="5"/>
       <c r="Y52" s="5"/>
       <c r="Z52" s="5" t="n">
-        <v>663</v>
+        <v>632</v>
       </c>
       <c r="AA52" s="3"/>
       <c r="AB52" s="5"/>
@@ -7698,24 +7661,24 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B53" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E53" s="4" t="str">
         <f aca="false">CONCATENATE(D53,"_vs_",C53)</f>
-        <v>carey_667_vs_carey_rv</v>
+        <v>carey_641_vs_carey_rv</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="G53" s="5" t="n">
         <v>14</v>
@@ -7724,25 +7687,25 @@
         <v>2</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="J53" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="P53" s="5" t="s">
         <v>32</v>
@@ -7763,7 +7726,7 @@
       <c r="X53" s="5"/>
       <c r="Y53" s="5"/>
       <c r="Z53" s="5" t="n">
-        <v>667</v>
+        <v>641</v>
       </c>
       <c r="AA53" s="3"/>
       <c r="AB53" s="5"/>
@@ -7821,76 +7784,72 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B54" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>291</v>
+        <v>264</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="E54" s="4" t="str">
         <f aca="false">CONCATENATE(D54,"_vs_",C54)</f>
-        <v>ritterhaus_hypoxia_H3_vs_ritterhaus_hypoxia_input</v>
+        <v>carey_662_vs_carey_rv</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="G54" s="5" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H54" s="5" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="J54" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>298</v>
+        <v>270</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>30</v>
+        <v>271</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>32</v>
       </c>
       <c r="Q54" s="5" t="s">
-        <v>218</v>
+        <v>33</v>
       </c>
       <c r="R54" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S54" s="5" t="s">
-        <v>299</v>
-      </c>
+      <c r="S54" s="5"/>
       <c r="T54" s="5"/>
       <c r="U54" s="5"/>
       <c r="V54" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W54" s="5" t="s">
-        <v>179</v>
-      </c>
+      <c r="W54" s="5"/>
       <c r="X54" s="5"/>
       <c r="Y54" s="5"/>
-      <c r="Z54" s="5" t="s">
-        <v>65</v>
+      <c r="Z54" s="5" t="n">
+        <v>662</v>
       </c>
       <c r="AA54" s="3"/>
       <c r="AB54" s="5"/>
@@ -7948,76 +7907,72 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="B55" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>291</v>
+        <v>264</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="E55" s="4" t="str">
         <f aca="false">CONCATENATE(D55,"_vs_",C55)</f>
-        <v>ritterhaus_hypoxia_H6_vs_ritterhaus_hypoxia_input</v>
+        <v>carey_663_vs_carey_rv</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="G55" s="5" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H55" s="5" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="J55" s="5" t="n">
         <v>2018</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>298</v>
+        <v>270</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>30</v>
+        <v>271</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>32</v>
       </c>
       <c r="Q55" s="5" t="s">
-        <v>218</v>
+        <v>33</v>
       </c>
       <c r="R55" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S55" s="5" t="s">
-        <v>304</v>
-      </c>
+      <c r="S55" s="5"/>
       <c r="T55" s="5"/>
       <c r="U55" s="5"/>
       <c r="V55" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W55" s="5" t="s">
-        <v>179</v>
-      </c>
+      <c r="W55" s="5"/>
       <c r="X55" s="5"/>
       <c r="Y55" s="5"/>
-      <c r="Z55" s="5" t="s">
-        <v>65</v>
+      <c r="Z55" s="5" t="n">
+        <v>663</v>
       </c>
       <c r="AA55" s="3"/>
       <c r="AB55" s="5"/>
@@ -8075,68 +8030,72 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="B56" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>306</v>
+        <v>264</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="E56" s="4" t="str">
         <f aca="false">CONCATENATE(D56,"_vs_",C56)</f>
-        <v>bellerose_MB_d21_untreated_vs_bellerose_MB_pretreatment</v>
-      </c>
-      <c r="F56" s="4"/>
+        <v>carey_667_vs_carey_rv</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>290</v>
+      </c>
       <c r="G56" s="5" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H56" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I56" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>292</v>
+      </c>
       <c r="J56" s="5" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="L56" s="14" t="s">
-        <v>309</v>
+        <v>267</v>
+      </c>
+      <c r="L56" s="8" t="s">
+        <v>268</v>
       </c>
       <c r="M56" s="5" t="s">
-        <v>310</v>
+        <v>269</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>311</v>
+        <v>270</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>30</v>
+        <v>271</v>
       </c>
       <c r="P56" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q56" s="5"/>
-      <c r="R56" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="Q56" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R56" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="S56" s="5"/>
       <c r="T56" s="5"/>
       <c r="U56" s="5"/>
       <c r="V56" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W56" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="X56" s="5" t="s">
-        <v>312</v>
-      </c>
+      <c r="W56" s="5"/>
+      <c r="X56" s="5"/>
       <c r="Y56" s="5"/>
-      <c r="Z56" s="5" t="s">
-        <v>65</v>
+      <c r="Z56" s="5" t="n">
+        <v>667</v>
       </c>
       <c r="AA56" s="3"/>
       <c r="AB56" s="5"/>
@@ -8194,54 +8153,64 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="B57" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="E57" s="4" t="str">
         <f aca="false">CONCATENATE(D57,"_vs_",C57)</f>
-        <v>bellerose_MB_HRZE_wk1_vs_bellerose_MB_pretreatment</v>
-      </c>
-      <c r="F57" s="4"/>
+        <v>ritterhaus_hypoxia_H3_vs_ritterhaus_hypoxia_input</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>296</v>
+      </c>
       <c r="G57" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H57" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I57" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>297</v>
+      </c>
       <c r="J57" s="5" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="L57" s="14" t="s">
-        <v>309</v>
+        <v>298</v>
+      </c>
+      <c r="L57" s="8" t="s">
+        <v>299</v>
       </c>
       <c r="M57" s="5" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="O57" s="5" t="s">
         <v>30</v>
       </c>
       <c r="P57" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q57" s="5"/>
-      <c r="R57" s="5"/>
-      <c r="S57" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="Q57" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="R57" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S57" s="5" t="s">
+        <v>302</v>
+      </c>
       <c r="T57" s="5"/>
       <c r="U57" s="5"/>
       <c r="V57" s="5" t="s">
@@ -8250,9 +8219,7 @@
       <c r="W57" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X57" s="5" t="s">
-        <v>312</v>
-      </c>
+      <c r="X57" s="5"/>
       <c r="Y57" s="5"/>
       <c r="Z57" s="5" t="s">
         <v>65</v>
@@ -8313,54 +8280,64 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="B58" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E58" s="4" t="str">
         <f aca="false">CONCATENATE(D58,"_vs_",C58)</f>
-        <v>bellerose_MB_HRZE_wk1_vs_bellerose_MB_d21_untreated</v>
-      </c>
-      <c r="F58" s="4"/>
+        <v>ritterhaus_hypoxia_H6_vs_ritterhaus_hypoxia_input</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>305</v>
+      </c>
       <c r="G58" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H58" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I58" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>306</v>
+      </c>
       <c r="J58" s="5" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="L58" s="14" t="s">
-        <v>309</v>
+        <v>298</v>
+      </c>
+      <c r="L58" s="8" t="s">
+        <v>299</v>
       </c>
       <c r="M58" s="5" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="O58" s="5" t="s">
         <v>30</v>
       </c>
       <c r="P58" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q58" s="5"/>
-      <c r="R58" s="5"/>
-      <c r="S58" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="Q58" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="R58" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S58" s="5" t="s">
+        <v>307</v>
+      </c>
       <c r="T58" s="5"/>
       <c r="U58" s="5"/>
       <c r="V58" s="5" t="s">
@@ -8369,9 +8346,7 @@
       <c r="W58" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X58" s="5" t="s">
-        <v>312</v>
-      </c>
+      <c r="X58" s="5"/>
       <c r="Y58" s="5"/>
       <c r="Z58" s="5" t="s">
         <v>65</v>
@@ -8432,57 +8407,53 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B59" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="E59" s="4" t="str">
         <f aca="false">CONCATENATE(D59,"_vs_",C59)</f>
-        <v>minato_minimal_plate_vs_minato_rich_plate</v>
+        <v>bellerose_MB_d21_untreated_vs_bellerose_MB_pretreatment</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H59" s="5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I59" s="4"/>
       <c r="J59" s="5" t="n">
         <v>2019</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="L59" s="14" t="s">
-        <v>320</v>
+        <v>311</v>
+      </c>
+      <c r="L59" s="16" t="s">
+        <v>312</v>
       </c>
       <c r="M59" s="5" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="O59" s="5" t="s">
-        <v>323</v>
+        <v>30</v>
       </c>
       <c r="P59" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q59" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="R59" s="5" t="s">
-        <v>325</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
       <c r="S59" s="5"/>
       <c r="T59" s="5"/>
       <c r="U59" s="5"/>
@@ -8492,9 +8463,13 @@
       <c r="W59" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X59" s="5"/>
+      <c r="X59" s="5" t="s">
+        <v>315</v>
+      </c>
       <c r="Y59" s="5"/>
-      <c r="Z59" s="5"/>
+      <c r="Z59" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="AA59" s="3"/>
       <c r="AB59" s="5"/>
       <c r="AC59" s="5"/>
@@ -8551,63 +8526,55 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="B60" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="E60" s="4" t="str">
         <f aca="false">CONCATENATE(D60,"_vs_",C60)</f>
-        <v>dejesus_Rv0307c_day32_vs_dejesus_Rv0307c_day0</v>
+        <v>bellerose_MB_HRZE_wk1_vs_bellerose_MB_pretreatment</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H60" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="J60" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="K60" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="L60" s="5" t="s">
-        <v>330</v>
+        <v>5</v>
+      </c>
+      <c r="I60" s="4"/>
+      <c r="J60" s="5" t="n">
+        <v>2019</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="L60" s="16" t="s">
+        <v>312</v>
       </c>
       <c r="M60" s="5" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="N60" s="5" t="s">
-        <v>76</v>
+        <v>314</v>
       </c>
       <c r="O60" s="5" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="P60" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q60" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="R60" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="5"/>
       <c r="S60" s="5"/>
-      <c r="T60" s="5" t="s">
-        <v>331</v>
-      </c>
+      <c r="T60" s="5"/>
       <c r="U60" s="5"/>
       <c r="V60" s="5" t="s">
         <v>64</v>
@@ -8615,7 +8582,9 @@
       <c r="W60" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X60" s="5"/>
+      <c r="X60" s="5" t="s">
+        <v>315</v>
+      </c>
       <c r="Y60" s="5"/>
       <c r="Z60" s="5" t="s">
         <v>65</v>
@@ -8676,63 +8645,55 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="B61" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>333</v>
+        <v>310</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="E61" s="4" t="str">
         <f aca="false">CONCATENATE(D61,"_vs_",C61)</f>
-        <v>dejesus_Rv3916c_day32_vs_dejesus_Rv3916c_day0</v>
+        <v>bellerose_MB_HRZE_wk1_vs_bellerose_MB_d21_untreated</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H61" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="J61" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="K61" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="L61" s="5" t="s">
-        <v>330</v>
+        <v>5</v>
+      </c>
+      <c r="I61" s="4"/>
+      <c r="J61" s="5" t="n">
+        <v>2019</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="L61" s="16" t="s">
+        <v>312</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="N61" s="5" t="s">
-        <v>76</v>
+        <v>314</v>
       </c>
       <c r="O61" s="5" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="P61" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q61" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="R61" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
       <c r="S61" s="5"/>
-      <c r="T61" s="5" t="s">
-        <v>336</v>
-      </c>
+      <c r="T61" s="5"/>
       <c r="U61" s="5"/>
       <c r="V61" s="5" t="s">
         <v>64</v>
@@ -8740,7 +8701,9 @@
       <c r="W61" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="X61" s="5"/>
+      <c r="X61" s="5" t="s">
+        <v>315</v>
+      </c>
       <c r="Y61" s="5"/>
       <c r="Z61" s="5" t="s">
         <v>65</v>
@@ -8801,60 +8764,60 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="B62" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>339</v>
+        <v>320</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>321</v>
       </c>
       <c r="E62" s="4" t="str">
         <f aca="false">CONCATENATE(D62,"_vs_",C62)</f>
-        <v>Rv0950c_KO_vs_CB_WT</v>
+        <v>minato_minimal_plate_vs_minato_rich_plate</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H62" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="L62" s="5" t="s">
-        <v>330</v>
+        <v>2</v>
+      </c>
+      <c r="I62" s="4"/>
+      <c r="J62" s="5" t="n">
+        <v>2019</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="L62" s="16" t="s">
+        <v>323</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="N62" s="5"/>
-      <c r="O62" s="5"/>
+        <v>324</v>
+      </c>
+      <c r="N62" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="O62" s="5" t="s">
+        <v>326</v>
+      </c>
       <c r="P62" s="5" t="s">
         <v>32</v>
       </c>
       <c r="Q62" s="5" t="s">
-        <v>33</v>
+        <v>327</v>
       </c>
       <c r="R62" s="5" t="s">
-        <v>34</v>
+        <v>328</v>
       </c>
       <c r="S62" s="5"/>
-      <c r="T62" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="U62" s="5" t="s">
-        <v>341</v>
-      </c>
+      <c r="T62" s="5"/>
+      <c r="U62" s="5"/>
       <c r="V62" s="5" t="s">
         <v>64</v>
       </c>
@@ -8863,9 +8826,7 @@
       </c>
       <c r="X62" s="5"/>
       <c r="Y62" s="5"/>
-      <c r="Z62" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="Z62" s="5"/>
       <c r="AA62" s="3"/>
       <c r="AB62" s="5"/>
       <c r="AC62" s="5"/>
@@ -8922,44 +8883,50 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="B63" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>344</v>
+        <v>330</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>331</v>
       </c>
       <c r="E63" s="4" t="str">
         <f aca="false">CONCATENATE(D63,"_vs_",C63)</f>
-        <v>Rv0954_KO_vs_RJ_WT</v>
+        <v>dejesus_Rv0307c_day32_vs_dejesus_Rv0307c_day0</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="5" t="n">
         <v>2</v>
       </c>
       <c r="H63" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="J63" s="5"/>
+        <v>332</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>333</v>
+      </c>
       <c r="K63" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="N63" s="5"/>
-      <c r="O63" s="5"/>
+        <v>333</v>
+      </c>
+      <c r="N63" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O63" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="P63" s="5" t="s">
         <v>32</v>
       </c>
@@ -8971,11 +8938,9 @@
       </c>
       <c r="S63" s="5"/>
       <c r="T63" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="U63" s="5" t="s">
-        <v>346</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="U63" s="5"/>
       <c r="V63" s="5" t="s">
         <v>64</v>
       </c>
@@ -9043,44 +9008,50 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="B64" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>348</v>
+        <v>336</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>337</v>
       </c>
       <c r="E64" s="4" t="str">
         <f aca="false">CONCATENATE(D64,"_vs_",C64)</f>
-        <v>Rv1096_KO_vs_CB_WT</v>
+        <v>dejesus_Rv3916c_day32_vs_dejesus_Rv3916c_day0</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H64" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="J64" s="5"/>
+        <v>338</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>333</v>
+      </c>
       <c r="K64" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L64" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M64" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5"/>
+        <v>333</v>
+      </c>
+      <c r="N64" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O64" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="P64" s="5" t="s">
         <v>32</v>
       </c>
@@ -9092,11 +9063,9 @@
       </c>
       <c r="S64" s="5"/>
       <c r="T64" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="U64" s="5" t="s">
-        <v>350</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="U64" s="5"/>
       <c r="V64" s="5" t="s">
         <v>64</v>
       </c>
@@ -9164,41 +9133,41 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="B65" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C65" s="12" t="s">
-        <v>175</v>
+      <c r="C65" s="4" t="s">
+        <v>341</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="E65" s="4" t="str">
         <f aca="false">CONCATENATE(D65,"_vs_",C65)</f>
-        <v>Rv3005c_KO_day32_vs_dejesus_H37Rv_day32</v>
+        <v>Rv0950c_KO_vs_CB_WT</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H65" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="J65" s="5"/>
       <c r="K65" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L65" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M65" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
@@ -9213,10 +9182,10 @@
       </c>
       <c r="S65" s="5"/>
       <c r="T65" s="5" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="U65" s="5" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="V65" s="5" t="s">
         <v>64</v>
@@ -9285,41 +9254,41 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B66" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="E66" s="4" t="str">
         <f aca="false">CONCATENATE(D66,"_vs_",C66)</f>
-        <v>Rv3594_KO_vs_Rubin_FLUTE_WT</v>
+        <v>Rv0954_KO_vs_RJ_WT</v>
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H66" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="J66" s="5"/>
       <c r="K66" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M66" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
@@ -9334,10 +9303,10 @@
       </c>
       <c r="S66" s="5"/>
       <c r="T66" s="5" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="U66" s="5" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="V66" s="5" t="s">
         <v>64</v>
@@ -9406,21 +9375,21 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B67" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="E67" s="4" t="str">
         <f aca="false">CONCATENATE(D67,"_vs_",C67)</f>
-        <v>Rv3684_KO_vs_CB_WT</v>
+        <v>Rv1096_KO_vs_CB_WT</v>
       </c>
       <c r="F67" s="4"/>
       <c r="G67" s="5" t="n">
@@ -9430,17 +9399,17 @@
         <v>1</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="J67" s="5"/>
       <c r="K67" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M67" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
@@ -9455,10 +9424,10 @@
       </c>
       <c r="S67" s="5"/>
       <c r="T67" s="5" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="U67" s="5" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="V67" s="5" t="s">
         <v>64</v>
@@ -9527,41 +9496,41 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="B68" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>356</v>
+      <c r="C68" s="12" t="s">
+        <v>175</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="E68" s="4" t="str">
         <f aca="false">CONCATENATE(D68,"_vs_",C68)</f>
-        <v>Rv3717_KO_vs_Rubin_FLUTE_WT</v>
+        <v>Rv3005c_KO_day32_vs_dejesus_H37Rv_day32</v>
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H68" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="J68" s="5"/>
       <c r="K68" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L68" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M68" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
@@ -9576,10 +9545,10 @@
       </c>
       <c r="S68" s="5"/>
       <c r="T68" s="5" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="U68" s="5" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="V68" s="5" t="s">
         <v>64</v>
@@ -9648,21 +9617,21 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B69" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="E69" s="4" t="str">
         <f aca="false">CONCATENATE(D69,"_vs_",C69)</f>
-        <v>Rv3811_KO_vs_Rubin_FLUTE_WT</v>
+        <v>Rv3594_KO_vs_Rubin_FLUTE_WT</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="5" t="n">
@@ -9672,17 +9641,17 @@
         <v>1</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L69" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M69" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
@@ -9697,10 +9666,10 @@
       </c>
       <c r="S69" s="5"/>
       <c r="T69" s="5" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="U69" s="5" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="V69" s="5" t="s">
         <v>64</v>
@@ -9769,41 +9738,41 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B70" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C70" s="12" t="s">
-        <v>373</v>
+      <c r="C70" s="4" t="s">
+        <v>341</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="E70" s="4" t="str">
         <f aca="false">CONCATENATE(D70,"_vs_",C70)</f>
-        <v>marP_KO_vs_marP_WT</v>
+        <v>Rv3684_KO_vs_CB_WT</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H70" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="J70" s="5"/>
       <c r="K70" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L70" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M70" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="N70" s="5"/>
       <c r="O70" s="5"/>
@@ -9817,9 +9786,11 @@
         <v>34</v>
       </c>
       <c r="S70" s="5"/>
-      <c r="T70" s="5"/>
+      <c r="T70" s="5" t="s">
+        <v>366</v>
+      </c>
       <c r="U70" s="5" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="V70" s="5" t="s">
         <v>64</v>
@@ -9888,41 +9859,41 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B71" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>72</v>
+        <v>359</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="E71" s="4" t="str">
         <f aca="false">CONCATENATE(D71,"_vs_",C71)</f>
-        <v>eccD1_KO_vs_mbio_H37Rv</v>
+        <v>Rv3717_KO_vs_Rubin_FLUTE_WT</v>
       </c>
       <c r="F71" s="4"/>
       <c r="G71" s="5" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="H71" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="J71" s="5"/>
       <c r="K71" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L71" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M71" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="N71" s="5"/>
       <c r="O71" s="5"/>
@@ -9936,9 +9907,11 @@
         <v>34</v>
       </c>
       <c r="S71" s="5"/>
-      <c r="T71" s="5"/>
+      <c r="T71" s="5" t="s">
+        <v>370</v>
+      </c>
       <c r="U71" s="5" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="V71" s="5" t="s">
         <v>64</v>
@@ -10007,41 +9980,41 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="B72" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>72</v>
+        <v>359</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="E72" s="4" t="str">
         <f aca="false">CONCATENATE(D72,"_vs_",C72)</f>
-        <v>espI_KO_vs_mbio_H37Rv</v>
+        <v>Rv3811_KO_vs_Rubin_FLUTE_WT</v>
       </c>
       <c r="F72" s="4"/>
       <c r="G72" s="5" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="H72" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="J72" s="5"/>
       <c r="K72" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L72" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M72" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="N72" s="5"/>
       <c r="O72" s="5"/>
@@ -10055,9 +10028,11 @@
         <v>34</v>
       </c>
       <c r="S72" s="5"/>
-      <c r="T72" s="5"/>
+      <c r="T72" s="5" t="s">
+        <v>374</v>
+      </c>
       <c r="U72" s="5" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="V72" s="5" t="s">
         <v>64</v>
@@ -10126,41 +10101,41 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="B73" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C73" s="4" t="s">
-        <v>72</v>
+      <c r="C73" s="12" t="s">
+        <v>376</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="E73" s="4" t="str">
         <f aca="false">CONCATENATE(D73,"_vs_",C73)</f>
-        <v>PE35_KO_vs_mbio_H37Rv</v>
+        <v>marP_KO_vs_marP_WT</v>
       </c>
       <c r="F73" s="4"/>
       <c r="G73" s="5" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="H73" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="J73" s="5"/>
       <c r="K73" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L73" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M73" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="N73" s="5"/>
       <c r="O73" s="5"/>
@@ -10176,7 +10151,7 @@
       <c r="S73" s="5"/>
       <c r="T73" s="5"/>
       <c r="U73" s="5" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="V73" s="5" t="s">
         <v>64</v>
@@ -10245,7 +10220,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="B74" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -10255,11 +10230,11 @@
         <v>72</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="E74" s="4" t="str">
         <f aca="false">CONCATENATE(D74,"_vs_",C74)</f>
-        <v>PPE68_KO_vs_mbio_H37Rv</v>
+        <v>eccD1_KO_vs_mbio_H37Rv</v>
       </c>
       <c r="F74" s="4"/>
       <c r="G74" s="5" t="n">
@@ -10269,17 +10244,17 @@
         <v>1</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="J74" s="5"/>
       <c r="K74" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M74" s="5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="N74" s="5"/>
       <c r="O74" s="5"/>
@@ -10295,7 +10270,7 @@
       <c r="S74" s="5"/>
       <c r="T74" s="5"/>
       <c r="U74" s="5" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="V74" s="5" t="s">
         <v>64</v>
@@ -10362,6 +10337,363 @@
       <c r="BZ74" s="5"/>
       <c r="CA74" s="5"/>
     </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B75" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="E75" s="4" t="str">
+        <f aca="false">CONCATENATE(D75,"_vs_",C75)</f>
+        <v>espI_KO_vs_mbio_H37Rv</v>
+      </c>
+      <c r="F75" s="4"/>
+      <c r="G75" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="H75" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I75" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="L75" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="M75" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="N75" s="5"/>
+      <c r="O75" s="5"/>
+      <c r="P75" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q75" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R75" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S75" s="5"/>
+      <c r="T75" s="5"/>
+      <c r="U75" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="V75" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W75" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="X75" s="5"/>
+      <c r="Y75" s="5"/>
+      <c r="Z75" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA75" s="3"/>
+      <c r="AB75" s="5"/>
+      <c r="AC75" s="5"/>
+      <c r="AD75" s="5"/>
+      <c r="AE75" s="5"/>
+      <c r="AF75" s="5"/>
+      <c r="AG75" s="5"/>
+      <c r="AH75" s="5"/>
+      <c r="AI75" s="5"/>
+      <c r="AJ75" s="5"/>
+      <c r="AK75" s="5"/>
+      <c r="AL75" s="5"/>
+      <c r="AM75" s="5"/>
+      <c r="AN75" s="5"/>
+      <c r="AO75" s="5"/>
+      <c r="AP75" s="5"/>
+      <c r="AQ75" s="5"/>
+      <c r="AR75" s="5"/>
+      <c r="AS75" s="5"/>
+      <c r="AT75" s="5"/>
+      <c r="AU75" s="5"/>
+      <c r="AV75" s="5"/>
+      <c r="AW75" s="5"/>
+      <c r="AX75" s="5"/>
+      <c r="AY75" s="5"/>
+      <c r="AZ75" s="5"/>
+      <c r="BA75" s="5"/>
+      <c r="BB75" s="5"/>
+      <c r="BC75" s="5"/>
+      <c r="BD75" s="5"/>
+      <c r="BE75" s="5"/>
+      <c r="BF75" s="5"/>
+      <c r="BG75" s="5"/>
+      <c r="BH75" s="5"/>
+      <c r="BI75" s="5"/>
+      <c r="BJ75" s="5"/>
+      <c r="BK75" s="5"/>
+      <c r="BL75" s="5"/>
+      <c r="BM75" s="5"/>
+      <c r="BN75" s="5"/>
+      <c r="BO75" s="5"/>
+      <c r="BP75" s="5"/>
+      <c r="BQ75" s="5"/>
+      <c r="BR75" s="5"/>
+      <c r="BS75" s="5"/>
+      <c r="BT75" s="5"/>
+      <c r="BU75" s="5"/>
+      <c r="BV75" s="5"/>
+      <c r="BW75" s="5"/>
+      <c r="BX75" s="5"/>
+      <c r="BY75" s="5"/>
+      <c r="BZ75" s="5"/>
+      <c r="CA75" s="5"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="B76" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="E76" s="4" t="str">
+        <f aca="false">CONCATENATE(D76,"_vs_",C76)</f>
+        <v>PE35_KO_vs_mbio_H37Rv</v>
+      </c>
+      <c r="F76" s="4"/>
+      <c r="G76" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="H76" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="L76" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="M76" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="N76" s="5"/>
+      <c r="O76" s="5"/>
+      <c r="P76" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q76" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R76" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S76" s="5"/>
+      <c r="T76" s="5"/>
+      <c r="U76" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="V76" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W76" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="X76" s="5"/>
+      <c r="Y76" s="5"/>
+      <c r="Z76" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA76" s="3"/>
+      <c r="AB76" s="5"/>
+      <c r="AC76" s="5"/>
+      <c r="AD76" s="5"/>
+      <c r="AE76" s="5"/>
+      <c r="AF76" s="5"/>
+      <c r="AG76" s="5"/>
+      <c r="AH76" s="5"/>
+      <c r="AI76" s="5"/>
+      <c r="AJ76" s="5"/>
+      <c r="AK76" s="5"/>
+      <c r="AL76" s="5"/>
+      <c r="AM76" s="5"/>
+      <c r="AN76" s="5"/>
+      <c r="AO76" s="5"/>
+      <c r="AP76" s="5"/>
+      <c r="AQ76" s="5"/>
+      <c r="AR76" s="5"/>
+      <c r="AS76" s="5"/>
+      <c r="AT76" s="5"/>
+      <c r="AU76" s="5"/>
+      <c r="AV76" s="5"/>
+      <c r="AW76" s="5"/>
+      <c r="AX76" s="5"/>
+      <c r="AY76" s="5"/>
+      <c r="AZ76" s="5"/>
+      <c r="BA76" s="5"/>
+      <c r="BB76" s="5"/>
+      <c r="BC76" s="5"/>
+      <c r="BD76" s="5"/>
+      <c r="BE76" s="5"/>
+      <c r="BF76" s="5"/>
+      <c r="BG76" s="5"/>
+      <c r="BH76" s="5"/>
+      <c r="BI76" s="5"/>
+      <c r="BJ76" s="5"/>
+      <c r="BK76" s="5"/>
+      <c r="BL76" s="5"/>
+      <c r="BM76" s="5"/>
+      <c r="BN76" s="5"/>
+      <c r="BO76" s="5"/>
+      <c r="BP76" s="5"/>
+      <c r="BQ76" s="5"/>
+      <c r="BR76" s="5"/>
+      <c r="BS76" s="5"/>
+      <c r="BT76" s="5"/>
+      <c r="BU76" s="5"/>
+      <c r="BV76" s="5"/>
+      <c r="BW76" s="5"/>
+      <c r="BX76" s="5"/>
+      <c r="BY76" s="5"/>
+      <c r="BZ76" s="5"/>
+      <c r="CA76" s="5"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B77" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="E77" s="4" t="str">
+        <f aca="false">CONCATENATE(D77,"_vs_",C77)</f>
+        <v>PPE68_KO_vs_mbio_H37Rv</v>
+      </c>
+      <c r="F77" s="4"/>
+      <c r="G77" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="H77" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="L77" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="M77" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="N77" s="5"/>
+      <c r="O77" s="5"/>
+      <c r="P77" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q77" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R77" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S77" s="5"/>
+      <c r="T77" s="5"/>
+      <c r="U77" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="V77" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W77" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="X77" s="5"/>
+      <c r="Y77" s="5"/>
+      <c r="Z77" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA77" s="3"/>
+      <c r="AB77" s="5"/>
+      <c r="AC77" s="5"/>
+      <c r="AD77" s="5"/>
+      <c r="AE77" s="5"/>
+      <c r="AF77" s="5"/>
+      <c r="AG77" s="5"/>
+      <c r="AH77" s="5"/>
+      <c r="AI77" s="5"/>
+      <c r="AJ77" s="5"/>
+      <c r="AK77" s="5"/>
+      <c r="AL77" s="5"/>
+      <c r="AM77" s="5"/>
+      <c r="AN77" s="5"/>
+      <c r="AO77" s="5"/>
+      <c r="AP77" s="5"/>
+      <c r="AQ77" s="5"/>
+      <c r="AR77" s="5"/>
+      <c r="AS77" s="5"/>
+      <c r="AT77" s="5"/>
+      <c r="AU77" s="5"/>
+      <c r="AV77" s="5"/>
+      <c r="AW77" s="5"/>
+      <c r="AX77" s="5"/>
+      <c r="AY77" s="5"/>
+      <c r="AZ77" s="5"/>
+      <c r="BA77" s="5"/>
+      <c r="BB77" s="5"/>
+      <c r="BC77" s="5"/>
+      <c r="BD77" s="5"/>
+      <c r="BE77" s="5"/>
+      <c r="BF77" s="5"/>
+      <c r="BG77" s="5"/>
+      <c r="BH77" s="5"/>
+      <c r="BI77" s="5"/>
+      <c r="BJ77" s="5"/>
+      <c r="BK77" s="5"/>
+      <c r="BL77" s="5"/>
+      <c r="BM77" s="5"/>
+      <c r="BN77" s="5"/>
+      <c r="BO77" s="5"/>
+      <c r="BP77" s="5"/>
+      <c r="BQ77" s="5"/>
+      <c r="BR77" s="5"/>
+      <c r="BS77" s="5"/>
+      <c r="BT77" s="5"/>
+      <c r="BU77" s="5"/>
+      <c r="BV77" s="5"/>
+      <c r="BW77" s="5"/>
+      <c r="BX77" s="5"/>
+      <c r="BY77" s="5"/>
+      <c r="BZ77" s="5"/>
+      <c r="CA77" s="5"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="https://onlinelibrary.wiley.com/doi/full/10.1046/j.1365-2958.2003.03425.x"/>
@@ -10395,30 +10727,33 @@
     <hyperlink ref="L33" r:id="rId29" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5499643/"/>
     <hyperlink ref="L34" r:id="rId30" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5499643/"/>
     <hyperlink ref="L35" r:id="rId31" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5499643/"/>
-    <hyperlink ref="L36" r:id="rId32" display="https://aac.asm.org/content/61/12/e01334-17"/>
-    <hyperlink ref="L37" r:id="rId33" display="https://aac.asm.org/content/61/12/e01334-17"/>
-    <hyperlink ref="L38" r:id="rId34" display="https://aac.asm.org/content/61/12/e01334-17"/>
+    <hyperlink ref="L36" r:id="rId32" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5499643/"/>
+    <hyperlink ref="L37" r:id="rId33" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5499643/"/>
+    <hyperlink ref="L38" r:id="rId34" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5499643/"/>
     <hyperlink ref="L39" r:id="rId35" display="https://aac.asm.org/content/61/12/e01334-17"/>
     <hyperlink ref="L40" r:id="rId36" display="https://aac.asm.org/content/61/12/e01334-17"/>
     <hyperlink ref="L41" r:id="rId37" display="https://aac.asm.org/content/61/12/e01334-17"/>
     <hyperlink ref="L42" r:id="rId38" display="https://aac.asm.org/content/61/12/e01334-17"/>
-    <hyperlink ref="L43" r:id="rId39" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5461879/"/>
-    <hyperlink ref="L44" r:id="rId40" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5461879/"/>
-    <hyperlink ref="L45" r:id="rId41" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5461879/"/>
-    <hyperlink ref="L46" r:id="rId42" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5854444/"/>
-    <hyperlink ref="L47" r:id="rId43" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5854444/"/>
-    <hyperlink ref="L48" r:id="rId44" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5854444/"/>
+    <hyperlink ref="L43" r:id="rId39" display="https://aac.asm.org/content/61/12/e01334-17"/>
+    <hyperlink ref="L44" r:id="rId40" display="https://aac.asm.org/content/61/12/e01334-17"/>
+    <hyperlink ref="L45" r:id="rId41" display="https://aac.asm.org/content/61/12/e01334-17"/>
+    <hyperlink ref="L46" r:id="rId42" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5461879/"/>
+    <hyperlink ref="L47" r:id="rId43" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5461879/"/>
+    <hyperlink ref="L48" r:id="rId44" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5461879/"/>
     <hyperlink ref="L49" r:id="rId45" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5854444/"/>
     <hyperlink ref="L50" r:id="rId46" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5854444/"/>
     <hyperlink ref="L51" r:id="rId47" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5854444/"/>
     <hyperlink ref="L52" r:id="rId48" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5854444/"/>
     <hyperlink ref="L53" r:id="rId49" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5854444/"/>
-    <hyperlink ref="L54" r:id="rId50" display="https://www.sciencedirect.com/science/article/pii/S2451945618303295"/>
-    <hyperlink ref="L55" r:id="rId51" display="https://www.sciencedirect.com/science/article/pii/S2451945618303295"/>
-    <hyperlink ref="L56" r:id="rId52" display="https://mbio.asm.org/content/10/4/e00663-19"/>
-    <hyperlink ref="L57" r:id="rId53" display="https://mbio.asm.org/content/10/4/e00663-19"/>
-    <hyperlink ref="L58" r:id="rId54" display="https://mbio.asm.org/content/10/4/e00663-19"/>
-    <hyperlink ref="L59" r:id="rId55" display="https://msystems.asm.org/content/4/4/e00070-19"/>
+    <hyperlink ref="L54" r:id="rId50" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5854444/"/>
+    <hyperlink ref="L55" r:id="rId51" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5854444/"/>
+    <hyperlink ref="L56" r:id="rId52" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5854444/"/>
+    <hyperlink ref="L57" r:id="rId53" display="https://www.sciencedirect.com/science/article/pii/S2451945618303295"/>
+    <hyperlink ref="L58" r:id="rId54" display="https://www.sciencedirect.com/science/article/pii/S2451945618303295"/>
+    <hyperlink ref="L59" r:id="rId55" display="https://mbio.asm.org/content/10/4/e00663-19"/>
+    <hyperlink ref="L60" r:id="rId56" display="https://mbio.asm.org/content/10/4/e00663-19"/>
+    <hyperlink ref="L61" r:id="rId57" display="https://mbio.asm.org/content/10/4/e00663-19"/>
+    <hyperlink ref="L62" r:id="rId58" display="https://msystems.asm.org/content/4/4/e00070-19"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
unhid col desc columns
</commit_message>
<xml_diff>
--- a/data/column_descriptors_standardized.xlsx
+++ b/data/column_descriptors_standardized.xlsx
@@ -1261,7 +1261,7 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val=""/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -1500,28 +1500,25 @@
   <dimension ref="A1:CA77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA9" activeCellId="0" sqref="AA9"/>
+      <selection pane="bottomRight" activeCell="AC15" activeCellId="0" sqref="AC15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="56.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.06"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="0" width="25.06"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="0" width="31.3"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="0" width="115.66"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="0" width="5.83"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="18" min="11" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="0" width="36.65"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="20" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="25.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="115.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="36.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>